<commit_message>
MS-WOPI: Update capture code according to RS.
</commit_message>
<xml_diff>
--- a/FileSyncandWOPI/Docs/MS-WOPI/MS-WOPI_RequirementSpecification.xlsx
+++ b/FileSyncandWOPI/Docs/MS-WOPI/MS-WOPI_RequirementSpecification.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6789" uniqueCount="2079">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6798" uniqueCount="2088">
   <si>
     <t>Req ID</t>
   </si>
@@ -5708,9 +5708,6 @@
 X-WOPI-Lock</t>
   </si>
   <si>
-    <t>[In PutFile] The response message for this operation can contain the following HTTP headers.</t>
-  </si>
-  <si>
     <t>[In PutFile] X-WOPI-Lock is a string.</t>
   </si>
   <si>
@@ -6855,6 +6852,39 @@
 X-WOPI-Lock
 X-WOPI-LockFailureReason
 X-WOPI-LockedByOtherInterface</t>
+  </si>
+  <si>
+    <t>Verified by derived requirements: MS-WOPI_R563, MS-WOPI_R566, MS-WOPI_R565.</t>
+  </si>
+  <si>
+    <t>[In PutFile] The response message for this operation can contain the following HTTP headers.
+X-WOPI-Lock
+X-WOPI-LockFailureReason
+X-WOPI-LockedByOtherInterface</t>
+  </si>
+  <si>
+    <t>Verified by requirements:MS-WOPI_R370002, MS-WOPI_R370003, MS-WOPI_R370004, MS-WOPI_R370005, MS-WOPI_R370006, MS-WOPI_R370007, MS-WOPI_R370008, MS-WOPI_R370011, MS-WOPI_R370012, MS-WOPI_R370013, MS-WOPI_R370014, MS-WOPI_R370015.</t>
+  </si>
+  <si>
+    <t>Verified by requirements:MS-WOPI_R401, MS-WOPI_R401001, MS-WOPI_R401002, MS-WOPI_R401003, MS-WOPI_R401006, MS-WOPI_R401007, MS-WOPI_R401008, MS-WOPI_R401009, MS-WOPI_R401010.</t>
+  </si>
+  <si>
+    <t>Verified by requirements: MS-WOPI_R422002, MS-WOPI_R422003, MS-WOPI_R422004, MS-WOPI_R422005, MS-WOPI_R422008, MS-WOPI_R422009, MS-WOPI_R422010, MS-WOPI_R422011, MS-WOPI_R422012.</t>
+  </si>
+  <si>
+    <t>Verified by requirements: MS-WOPI_R469008, MS-WOPI_R469009, MS-WOPI_R469010, MS-WOPI_R469011, MS-WOPI_R469014, MS-WOPI_R469015, MS-WOPI_R469016, MS-WOPI_R469017, MS-WOPI_R469018.</t>
+  </si>
+  <si>
+    <t>Verified by requirements: MS-WOPI_R460002, MS-WOPI_R460003, MS-WOPI_R460004, MS-WOPI_R460005, MS-WOPI_R460008, MS-WOPI_R460009, MS-WOPI_R460010, MS-WOPI_R460011, MS-WOPI_R460012.</t>
+  </si>
+  <si>
+    <t>Verified by requirements: MS-WOPI_R439002, MS-WOPI_R439003, MS-WOPI_R439004, MS-WOPI_R439005, MS-WOPI_R439008, MS-WOPI_R439009, MS-WOPI_R439010, MS-WOPI_R439011, MS-WOPI_R439012.</t>
+  </si>
+  <si>
+    <t>Verified by requirement: MS-WOPI_R685002, MS-WOPI_R685003, MS-WOPI_R685004, MS-WOPI_R685002, MS-WOPI_R685008, MS-WOPI_R685009, MS-WOPI_R685010, MS-WOPI_R685011, MS-WOPI_R685012.</t>
+  </si>
+  <si>
+    <t>Verified by requirements: MS-WOPI_R40002, MS-WOPI_R42001, MS-WOPI_R44, MS-WOPI_R45, MS-WOPI_R45001, MS-WOPI_R46001, MS-WOPI_R467001, MS-WOPI_R793, MS-WOPI_R795.</t>
   </si>
 </sst>
 </file>
@@ -7141,21 +7171,6 @@
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7180,355 +7195,26 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="87">
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
+  <dxfs count="57">
     <dxf>
       <font>
         <b val="0"/>
@@ -7867,6 +7553,200 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -7996,34 +7876,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I961" tableType="xml" totalsRowShown="0" headerRowDxfId="86" dataDxfId="85" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I961" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
   <autoFilter ref="A19:I961"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="84">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="83">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="82">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="81">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="80">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="79">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="78">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="77">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="76">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -8032,12 +7912,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="75" dataDxfId="73" headerRowBorderDxfId="74" tableBorderDxfId="72" totalsRowBorderDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="70"/>
-    <tableColumn id="2" name="Test" dataDxfId="69"/>
-    <tableColumn id="3" name="Description" dataDxfId="68"/>
+    <tableColumn id="1" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8333,7 +8213,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L964"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -8376,7 +8258,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>1427</v>
@@ -8387,127 +8269,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -8520,12 +8402,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -8538,12 +8420,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -8556,12 +8438,12 @@
       <c r="C14" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -8574,60 +8456,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -9586,7 +9468,7 @@
       </c>
       <c r="I56" s="31"/>
     </row>
-    <row r="57" spans="1:9" ht="105">
+    <row r="57" spans="1:9" ht="120">
       <c r="A57" s="29" t="s">
         <v>73</v>
       </c>
@@ -9607,9 +9489,11 @@
         <v>15</v>
       </c>
       <c r="H57" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="I57" s="31"/>
+        <v>17</v>
+      </c>
+      <c r="I57" s="20" t="s">
+        <v>2087</v>
+      </c>
     </row>
     <row r="58" spans="1:9" ht="30">
       <c r="A58" s="22" t="s">
@@ -9737,7 +9621,7 @@
       <c r="I62" s="31"/>
     </row>
     <row r="63" spans="1:9" ht="30">
-      <c r="A63" s="29" t="s">
+      <c r="A63" s="22" t="s">
         <v>76</v>
       </c>
       <c r="B63" s="30" t="s">
@@ -9769,7 +9653,7 @@
         <v>730</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
       <c r="D64" s="29"/>
       <c r="E64" s="29" t="s">
@@ -9788,13 +9672,13 @@
     </row>
     <row r="65" spans="1:9" ht="45">
       <c r="A65" s="22" t="s">
-        <v>2066</v>
+        <v>2065</v>
       </c>
       <c r="B65" s="30" t="s">
         <v>730</v>
       </c>
       <c r="C65" s="35" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
       <c r="D65" s="33"/>
       <c r="E65" s="29" t="s">
@@ -9844,7 +9728,7 @@
         <v>730</v>
       </c>
       <c r="C67" s="35" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
       <c r="D67" s="33"/>
       <c r="E67" s="29" t="s">
@@ -9869,7 +9753,7 @@
         <v>730</v>
       </c>
       <c r="C68" s="20" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
       <c r="D68" s="29"/>
       <c r="E68" s="29" t="s">
@@ -9888,13 +9772,13 @@
     </row>
     <row r="69" spans="1:9" ht="30">
       <c r="A69" s="22" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
       <c r="B69" s="30" t="s">
         <v>730</v>
       </c>
       <c r="C69" s="20" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
       <c r="D69" s="33"/>
       <c r="E69" s="22" t="s">
@@ -9912,7 +9796,7 @@
       <c r="I69" s="35"/>
     </row>
     <row r="70" spans="1:9" ht="45">
-      <c r="A70" s="29" t="s">
+      <c r="A70" s="22" t="s">
         <v>80</v>
       </c>
       <c r="B70" s="30" t="s">
@@ -9935,7 +9819,7 @@
         <v>17</v>
       </c>
       <c r="I70" s="20" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="30">
@@ -11448,7 +11332,7 @@
         <v>744</v>
       </c>
       <c r="C131" s="20" t="s">
-        <v>2073</v>
+        <v>2072</v>
       </c>
       <c r="D131" s="29"/>
       <c r="E131" s="29" t="s">
@@ -15777,7 +15661,7 @@
         <v>757</v>
       </c>
       <c r="C304" s="35" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="D304" s="33"/>
       <c r="E304" s="29" t="s">
@@ -15800,7 +15684,7 @@
       </c>
       <c r="B305" s="34"/>
       <c r="C305" s="35" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="D305" s="33"/>
       <c r="E305" s="29" t="s">
@@ -15819,7 +15703,7 @@
     </row>
     <row r="306" spans="1:9" ht="30">
       <c r="A306" s="22" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="B306" s="30" t="s">
         <v>757</v>
@@ -16837,7 +16721,7 @@
         <v>757</v>
       </c>
       <c r="C346" s="20" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="D346" s="29" t="s">
         <v>1393</v>
@@ -16855,7 +16739,7 @@
         <v>17</v>
       </c>
       <c r="I346" s="20" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="347" spans="1:9" ht="45">
@@ -16963,21 +16847,21 @@
         <v>17</v>
       </c>
       <c r="I350" s="20" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
     </row>
     <row r="351" spans="1:9">
       <c r="A351" s="33" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="B351" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C351" s="35" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="D351" s="33" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="E351" s="29" t="s">
         <v>19</v>
@@ -16995,16 +16879,16 @@
     </row>
     <row r="352" spans="1:9" ht="30">
       <c r="A352" s="33" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="B352" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C352" s="35" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="D352" s="33" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="E352" s="29" t="s">
         <v>19</v>
@@ -17044,21 +16928,21 @@
         <v>17</v>
       </c>
       <c r="I353" s="20" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
     </row>
     <row r="354" spans="1:9">
       <c r="A354" s="33" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
       <c r="B354" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C354" s="35" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="D354" s="33" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="E354" s="29" t="s">
         <v>19</v>
@@ -17076,16 +16960,16 @@
     </row>
     <row r="355" spans="1:9" ht="30">
       <c r="A355" s="33" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
       <c r="B355" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C355" s="35" t="s">
+        <v>1750</v>
+      </c>
+      <c r="D355" s="33" t="s">
         <v>1751</v>
-      </c>
-      <c r="D355" s="33" t="s">
-        <v>1752</v>
       </c>
       <c r="E355" s="29" t="s">
         <v>19</v>
@@ -17206,21 +17090,21 @@
         <v>17</v>
       </c>
       <c r="I359" s="20" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
     </row>
     <row r="360" spans="1:9">
       <c r="A360" s="22" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="B360" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C360" s="35" t="s">
-        <v>1758</v>
+        <v>1757</v>
       </c>
       <c r="D360" s="33" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="E360" s="29" t="s">
         <v>19</v>
@@ -17238,16 +17122,16 @@
     </row>
     <row r="361" spans="1:9" ht="30">
       <c r="A361" s="22" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
       <c r="B361" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C361" s="35" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="D361" s="33" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="E361" s="29" t="s">
         <v>19</v>
@@ -17368,21 +17252,21 @@
         <v>17</v>
       </c>
       <c r="I365" s="20" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
     </row>
     <row r="366" spans="1:9">
       <c r="A366" s="22" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="B366" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C366" s="35" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="D366" s="33" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="E366" s="29" t="s">
         <v>19</v>
@@ -17400,16 +17284,16 @@
     </row>
     <row r="367" spans="1:9" ht="30">
       <c r="A367" s="22" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
       <c r="B367" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C367" s="35" t="s">
+        <v>1766</v>
+      </c>
+      <c r="D367" s="33" t="s">
         <v>1767</v>
-      </c>
-      <c r="D367" s="33" t="s">
-        <v>1768</v>
       </c>
       <c r="E367" s="29" t="s">
         <v>19</v>
@@ -17614,7 +17498,7 @@
     </row>
     <row r="375" spans="1:9" ht="60">
       <c r="A375" s="22" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
       <c r="B375" s="30" t="s">
         <v>757</v>
@@ -17636,21 +17520,21 @@
         <v>17</v>
       </c>
       <c r="I375" s="20" t="s">
-        <v>1776</v>
+        <v>1775</v>
       </c>
     </row>
     <row r="376" spans="1:9">
       <c r="A376" s="22" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="B376" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C376" s="20" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="D376" s="22" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="E376" s="29" t="s">
         <v>19</v>
@@ -17668,16 +17552,16 @@
     </row>
     <row r="377" spans="1:9" ht="30">
       <c r="A377" s="22" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="B377" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C377" s="20" t="s">
+        <v>1773</v>
+      </c>
+      <c r="D377" s="22" t="s">
         <v>1774</v>
-      </c>
-      <c r="D377" s="22" t="s">
-        <v>1775</v>
       </c>
       <c r="E377" s="29" t="s">
         <v>19</v>
@@ -17770,7 +17654,7 @@
     </row>
     <row r="381" spans="1:9" ht="45">
       <c r="A381" s="22" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="B381" s="30" t="s">
         <v>757</v>
@@ -17792,21 +17676,21 @@
         <v>17</v>
       </c>
       <c r="I381" s="20" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="382" spans="1:9">
       <c r="A382" s="22" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="B382" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C382" s="20" t="s">
+        <v>1777</v>
+      </c>
+      <c r="D382" s="22" t="s">
         <v>1778</v>
-      </c>
-      <c r="D382" s="22" t="s">
-        <v>1779</v>
       </c>
       <c r="E382" s="29" t="s">
         <v>19</v>
@@ -17824,7 +17708,7 @@
     </row>
     <row r="383" spans="1:9" ht="30">
       <c r="A383" s="22" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="B383" s="30" t="s">
         <v>757</v>
@@ -17849,7 +17733,7 @@
     </row>
     <row r="384" spans="1:9" ht="30">
       <c r="A384" s="22" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
       <c r="B384" s="30" t="s">
         <v>757</v>
@@ -18105,7 +17989,7 @@
     </row>
     <row r="394" spans="1:9" ht="60">
       <c r="A394" s="22" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="B394" s="30" t="s">
         <v>757</v>
@@ -18127,21 +18011,21 @@
         <v>17</v>
       </c>
       <c r="I394" s="20" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
     </row>
     <row r="395" spans="1:9">
       <c r="A395" s="22" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="B395" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C395" s="20" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="D395" s="22" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
       <c r="E395" s="22" t="s">
         <v>19</v>
@@ -18159,16 +18043,16 @@
     </row>
     <row r="396" spans="1:9" ht="30">
       <c r="A396" s="22" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
       <c r="B396" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C396" s="20" t="s">
+        <v>1787</v>
+      </c>
+      <c r="D396" s="22" t="s">
         <v>1788</v>
-      </c>
-      <c r="D396" s="22" t="s">
-        <v>1789</v>
       </c>
       <c r="E396" s="22" t="s">
         <v>19</v>
@@ -18342,7 +18226,7 @@
     </row>
     <row r="403" spans="1:9" ht="30">
       <c r="A403" s="22" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="B403" s="30" t="s">
         <v>757</v>
@@ -18367,7 +18251,7 @@
     </row>
     <row r="404" spans="1:9" ht="30">
       <c r="A404" s="22" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="B404" s="30" t="s">
         <v>757</v>
@@ -19100,15 +18984,15 @@
       </c>
       <c r="I432" s="31"/>
     </row>
-    <row r="433" spans="1:9" ht="90">
+    <row r="433" spans="1:9" ht="195">
       <c r="A433" s="22" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
       <c r="B433" s="30" t="s">
         <v>759</v>
       </c>
       <c r="C433" s="20" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
       <c r="D433" s="33"/>
       <c r="E433" s="22" t="s">
@@ -19121,13 +19005,15 @@
         <v>15</v>
       </c>
       <c r="H433" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="I433" s="35"/>
+        <v>17</v>
+      </c>
+      <c r="I433" s="35" t="s">
+        <v>2080</v>
+      </c>
     </row>
     <row r="434" spans="1:9" ht="45">
       <c r="A434" s="22" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="B434" s="30" t="s">
         <v>759</v>
@@ -19152,13 +19038,13 @@
     </row>
     <row r="435" spans="1:9" ht="60">
       <c r="A435" s="22" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
       <c r="B435" s="30" t="s">
         <v>759</v>
       </c>
       <c r="C435" s="20" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="D435" s="33"/>
       <c r="E435" s="22" t="s">
@@ -19174,18 +19060,18 @@
         <v>17</v>
       </c>
       <c r="I435" s="35" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="436" spans="1:9" ht="45">
       <c r="A436" s="22" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
       <c r="B436" s="30" t="s">
         <v>759</v>
       </c>
       <c r="C436" s="20" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="D436" s="22"/>
       <c r="E436" s="22" t="s">
@@ -19201,12 +19087,12 @@
         <v>17</v>
       </c>
       <c r="I436" s="20" t="s">
-        <v>1808</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="437" spans="1:9">
       <c r="A437" s="22" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="B437" s="30" t="s">
         <v>759</v>
@@ -19231,7 +19117,7 @@
     </row>
     <row r="438" spans="1:9" ht="30">
       <c r="A438" s="22" t="s">
-        <v>1798</v>
+        <v>1797</v>
       </c>
       <c r="B438" s="30" t="s">
         <v>759</v>
@@ -19256,7 +19142,7 @@
     </row>
     <row r="439" spans="1:9" ht="30">
       <c r="A439" s="22" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="B439" s="30" t="s">
         <v>759</v>
@@ -19281,7 +19167,7 @@
     </row>
     <row r="440" spans="1:9">
       <c r="A440" s="22" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="B440" s="30" t="s">
         <v>759</v>
@@ -19306,7 +19192,7 @@
     </row>
     <row r="441" spans="1:9" ht="30">
       <c r="A441" s="22" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
       <c r="B441" s="30" t="s">
         <v>759</v>
@@ -19331,7 +19217,7 @@
     </row>
     <row r="442" spans="1:9" ht="30">
       <c r="A442" s="22" t="s">
-        <v>1810</v>
+        <v>1809</v>
       </c>
       <c r="B442" s="30" t="s">
         <v>759</v>
@@ -19356,7 +19242,7 @@
     </row>
     <row r="443" spans="1:9" ht="30">
       <c r="A443" s="22" t="s">
-        <v>1811</v>
+        <v>1810</v>
       </c>
       <c r="B443" s="30" t="s">
         <v>759</v>
@@ -19381,7 +19267,7 @@
     </row>
     <row r="444" spans="1:9" ht="45">
       <c r="A444" s="22" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="B444" s="30" t="s">
         <v>759</v>
@@ -19403,12 +19289,12 @@
         <v>17</v>
       </c>
       <c r="I444" s="35" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
     </row>
     <row r="445" spans="1:9">
       <c r="A445" s="22" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
       <c r="B445" s="30" t="s">
         <v>759</v>
@@ -19433,13 +19319,13 @@
     </row>
     <row r="446" spans="1:9" ht="30">
       <c r="A446" s="22" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="B446" s="30" t="s">
         <v>759</v>
       </c>
       <c r="C446" s="35" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
       <c r="D446" s="33"/>
       <c r="E446" s="33" t="s">
@@ -19458,7 +19344,7 @@
     </row>
     <row r="447" spans="1:9" ht="45">
       <c r="A447" s="22" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="B447" s="30" t="s">
         <v>759</v>
@@ -19480,7 +19366,7 @@
         <v>17</v>
       </c>
       <c r="I447" s="35" t="s">
-        <v>1827</v>
+        <v>1826</v>
       </c>
     </row>
     <row r="448" spans="1:9" ht="30">
@@ -19660,7 +19546,7 @@
     </row>
     <row r="455" spans="1:9" ht="30">
       <c r="A455" s="33" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
       <c r="B455" s="30" t="s">
         <v>759</v>
@@ -20258,7 +20144,7 @@
       </c>
       <c r="I478" s="31"/>
     </row>
-    <row r="479" spans="1:9" ht="75">
+    <row r="479" spans="1:9" ht="150">
       <c r="A479" s="29" t="s">
         <v>422</v>
       </c>
@@ -20266,7 +20152,7 @@
         <v>763</v>
       </c>
       <c r="C479" s="20" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="D479" s="29"/>
       <c r="E479" s="29" t="s">
@@ -20279,9 +20165,11 @@
         <v>15</v>
       </c>
       <c r="H479" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="I479" s="31"/>
+        <v>17</v>
+      </c>
+      <c r="I479" s="20" t="s">
+        <v>2081</v>
+      </c>
     </row>
     <row r="480" spans="1:9" ht="30">
       <c r="A480" s="22" t="s">
@@ -20310,7 +20198,7 @@
     </row>
     <row r="481" spans="1:9" ht="30">
       <c r="A481" s="33" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="B481" s="30" t="s">
         <v>763</v>
@@ -20335,7 +20223,7 @@
     </row>
     <row r="482" spans="1:9" ht="45">
       <c r="A482" s="33" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="B482" s="30" t="s">
         <v>763</v>
@@ -20357,12 +20245,12 @@
         <v>17</v>
       </c>
       <c r="I482" s="35" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="483" spans="1:9">
       <c r="A483" s="33" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="B483" s="30" t="s">
         <v>763</v>
@@ -20387,7 +20275,7 @@
     </row>
     <row r="484" spans="1:9">
       <c r="A484" s="33" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="B484" s="30" t="s">
         <v>763</v>
@@ -20412,7 +20300,7 @@
     </row>
     <row r="485" spans="1:9" ht="30">
       <c r="A485" s="33" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="B485" s="30" t="s">
         <v>763</v>
@@ -20437,7 +20325,7 @@
     </row>
     <row r="486" spans="1:9" ht="30">
       <c r="A486" s="33" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
       <c r="B486" s="30" t="s">
         <v>763</v>
@@ -20462,7 +20350,7 @@
     </row>
     <row r="487" spans="1:9" ht="45">
       <c r="A487" s="33" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
       <c r="B487" s="30" t="s">
         <v>763</v>
@@ -20484,12 +20372,12 @@
         <v>17</v>
       </c>
       <c r="I487" s="35" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="488" spans="1:9">
       <c r="A488" s="33" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
       <c r="B488" s="30" t="s">
         <v>763</v>
@@ -20514,13 +20402,13 @@
     </row>
     <row r="489" spans="1:9" ht="30">
       <c r="A489" s="33" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
       <c r="B489" s="30" t="s">
         <v>763</v>
       </c>
       <c r="C489" s="35" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
       <c r="D489" s="33"/>
       <c r="E489" s="29" t="s">
@@ -20539,7 +20427,7 @@
     </row>
     <row r="490" spans="1:9" ht="45">
       <c r="A490" s="33" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
       <c r="B490" s="30" t="s">
         <v>763</v>
@@ -20561,7 +20449,7 @@
         <v>17</v>
       </c>
       <c r="I490" s="35" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="491" spans="1:9">
@@ -20716,13 +20604,13 @@
     </row>
     <row r="497" spans="1:9" ht="30">
       <c r="A497" s="22" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="B497" s="30" t="s">
         <v>763</v>
       </c>
       <c r="C497" s="35" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
       <c r="D497" s="33"/>
       <c r="E497" s="33" t="s">
@@ -21089,15 +20977,15 @@
       </c>
       <c r="I511" s="31"/>
     </row>
-    <row r="512" spans="1:9" ht="75">
+    <row r="512" spans="1:9" ht="150">
       <c r="A512" s="33" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
       <c r="B512" s="30" t="s">
         <v>765</v>
       </c>
       <c r="C512" s="20" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
       <c r="D512" s="33"/>
       <c r="E512" s="33" t="s">
@@ -21110,13 +20998,15 @@
         <v>15</v>
       </c>
       <c r="H512" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="I512" s="35"/>
+        <v>17</v>
+      </c>
+      <c r="I512" s="35" t="s">
+        <v>2082</v>
+      </c>
     </row>
     <row r="513" spans="1:9" ht="30">
       <c r="A513" s="33" t="s">
-        <v>1846</v>
+        <v>1845</v>
       </c>
       <c r="B513" s="30" t="s">
         <v>765</v>
@@ -21141,7 +21031,7 @@
     </row>
     <row r="514" spans="1:9" ht="30">
       <c r="A514" s="33" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
       <c r="B514" s="30" t="s">
         <v>765</v>
@@ -21166,7 +21056,7 @@
     </row>
     <row r="515" spans="1:9" ht="45">
       <c r="A515" s="33" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="B515" s="30" t="s">
         <v>765</v>
@@ -21188,12 +21078,12 @@
         <v>17</v>
       </c>
       <c r="I515" s="35" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
     </row>
     <row r="516" spans="1:9">
       <c r="A516" s="33" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="B516" s="30" t="s">
         <v>765</v>
@@ -21218,7 +21108,7 @@
     </row>
     <row r="517" spans="1:9">
       <c r="A517" s="33" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
       <c r="B517" s="30" t="s">
         <v>765</v>
@@ -21243,7 +21133,7 @@
     </row>
     <row r="518" spans="1:9" ht="30">
       <c r="A518" s="33" t="s">
-        <v>1851</v>
+        <v>1850</v>
       </c>
       <c r="B518" s="30" t="s">
         <v>765</v>
@@ -21268,7 +21158,7 @@
     </row>
     <row r="519" spans="1:9" ht="30">
       <c r="A519" s="33" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="B519" s="30" t="s">
         <v>765</v>
@@ -21293,7 +21183,7 @@
     </row>
     <row r="520" spans="1:9" ht="45">
       <c r="A520" s="33" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="B520" s="30" t="s">
         <v>765</v>
@@ -21315,12 +21205,12 @@
         <v>17</v>
       </c>
       <c r="I520" s="35" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
     </row>
     <row r="521" spans="1:9">
       <c r="A521" s="33" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="B521" s="30" t="s">
         <v>765</v>
@@ -21345,13 +21235,13 @@
     </row>
     <row r="522" spans="1:9" ht="30">
       <c r="A522" s="33" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="B522" s="30" t="s">
         <v>765</v>
       </c>
       <c r="C522" s="35" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="D522" s="33"/>
       <c r="E522" s="33" t="s">
@@ -21370,7 +21260,7 @@
     </row>
     <row r="523" spans="1:9" ht="45">
       <c r="A523" s="33" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="B523" s="30" t="s">
         <v>765</v>
@@ -21392,7 +21282,7 @@
         <v>17</v>
       </c>
       <c r="I523" s="35" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="524" spans="1:9">
@@ -21870,15 +21760,15 @@
       </c>
       <c r="I542" s="31"/>
     </row>
-    <row r="543" spans="1:9" ht="75">
+    <row r="543" spans="1:9" ht="150">
       <c r="A543" s="22" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="B543" s="30" t="s">
         <v>767</v>
       </c>
       <c r="C543" s="20" t="s">
-        <v>2077</v>
+        <v>2076</v>
       </c>
       <c r="D543" s="33"/>
       <c r="E543" s="29" t="s">
@@ -21891,13 +21781,15 @@
         <v>15</v>
       </c>
       <c r="H543" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="I543" s="35"/>
+        <v>17</v>
+      </c>
+      <c r="I543" s="35" t="s">
+        <v>2085</v>
+      </c>
     </row>
     <row r="544" spans="1:9" ht="30">
       <c r="A544" s="22" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="B544" s="30" t="s">
         <v>767</v>
@@ -21922,7 +21814,7 @@
     </row>
     <row r="545" spans="1:9" ht="30">
       <c r="A545" s="22" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
       <c r="B545" s="30" t="s">
         <v>767</v>
@@ -21947,7 +21839,7 @@
     </row>
     <row r="546" spans="1:9" ht="45">
       <c r="A546" s="22" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="B546" s="30" t="s">
         <v>767</v>
@@ -21969,12 +21861,12 @@
         <v>17</v>
       </c>
       <c r="I546" s="35" t="s">
-        <v>1888</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="547" spans="1:9">
       <c r="A547" s="22" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="B547" s="30" t="s">
         <v>767</v>
@@ -21999,7 +21891,7 @@
     </row>
     <row r="548" spans="1:9">
       <c r="A548" s="22" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="B548" s="30" t="s">
         <v>767</v>
@@ -22024,7 +21916,7 @@
     </row>
     <row r="549" spans="1:9" ht="30">
       <c r="A549" s="22" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="B549" s="30" t="s">
         <v>767</v>
@@ -22049,7 +21941,7 @@
     </row>
     <row r="550" spans="1:9" ht="30">
       <c r="A550" s="22" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="B550" s="30" t="s">
         <v>767</v>
@@ -22074,7 +21966,7 @@
     </row>
     <row r="551" spans="1:9" ht="45">
       <c r="A551" s="22" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="B551" s="30" t="s">
         <v>767</v>
@@ -22096,12 +21988,12 @@
         <v>17</v>
       </c>
       <c r="I551" s="20" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="552" spans="1:9">
       <c r="A552" s="22" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
       <c r="B552" s="30" t="s">
         <v>767</v>
@@ -22126,13 +22018,13 @@
     </row>
     <row r="553" spans="1:9" ht="30">
       <c r="A553" s="22" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="B553" s="30" t="s">
         <v>767</v>
       </c>
       <c r="C553" s="35" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="D553" s="33"/>
       <c r="E553" s="29" t="s">
@@ -22151,7 +22043,7 @@
     </row>
     <row r="554" spans="1:9" ht="45">
       <c r="A554" s="22" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="B554" s="30" t="s">
         <v>767</v>
@@ -22173,7 +22065,7 @@
         <v>17</v>
       </c>
       <c r="I554" s="35" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
     </row>
     <row r="555" spans="1:9" ht="30">
@@ -22751,34 +22643,36 @@
       </c>
       <c r="I577" s="31"/>
     </row>
-    <row r="578" spans="1:9" ht="75">
+    <row r="578" spans="1:9" ht="150">
       <c r="A578" s="33" t="s">
-        <v>1895</v>
+        <v>1894</v>
       </c>
       <c r="B578" s="30" t="s">
         <v>769</v>
       </c>
       <c r="C578" s="20" t="s">
-        <v>2078</v>
+        <v>2077</v>
       </c>
       <c r="D578" s="33"/>
       <c r="E578" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F578" s="33" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="G578" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H578" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="I578" s="35"/>
+        <v>17</v>
+      </c>
+      <c r="I578" s="35" t="s">
+        <v>2084</v>
+      </c>
     </row>
     <row r="579" spans="1:9" ht="30">
       <c r="A579" s="33" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="B579" s="30" t="s">
         <v>769</v>
@@ -22791,7 +22685,7 @@
         <v>19</v>
       </c>
       <c r="F579" s="33" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="G579" s="33" t="s">
         <v>15</v>
@@ -22803,7 +22697,7 @@
     </row>
     <row r="580" spans="1:9" ht="30">
       <c r="A580" s="33" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="B580" s="30" t="s">
         <v>769</v>
@@ -22816,7 +22710,7 @@
         <v>19</v>
       </c>
       <c r="F580" s="33" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="G580" s="33" t="s">
         <v>15</v>
@@ -22828,7 +22722,7 @@
     </row>
     <row r="581" spans="1:9" ht="45">
       <c r="A581" s="33" t="s">
-        <v>1900</v>
+        <v>1899</v>
       </c>
       <c r="B581" s="30" t="s">
         <v>769</v>
@@ -22841,7 +22735,7 @@
         <v>19</v>
       </c>
       <c r="F581" s="33" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="G581" s="33" t="s">
         <v>15</v>
@@ -22850,12 +22744,12 @@
         <v>17</v>
       </c>
       <c r="I581" s="35" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="582" spans="1:9">
       <c r="A582" s="33" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
       <c r="B582" s="30" t="s">
         <v>769</v>
@@ -22868,7 +22762,7 @@
         <v>19</v>
       </c>
       <c r="F582" s="33" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="G582" s="33" t="s">
         <v>15</v>
@@ -22880,7 +22774,7 @@
     </row>
     <row r="583" spans="1:9" ht="30">
       <c r="A583" s="33" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
       <c r="B583" s="30" t="s">
         <v>769</v>
@@ -22893,7 +22787,7 @@
         <v>19</v>
       </c>
       <c r="F583" s="33" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="G583" s="33" t="s">
         <v>16</v>
@@ -22905,7 +22799,7 @@
     </row>
     <row r="584" spans="1:9" ht="30">
       <c r="A584" s="33" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
       <c r="B584" s="30" t="s">
         <v>769</v>
@@ -22918,7 +22812,7 @@
         <v>19</v>
       </c>
       <c r="F584" s="33" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="G584" s="33" t="s">
         <v>16</v>
@@ -22930,7 +22824,7 @@
     </row>
     <row r="585" spans="1:9">
       <c r="A585" s="33" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
       <c r="B585" s="30" t="s">
         <v>769</v>
@@ -22943,7 +22837,7 @@
         <v>19</v>
       </c>
       <c r="F585" s="33" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="G585" s="33" t="s">
         <v>15</v>
@@ -22955,20 +22849,20 @@
     </row>
     <row r="586" spans="1:9" ht="45">
       <c r="A586" s="33" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="B586" s="30" t="s">
         <v>769</v>
       </c>
       <c r="C586" s="35" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="D586" s="33"/>
       <c r="E586" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F586" s="33" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="G586" s="33" t="s">
         <v>15</v>
@@ -22977,12 +22871,12 @@
         <v>17</v>
       </c>
       <c r="I586" s="35" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
     </row>
     <row r="587" spans="1:9">
       <c r="A587" s="33" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="B587" s="30" t="s">
         <v>769</v>
@@ -22995,7 +22889,7 @@
         <v>19</v>
       </c>
       <c r="F587" s="33" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="G587" s="33" t="s">
         <v>15</v>
@@ -23007,20 +22901,20 @@
     </row>
     <row r="588" spans="1:9" ht="30">
       <c r="A588" s="33" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="B588" s="30" t="s">
         <v>769</v>
       </c>
       <c r="C588" s="35" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
       <c r="D588" s="33"/>
       <c r="E588" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F588" s="33" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="G588" s="33" t="s">
         <v>15</v>
@@ -23032,7 +22926,7 @@
     </row>
     <row r="589" spans="1:9" ht="45">
       <c r="A589" s="33" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="B589" s="30" t="s">
         <v>769</v>
@@ -23045,7 +22939,7 @@
         <v>19</v>
       </c>
       <c r="F589" s="33" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="G589" s="33" t="s">
         <v>15</v>
@@ -23054,7 +22948,7 @@
         <v>17</v>
       </c>
       <c r="I589" s="35" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="590" spans="1:9" ht="30">
@@ -23334,7 +23228,7 @@
     </row>
     <row r="601" spans="1:9">
       <c r="A601" s="33" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="B601" s="34" t="s">
         <v>771</v>
@@ -23359,7 +23253,7 @@
     </row>
     <row r="602" spans="1:9" ht="45">
       <c r="A602" s="33" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
       <c r="B602" s="34" t="s">
         <v>771</v>
@@ -23384,7 +23278,7 @@
     </row>
     <row r="603" spans="1:9" ht="30">
       <c r="A603" s="33" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
       <c r="B603" s="34" t="s">
         <v>771</v>
@@ -23409,7 +23303,7 @@
     </row>
     <row r="604" spans="1:9" ht="30">
       <c r="A604" s="33" t="s">
-        <v>1929</v>
+        <v>1928</v>
       </c>
       <c r="B604" s="34" t="s">
         <v>771</v>
@@ -23434,7 +23328,7 @@
     </row>
     <row r="605" spans="1:9">
       <c r="A605" s="33" t="s">
-        <v>1930</v>
+        <v>1929</v>
       </c>
       <c r="B605" s="34" t="s">
         <v>771</v>
@@ -23459,7 +23353,7 @@
     </row>
     <row r="606" spans="1:9">
       <c r="A606" s="33" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
       <c r="B606" s="34" t="s">
         <v>771</v>
@@ -23482,9 +23376,9 @@
       </c>
       <c r="I606" s="35"/>
     </row>
-    <row r="607" spans="1:9" ht="75">
+    <row r="607" spans="1:9" ht="150">
       <c r="A607" s="33" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="B607" s="34" t="s">
         <v>771</v>
@@ -23500,16 +23394,18 @@
         <v>6</v>
       </c>
       <c r="G607" s="33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H607" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="I607" s="35"/>
+        <v>17</v>
+      </c>
+      <c r="I607" s="35" t="s">
+        <v>2083</v>
+      </c>
     </row>
     <row r="608" spans="1:9" ht="30">
       <c r="A608" s="33" t="s">
-        <v>1933</v>
+        <v>1932</v>
       </c>
       <c r="B608" s="34" t="s">
         <v>771</v>
@@ -23534,13 +23430,13 @@
     </row>
     <row r="609" spans="1:9" ht="45">
       <c r="A609" s="33" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
       <c r="B609" s="34" t="s">
         <v>771</v>
       </c>
       <c r="C609" s="35" t="s">
-        <v>1925</v>
+        <v>1924</v>
       </c>
       <c r="D609" s="33"/>
       <c r="E609" s="29" t="s">
@@ -23559,13 +23455,13 @@
     </row>
     <row r="610" spans="1:9" ht="45">
       <c r="A610" s="33" t="s">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="B610" s="34" t="s">
         <v>771</v>
       </c>
       <c r="C610" s="35" t="s">
-        <v>1924</v>
+        <v>1923</v>
       </c>
       <c r="D610" s="33"/>
       <c r="E610" s="33" t="s">
@@ -23584,7 +23480,7 @@
     </row>
     <row r="611" spans="1:9">
       <c r="A611" s="33" t="s">
-        <v>1936</v>
+        <v>1935</v>
       </c>
       <c r="B611" s="34" t="s">
         <v>771</v>
@@ -23609,7 +23505,7 @@
     </row>
     <row r="612" spans="1:9">
       <c r="A612" s="33" t="s">
-        <v>1937</v>
+        <v>1936</v>
       </c>
       <c r="B612" s="34" t="s">
         <v>771</v>
@@ -23634,7 +23530,7 @@
     </row>
     <row r="613" spans="1:9" ht="30">
       <c r="A613" s="33" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
       <c r="B613" s="34" t="s">
         <v>771</v>
@@ -23659,7 +23555,7 @@
     </row>
     <row r="614" spans="1:9" ht="30">
       <c r="A614" s="33" t="s">
-        <v>1939</v>
+        <v>1938</v>
       </c>
       <c r="B614" s="34" t="s">
         <v>771</v>
@@ -23684,7 +23580,7 @@
     </row>
     <row r="615" spans="1:9" ht="45">
       <c r="A615" s="33" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="B615" s="34" t="s">
         <v>771</v>
@@ -23706,12 +23602,12 @@
         <v>17</v>
       </c>
       <c r="I615" s="35" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="616" spans="1:9">
       <c r="A616" s="33" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="B616" s="34" t="s">
         <v>771</v>
@@ -23736,13 +23632,13 @@
     </row>
     <row r="617" spans="1:9" ht="30">
       <c r="A617" s="33" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="B617" s="34" t="s">
         <v>771</v>
       </c>
       <c r="C617" s="35" t="s">
-        <v>1923</v>
+        <v>1922</v>
       </c>
       <c r="D617" s="33"/>
       <c r="E617" s="29" t="s">
@@ -23761,7 +23657,7 @@
     </row>
     <row r="618" spans="1:9" ht="45">
       <c r="A618" s="33" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="B618" s="34" t="s">
         <v>771</v>
@@ -23774,7 +23670,7 @@
         <v>19</v>
       </c>
       <c r="F618" s="33" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="G618" s="33" t="s">
         <v>15</v>
@@ -23783,12 +23679,12 @@
         <v>17</v>
       </c>
       <c r="I618" s="35" t="s">
-        <v>1963</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="619" spans="1:9" ht="30">
       <c r="A619" s="33" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="B619" s="34" t="s">
         <v>771</v>
@@ -23813,7 +23709,7 @@
     </row>
     <row r="620" spans="1:9">
       <c r="A620" s="33" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="B620" s="34" t="s">
         <v>771</v>
@@ -23838,7 +23734,7 @@
     </row>
     <row r="621" spans="1:9">
       <c r="A621" s="33" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="B621" s="34" t="s">
         <v>771</v>
@@ -23863,7 +23759,7 @@
     </row>
     <row r="622" spans="1:9">
       <c r="A622" s="33" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
       <c r="B622" s="34" t="s">
         <v>771</v>
@@ -23888,7 +23784,7 @@
     </row>
     <row r="623" spans="1:9">
       <c r="A623" s="33" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="B623" s="34" t="s">
         <v>771</v>
@@ -23913,7 +23809,7 @@
     </row>
     <row r="624" spans="1:9">
       <c r="A624" s="33" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="B624" s="34" t="s">
         <v>771</v>
@@ -23938,7 +23834,7 @@
     </row>
     <row r="625" spans="1:9" ht="30">
       <c r="A625" s="33" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="B625" s="34" t="s">
         <v>771</v>
@@ -23963,7 +23859,7 @@
     </row>
     <row r="626" spans="1:9">
       <c r="A626" s="33" t="s">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="B626" s="34" t="s">
         <v>771</v>
@@ -23988,7 +23884,7 @@
     </row>
     <row r="627" spans="1:9">
       <c r="A627" s="33" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="B627" s="34" t="s">
         <v>771</v>
@@ -24013,7 +23909,7 @@
     </row>
     <row r="628" spans="1:9">
       <c r="A628" s="33" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="B628" s="34" t="s">
         <v>772</v>
@@ -26211,7 +26107,7 @@
       </c>
       <c r="I715" s="31"/>
     </row>
-    <row r="716" spans="1:9" ht="45">
+    <row r="716" spans="1:9" ht="60">
       <c r="A716" s="29" t="s">
         <v>580</v>
       </c>
@@ -26228,16 +26124,18 @@
       <c r="F716" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G716" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="H716" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="I716" s="31"/>
+      <c r="G716" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H716" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I716" s="20" t="s">
+        <v>2078</v>
+      </c>
     </row>
     <row r="717" spans="1:9" ht="30">
-      <c r="A717" s="29" t="s">
+      <c r="A717" s="22" t="s">
         <v>581</v>
       </c>
       <c r="B717" s="24" t="s">
@@ -26963,7 +26861,7 @@
     </row>
     <row r="746" spans="1:9">
       <c r="A746" s="33" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="B746" s="24" t="s">
         <v>1648</v>
@@ -26988,7 +26886,7 @@
     </row>
     <row r="747" spans="1:9" ht="45">
       <c r="A747" s="33" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
       <c r="B747" s="24" t="s">
         <v>1648</v>
@@ -27013,7 +26911,7 @@
     </row>
     <row r="748" spans="1:9" ht="75">
       <c r="A748" s="33" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
       <c r="B748" s="24" t="s">
         <v>1648</v>
@@ -27038,7 +26936,7 @@
     </row>
     <row r="749" spans="1:9" ht="30">
       <c r="A749" s="33" t="s">
-        <v>1968</v>
+        <v>1967</v>
       </c>
       <c r="B749" s="24" t="s">
         <v>1648</v>
@@ -27063,7 +26961,7 @@
     </row>
     <row r="750" spans="1:9">
       <c r="A750" s="33" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
       <c r="B750" s="24" t="s">
         <v>1648</v>
@@ -27088,7 +26986,7 @@
     </row>
     <row r="751" spans="1:9">
       <c r="A751" s="33" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="B751" s="24" t="s">
         <v>1648</v>
@@ -27113,7 +27011,7 @@
     </row>
     <row r="752" spans="1:9" ht="30">
       <c r="A752" s="33" t="s">
-        <v>1971</v>
+        <v>1970</v>
       </c>
       <c r="B752" s="24" t="s">
         <v>1648</v>
@@ -27138,7 +27036,7 @@
     </row>
     <row r="753" spans="1:9">
       <c r="A753" s="33" t="s">
-        <v>1972</v>
+        <v>1971</v>
       </c>
       <c r="B753" s="24" t="s">
         <v>1648</v>
@@ -27163,7 +27061,7 @@
     </row>
     <row r="754" spans="1:9" ht="30">
       <c r="A754" s="33" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
       <c r="B754" s="24" t="s">
         <v>1648</v>
@@ -27188,7 +27086,7 @@
     </row>
     <row r="755" spans="1:9">
       <c r="A755" s="33" t="s">
-        <v>1974</v>
+        <v>1973</v>
       </c>
       <c r="B755" s="24" t="s">
         <v>1648</v>
@@ -27213,7 +27111,7 @@
     </row>
     <row r="756" spans="1:9">
       <c r="A756" s="33" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
       <c r="B756" s="24" t="s">
         <v>1648</v>
@@ -27238,7 +27136,7 @@
     </row>
     <row r="757" spans="1:9">
       <c r="A757" s="33" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="B757" s="24" t="s">
         <v>1648</v>
@@ -27263,7 +27161,7 @@
     </row>
     <row r="758" spans="1:9" ht="90">
       <c r="A758" s="33" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="B758" s="24" t="s">
         <v>1648</v>
@@ -27288,7 +27186,7 @@
     </row>
     <row r="759" spans="1:9" ht="30">
       <c r="A759" s="33" t="s">
-        <v>1978</v>
+        <v>1977</v>
       </c>
       <c r="B759" s="24" t="s">
         <v>1648</v>
@@ -27313,7 +27211,7 @@
     </row>
     <row r="760" spans="1:9" ht="30">
       <c r="A760" s="33" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
       <c r="B760" s="24" t="s">
         <v>1648</v>
@@ -27338,7 +27236,7 @@
     </row>
     <row r="761" spans="1:9" ht="30">
       <c r="A761" s="33" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
       <c r="B761" s="24" t="s">
         <v>1648</v>
@@ -27363,7 +27261,7 @@
     </row>
     <row r="762" spans="1:9" ht="45">
       <c r="A762" s="33" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="B762" s="24" t="s">
         <v>1648</v>
@@ -27385,12 +27283,12 @@
         <v>17</v>
       </c>
       <c r="I762" s="35" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="763" spans="1:9">
       <c r="A763" s="33" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="B763" s="24" t="s">
         <v>1648</v>
@@ -27415,7 +27313,7 @@
     </row>
     <row r="764" spans="1:9" ht="30">
       <c r="A764" s="33" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="B764" s="24" t="s">
         <v>1648</v>
@@ -27440,7 +27338,7 @@
     </row>
     <row r="765" spans="1:9" ht="30">
       <c r="A765" s="33" t="s">
-        <v>1984</v>
+        <v>1983</v>
       </c>
       <c r="B765" s="24" t="s">
         <v>1648</v>
@@ -27465,7 +27363,7 @@
     </row>
     <row r="766" spans="1:9" ht="45">
       <c r="A766" s="33" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="B766" s="24" t="s">
         <v>1648</v>
@@ -27487,12 +27385,12 @@
         <v>20</v>
       </c>
       <c r="I766" s="35" t="s">
-        <v>2029</v>
+        <v>2028</v>
       </c>
     </row>
     <row r="767" spans="1:9">
       <c r="A767" s="33" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
       <c r="B767" s="24" t="s">
         <v>1648</v>
@@ -27517,7 +27415,7 @@
     </row>
     <row r="768" spans="1:9">
       <c r="A768" s="33" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
       <c r="B768" s="24" t="s">
         <v>1648</v>
@@ -27542,7 +27440,7 @@
     </row>
     <row r="769" spans="1:9" ht="30">
       <c r="A769" s="33" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="B769" s="24" t="s">
         <v>1648</v>
@@ -27567,7 +27465,7 @@
     </row>
     <row r="770" spans="1:9" ht="30">
       <c r="A770" s="33" t="s">
-        <v>1989</v>
+        <v>1988</v>
       </c>
       <c r="B770" s="24" t="s">
         <v>1648</v>
@@ -27592,7 +27490,7 @@
     </row>
     <row r="771" spans="1:9" ht="45">
       <c r="A771" s="33" t="s">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="B771" s="24" t="s">
         <v>1648</v>
@@ -27614,12 +27512,12 @@
         <v>17</v>
       </c>
       <c r="I771" s="35" t="s">
-        <v>2032</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="772" spans="1:9">
       <c r="A772" s="33" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="B772" s="24" t="s">
         <v>1648</v>
@@ -27644,13 +27542,13 @@
     </row>
     <row r="773" spans="1:9" ht="30">
       <c r="A773" s="33" t="s">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="B773" s="24" t="s">
         <v>1648</v>
       </c>
       <c r="C773" s="35" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="D773" s="33"/>
       <c r="E773" s="33" t="s">
@@ -27669,7 +27567,7 @@
     </row>
     <row r="774" spans="1:9" ht="45">
       <c r="A774" s="33" t="s">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="B774" s="24" t="s">
         <v>1648</v>
@@ -27691,12 +27589,12 @@
         <v>17</v>
       </c>
       <c r="I774" s="35" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
     </row>
     <row r="775" spans="1:9" ht="30">
       <c r="A775" s="33" t="s">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="B775" s="24" t="s">
         <v>1648</v>
@@ -27721,7 +27619,7 @@
     </row>
     <row r="776" spans="1:9">
       <c r="A776" s="33" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="B776" s="24" t="s">
         <v>1648</v>
@@ -27746,7 +27644,7 @@
     </row>
     <row r="777" spans="1:9">
       <c r="A777" s="33" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="B777" s="24" t="s">
         <v>1648</v>
@@ -27771,7 +27669,7 @@
     </row>
     <row r="778" spans="1:9">
       <c r="A778" s="33" t="s">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="B778" s="24" t="s">
         <v>1648</v>
@@ -27796,7 +27694,7 @@
     </row>
     <row r="779" spans="1:9">
       <c r="A779" s="33" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="B779" s="24" t="s">
         <v>1648</v>
@@ -27821,7 +27719,7 @@
     </row>
     <row r="780" spans="1:9">
       <c r="A780" s="33" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="B780" s="24" t="s">
         <v>1648</v>
@@ -27846,7 +27744,7 @@
     </row>
     <row r="781" spans="1:9" ht="30">
       <c r="A781" s="33" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="B781" s="24" t="s">
         <v>1648</v>
@@ -27871,7 +27769,7 @@
     </row>
     <row r="782" spans="1:9">
       <c r="A782" s="33" t="s">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="B782" s="24" t="s">
         <v>1648</v>
@@ -27896,7 +27794,7 @@
     </row>
     <row r="783" spans="1:9">
       <c r="A783" s="33" t="s">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="B783" s="24" t="s">
         <v>1648</v>
@@ -27921,7 +27819,7 @@
     </row>
     <row r="784" spans="1:9" ht="105">
       <c r="A784" s="33" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="B784" s="24" t="s">
         <v>1648</v>
@@ -27946,7 +27844,7 @@
     </row>
     <row r="785" spans="1:9">
       <c r="A785" s="33" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="B785" s="24" t="s">
         <v>1648</v>
@@ -27971,7 +27869,7 @@
     </row>
     <row r="786" spans="1:9">
       <c r="A786" s="33" t="s">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="B786" s="34" t="s">
         <v>1687</v>
@@ -27996,7 +27894,7 @@
     </row>
     <row r="787" spans="1:9" ht="45">
       <c r="A787" s="33" t="s">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="B787" s="34" t="s">
         <v>1687</v>
@@ -28021,7 +27919,7 @@
     </row>
     <row r="788" spans="1:9" ht="45">
       <c r="A788" s="33" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="B788" s="34" t="s">
         <v>1687</v>
@@ -28046,7 +27944,7 @@
     </row>
     <row r="789" spans="1:9" ht="30">
       <c r="A789" s="33" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="B789" s="34" t="s">
         <v>1687</v>
@@ -28071,7 +27969,7 @@
     </row>
     <row r="790" spans="1:9">
       <c r="A790" s="33" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="B790" s="34" t="s">
         <v>1687</v>
@@ -28096,7 +27994,7 @@
     </row>
     <row r="791" spans="1:9">
       <c r="A791" s="33" t="s">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="B791" s="34" t="s">
         <v>1687</v>
@@ -28121,7 +28019,7 @@
     </row>
     <row r="792" spans="1:9" ht="30">
       <c r="A792" s="33" t="s">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="B792" s="34" t="s">
         <v>1687</v>
@@ -28146,7 +28044,7 @@
     </row>
     <row r="793" spans="1:9">
       <c r="A793" s="33" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="B793" s="34" t="s">
         <v>1687</v>
@@ -28171,7 +28069,7 @@
     </row>
     <row r="794" spans="1:9">
       <c r="A794" s="33" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="B794" s="34" t="s">
         <v>1687</v>
@@ -28196,7 +28094,7 @@
     </row>
     <row r="795" spans="1:9">
       <c r="A795" s="33" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="B795" s="34" t="s">
         <v>1687</v>
@@ -28221,7 +28119,7 @@
     </row>
     <row r="796" spans="1:9">
       <c r="A796" s="33" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="B796" s="34" t="s">
         <v>1687</v>
@@ -28246,7 +28144,7 @@
     </row>
     <row r="797" spans="1:9">
       <c r="A797" s="33" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B797" s="34" t="s">
         <v>1687</v>
@@ -28271,7 +28169,7 @@
     </row>
     <row r="798" spans="1:9">
       <c r="A798" s="33" t="s">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B798" s="34" t="s">
         <v>1687</v>
@@ -28296,7 +28194,7 @@
     </row>
     <row r="799" spans="1:9">
       <c r="A799" s="33" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="B799" s="34" t="s">
         <v>1687</v>
@@ -28321,7 +28219,7 @@
     </row>
     <row r="800" spans="1:9">
       <c r="A800" s="33" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B800" s="34" t="s">
         <v>1687</v>
@@ -28346,7 +28244,7 @@
     </row>
     <row r="801" spans="1:9" ht="30">
       <c r="A801" s="33" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="B801" s="34" t="s">
         <v>1687</v>
@@ -28371,7 +28269,7 @@
     </row>
     <row r="802" spans="1:9" ht="30">
       <c r="A802" s="33" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="B802" s="34" t="s">
         <v>1687</v>
@@ -30373,15 +30271,15 @@
       </c>
       <c r="I881" s="31"/>
     </row>
-    <row r="882" spans="1:9" ht="30">
+    <row r="882" spans="1:9" ht="150">
       <c r="A882" s="33" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
       <c r="B882" s="30" t="s">
         <v>793</v>
       </c>
       <c r="C882" s="35" t="s">
-        <v>1709</v>
+        <v>2079</v>
       </c>
       <c r="D882" s="33"/>
       <c r="E882" s="33" t="s">
@@ -30391,16 +30289,18 @@
         <v>6</v>
       </c>
       <c r="G882" s="33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H882" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="I882" s="35"/>
+        <v>17</v>
+      </c>
+      <c r="I882" s="35" t="s">
+        <v>2086</v>
+      </c>
     </row>
     <row r="883" spans="1:9" ht="30">
       <c r="A883" s="33" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
       <c r="B883" s="30" t="s">
         <v>793</v>
@@ -30425,13 +30325,13 @@
     </row>
     <row r="884" spans="1:9" ht="30">
       <c r="A884" s="33" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
       <c r="B884" s="30" t="s">
         <v>793</v>
       </c>
       <c r="C884" s="35" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="D884" s="33"/>
       <c r="E884" s="33" t="s">
@@ -30450,13 +30350,13 @@
     </row>
     <row r="885" spans="1:9" ht="45">
       <c r="A885" s="33" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
       <c r="B885" s="30" t="s">
         <v>793</v>
       </c>
       <c r="C885" s="35" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="D885" s="33"/>
       <c r="E885" s="33" t="s">
@@ -30472,18 +30372,18 @@
         <v>17</v>
       </c>
       <c r="I885" s="35" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="886" spans="1:9">
       <c r="A886" s="33" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="B886" s="30" t="s">
         <v>793</v>
       </c>
       <c r="C886" s="35" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="D886" s="33"/>
       <c r="E886" s="33" t="s">
@@ -30502,13 +30402,13 @@
     </row>
     <row r="887" spans="1:9">
       <c r="A887" s="33" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
       <c r="B887" s="30" t="s">
         <v>793</v>
       </c>
       <c r="C887" s="35" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="D887" s="33"/>
       <c r="E887" s="33" t="s">
@@ -30527,13 +30427,13 @@
     </row>
     <row r="888" spans="1:9" ht="30">
       <c r="A888" s="33" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
       <c r="B888" s="30" t="s">
         <v>793</v>
       </c>
       <c r="C888" s="35" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="D888" s="33"/>
       <c r="E888" s="33" t="s">
@@ -30552,13 +30452,13 @@
     </row>
     <row r="889" spans="1:9" ht="30">
       <c r="A889" s="33" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="B889" s="30" t="s">
         <v>793</v>
       </c>
       <c r="C889" s="35" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="D889" s="33"/>
       <c r="E889" s="33" t="s">
@@ -30577,13 +30477,13 @@
     </row>
     <row r="890" spans="1:9" ht="45">
       <c r="A890" s="33" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="B890" s="30" t="s">
         <v>793</v>
       </c>
       <c r="C890" s="35" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="D890" s="33"/>
       <c r="E890" s="33" t="s">
@@ -30599,18 +30499,18 @@
         <v>17</v>
       </c>
       <c r="I890" s="35" t="s">
-        <v>2061</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="891" spans="1:9">
       <c r="A891" s="33" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
       <c r="B891" s="30" t="s">
         <v>793</v>
       </c>
       <c r="C891" s="35" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="D891" s="33"/>
       <c r="E891" s="33" t="s">
@@ -30629,13 +30529,13 @@
     </row>
     <row r="892" spans="1:9" ht="30">
       <c r="A892" s="33" t="s">
-        <v>2049</v>
+        <v>2048</v>
       </c>
       <c r="B892" s="30" t="s">
         <v>793</v>
       </c>
       <c r="C892" s="35" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
       <c r="D892" s="33"/>
       <c r="E892" s="33" t="s">
@@ -30654,13 +30554,13 @@
     </row>
     <row r="893" spans="1:9" ht="45">
       <c r="A893" s="33" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
       <c r="B893" s="30" t="s">
         <v>793</v>
       </c>
       <c r="C893" s="35" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="D893" s="33"/>
       <c r="E893" s="33" t="s">
@@ -30676,7 +30576,7 @@
         <v>17</v>
       </c>
       <c r="I893" s="35" t="s">
-        <v>2062</v>
+        <v>2061</v>
       </c>
     </row>
     <row r="894" spans="1:9">
@@ -30831,13 +30731,13 @@
     </row>
     <row r="900" spans="1:9" ht="30">
       <c r="A900" s="33" t="s">
-        <v>2064</v>
+        <v>2063</v>
       </c>
       <c r="B900" s="30" t="s">
         <v>793</v>
       </c>
       <c r="C900" s="35" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="D900" s="33"/>
       <c r="E900" s="29" t="s">
@@ -31062,7 +30962,7 @@
         <v>796</v>
       </c>
       <c r="C909" s="20" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="D909" s="29"/>
       <c r="E909" s="29" t="s">
@@ -31087,7 +30987,7 @@
         <v>796</v>
       </c>
       <c r="C910" s="20" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="D910" s="29"/>
       <c r="E910" s="29" t="s">
@@ -31112,7 +31012,7 @@
         <v>796</v>
       </c>
       <c r="C911" s="20" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="D911" s="29"/>
       <c r="E911" s="29" t="s">
@@ -31137,7 +31037,7 @@
         <v>796</v>
       </c>
       <c r="C912" s="20" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="D912" s="29"/>
       <c r="E912" s="29" t="s">
@@ -31162,7 +31062,7 @@
         <v>796</v>
       </c>
       <c r="C913" s="20" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="D913" s="29"/>
       <c r="E913" s="29" t="s">
@@ -31212,7 +31112,7 @@
         <v>797</v>
       </c>
       <c r="C915" s="20" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="D915" s="29"/>
       <c r="E915" s="29" t="s">
@@ -31362,7 +31262,7 @@
         <v>798</v>
       </c>
       <c r="C921" s="20" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="D921" s="29"/>
       <c r="E921" s="29" t="s">
@@ -31674,7 +31574,7 @@
         <v>800</v>
       </c>
       <c r="C933" s="20" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="D933" s="22" t="s">
         <v>1407</v>
@@ -31697,16 +31597,16 @@
     </row>
     <row r="934" spans="1:9" ht="45">
       <c r="A934" s="33" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="B934" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C934" s="35" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="D934" s="33" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
       <c r="E934" s="29" t="s">
         <v>22</v>
@@ -31726,16 +31626,16 @@
     </row>
     <row r="935" spans="1:9" ht="45">
       <c r="A935" s="33" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="B935" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C935" s="35" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="D935" s="33" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="E935" s="29" t="s">
         <v>22</v>
@@ -31755,16 +31655,16 @@
     </row>
     <row r="936" spans="1:9" ht="60">
       <c r="A936" s="22" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="B936" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C936" s="20" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="D936" s="33" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="E936" s="29" t="s">
         <v>22</v>
@@ -31784,16 +31684,16 @@
     </row>
     <row r="937" spans="1:9" ht="60">
       <c r="A937" s="33" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="B937" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C937" s="35" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="D937" s="33" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="E937" s="29" t="s">
         <v>22</v>
@@ -31813,16 +31713,16 @@
     </row>
     <row r="938" spans="1:9" ht="45">
       <c r="A938" s="33" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
       <c r="B938" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C938" s="35" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="D938" s="33" t="s">
-        <v>1816</v>
+        <v>1815</v>
       </c>
       <c r="E938" s="29" t="s">
         <v>22</v>
@@ -31842,16 +31742,16 @@
     </row>
     <row r="939" spans="1:9" ht="45">
       <c r="A939" s="33" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="B939" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C939" s="35" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="D939" s="33" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
       <c r="E939" s="29" t="s">
         <v>22</v>
@@ -31871,16 +31771,16 @@
     </row>
     <row r="940" spans="1:9" ht="45">
       <c r="A940" s="33" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
       <c r="B940" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C940" s="35" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
       <c r="D940" s="33" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
       <c r="E940" s="29" t="s">
         <v>22</v>
@@ -31900,16 +31800,16 @@
     </row>
     <row r="941" spans="1:9" ht="45">
       <c r="A941" s="33" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
       <c r="B941" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C941" s="35" t="s">
-        <v>1861</v>
+        <v>1860</v>
       </c>
       <c r="D941" s="33" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="E941" s="29" t="s">
         <v>22</v>
@@ -31929,16 +31829,16 @@
     </row>
     <row r="942" spans="1:9" ht="45">
       <c r="A942" s="33" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
       <c r="B942" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C942" s="35" t="s">
-        <v>1862</v>
+        <v>1861</v>
       </c>
       <c r="D942" s="33" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="E942" s="29" t="s">
         <v>22</v>
@@ -31958,16 +31858,16 @@
     </row>
     <row r="943" spans="1:9" ht="45">
       <c r="A943" s="33" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
       <c r="B943" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C943" s="35" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="D943" s="33" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="E943" s="29" t="s">
         <v>22</v>
@@ -31987,16 +31887,16 @@
     </row>
     <row r="944" spans="1:9" ht="45">
       <c r="A944" s="33" t="s">
-        <v>1865</v>
+        <v>1864</v>
       </c>
       <c r="B944" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C944" s="20" t="s">
+        <v>1865</v>
+      </c>
+      <c r="D944" s="33" t="s">
         <v>1866</v>
-      </c>
-      <c r="D944" s="33" t="s">
-        <v>1867</v>
       </c>
       <c r="E944" s="29" t="s">
         <v>22</v>
@@ -32016,16 +31916,16 @@
     </row>
     <row r="945" spans="1:9" ht="45">
       <c r="A945" s="33" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="B945" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C945" s="35" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
       <c r="D945" s="33" t="s">
-        <v>1922</v>
+        <v>1921</v>
       </c>
       <c r="E945" s="29" t="s">
         <v>22</v>
@@ -32045,16 +31945,16 @@
     </row>
     <row r="946" spans="1:9" ht="45">
       <c r="A946" s="22" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="B946" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C946" s="35" t="s">
-        <v>1890</v>
+        <v>1889</v>
       </c>
       <c r="D946" s="22" t="s">
-        <v>1921</v>
+        <v>1920</v>
       </c>
       <c r="E946" s="29" t="s">
         <v>22</v>
@@ -32074,16 +31974,16 @@
     </row>
     <row r="947" spans="1:9" ht="45">
       <c r="A947" s="22" t="s">
-        <v>1892</v>
+        <v>1891</v>
       </c>
       <c r="B947" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C947" s="20" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="D947" s="22" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="E947" s="29" t="s">
         <v>22</v>
@@ -32103,16 +32003,16 @@
     </row>
     <row r="948" spans="1:9" ht="45">
       <c r="A948" s="33" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
       <c r="B948" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C948" s="35" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="D948" s="33" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="E948" s="29" t="s">
         <v>22</v>
@@ -32132,16 +32032,16 @@
     </row>
     <row r="949" spans="1:9" ht="45">
       <c r="A949" s="33" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="B949" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C949" s="35" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="D949" s="33" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="E949" s="29" t="s">
         <v>22</v>
@@ -32161,16 +32061,16 @@
     </row>
     <row r="950" spans="1:9" ht="45">
       <c r="A950" s="33" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
       <c r="B950" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C950" s="35" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="D950" s="33" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
       <c r="E950" s="29" t="s">
         <v>22</v>
@@ -32190,16 +32090,16 @@
     </row>
     <row r="951" spans="1:9" ht="45">
       <c r="A951" s="33" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="B951" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C951" s="35" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="D951" s="33" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="E951" s="29" t="s">
         <v>22</v>
@@ -32219,16 +32119,16 @@
     </row>
     <row r="952" spans="1:9" ht="45">
       <c r="A952" s="33" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="B952" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C952" s="35" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
       <c r="D952" s="33" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="E952" s="29" t="s">
         <v>22</v>
@@ -32248,16 +32148,16 @@
     </row>
     <row r="953" spans="1:9" ht="45">
       <c r="A953" s="33" t="s">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B953" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C953" s="35" t="s">
+        <v>2022</v>
+      </c>
+      <c r="D953" s="33" t="s">
         <v>2023</v>
-      </c>
-      <c r="D953" s="33" t="s">
-        <v>2024</v>
       </c>
       <c r="E953" s="29" t="s">
         <v>22</v>
@@ -32277,16 +32177,16 @@
     </row>
     <row r="954" spans="1:9" ht="45">
       <c r="A954" s="33" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="B954" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C954" s="35" t="s">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="D954" s="33" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="E954" s="29" t="s">
         <v>22</v>
@@ -32306,16 +32206,16 @@
     </row>
     <row r="955" spans="1:9" ht="45">
       <c r="A955" s="33" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="B955" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C955" s="35" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
       <c r="D955" s="33" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="E955" s="29" t="s">
         <v>22</v>
@@ -32335,16 +32235,16 @@
     </row>
     <row r="956" spans="1:9" ht="45">
       <c r="A956" s="33" t="s">
-        <v>2033</v>
+        <v>2032</v>
       </c>
       <c r="B956" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C956" s="35" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="D956" s="33" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
       <c r="E956" s="29" t="s">
         <v>22</v>
@@ -32364,16 +32264,16 @@
     </row>
     <row r="957" spans="1:9" ht="45">
       <c r="A957" s="33" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="B957" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C957" s="35" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
       <c r="D957" s="33" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="E957" s="29" t="s">
         <v>22</v>
@@ -32393,16 +32293,16 @@
     </row>
     <row r="958" spans="1:9" ht="45">
       <c r="A958" s="33" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
       <c r="B958" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C958" s="35" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
       <c r="D958" s="33" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
       <c r="E958" s="29" t="s">
         <v>22</v>
@@ -32422,16 +32322,16 @@
     </row>
     <row r="959" spans="1:9" ht="45">
       <c r="A959" s="33" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
       <c r="B959" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C959" s="35" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
       <c r="D959" s="33" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
       <c r="E959" s="29" t="s">
         <v>22</v>
@@ -32451,16 +32351,16 @@
     </row>
     <row r="960" spans="1:9" ht="45">
       <c r="A960" s="33" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="B960" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C960" s="35" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="D960" s="33" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="E960" s="29" t="s">
         <v>22</v>
@@ -32480,16 +32380,16 @@
     </row>
     <row r="961" spans="1:9" ht="45">
       <c r="A961" s="33" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="B961" s="34">
         <v>8</v>
       </c>
       <c r="C961" s="35" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="D961" s="33" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="E961" s="29" t="s">
         <v>22</v>
@@ -32528,6 +32428,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -32535,150 +32440,145 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="I20:I46 D342:I342 A342:B342 A962:I962 A961 A960:D960 E960:E961 A20:H341 F960:I960 F961:H961 A36:I341 A343:I959">
-    <cfRule type="expression" dxfId="37" priority="83">
+    <cfRule type="expression" dxfId="56" priority="83">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="84">
+    <cfRule type="expression" dxfId="55" priority="84">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="91">
+    <cfRule type="expression" dxfId="54" priority="91">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:I46 D342:I342 A342:B342 A962:I962 A961 A960:D960 E960:E961 A20:H341 F960:I960 F961:H961 A36:I341 A343:I959">
-    <cfRule type="expression" dxfId="34" priority="37">
+    <cfRule type="expression" dxfId="53" priority="37">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="38">
+    <cfRule type="expression" dxfId="52" priority="38">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="39">
+    <cfRule type="expression" dxfId="51" priority="39">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F962">
-    <cfRule type="expression" dxfId="31" priority="43">
+    <cfRule type="expression" dxfId="50" priority="43">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="44">
+    <cfRule type="expression" dxfId="49" priority="44">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C342">
-    <cfRule type="expression" dxfId="29" priority="28">
+    <cfRule type="expression" dxfId="48" priority="28">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="29">
+    <cfRule type="expression" dxfId="47" priority="29">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="30">
+    <cfRule type="expression" dxfId="46" priority="30">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C342">
-    <cfRule type="expression" dxfId="26" priority="25">
+    <cfRule type="expression" dxfId="45" priority="25">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="26">
+    <cfRule type="expression" dxfId="44" priority="26">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="27">
+    <cfRule type="expression" dxfId="43" priority="27">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B961">
-    <cfRule type="expression" dxfId="23" priority="22">
+    <cfRule type="expression" dxfId="42" priority="22">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="23">
+    <cfRule type="expression" dxfId="41" priority="23">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="24">
+    <cfRule type="expression" dxfId="40" priority="24">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B961">
-    <cfRule type="expression" dxfId="20" priority="19">
+    <cfRule type="expression" dxfId="39" priority="19">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="20">
+    <cfRule type="expression" dxfId="38" priority="20">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="21">
+    <cfRule type="expression" dxfId="37" priority="21">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C961">
-    <cfRule type="expression" dxfId="17" priority="16">
+    <cfRule type="expression" dxfId="36" priority="16">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="35" priority="17">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="18">
+    <cfRule type="expression" dxfId="34" priority="18">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C961">
-    <cfRule type="expression" dxfId="14" priority="13">
+    <cfRule type="expression" dxfId="33" priority="13">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="14">
+    <cfRule type="expression" dxfId="32" priority="14">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="15">
+    <cfRule type="expression" dxfId="31" priority="15">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D961">
-    <cfRule type="expression" dxfId="11" priority="10">
+    <cfRule type="expression" dxfId="30" priority="10">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="29" priority="11">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="12">
+    <cfRule type="expression" dxfId="28" priority="12">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D961">
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="27" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="26" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="9">
+    <cfRule type="expression" dxfId="25" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I961">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="24" priority="4">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="23" priority="5">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="22" priority="6">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I961">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="21" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="20" priority="2">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="19" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
[MS-WOPI] Add 6 new cases for status code 409.
</commit_message>
<xml_diff>
--- a/FileSyncandWOPI/Docs/MS-WOPI/MS-WOPI_RequirementSpecification.xlsx
+++ b/FileSyncandWOPI/Docs/MS-WOPI/MS-WOPI_RequirementSpecification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6798" uniqueCount="2088">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6795" uniqueCount="2088">
   <si>
     <t>Req ID</t>
   </si>
@@ -6866,31 +6866,31 @@
     <t>Verified by requirements:MS-WOPI_R370002, MS-WOPI_R370003, MS-WOPI_R370004, MS-WOPI_R370005, MS-WOPI_R370006, MS-WOPI_R370007, MS-WOPI_R370008, MS-WOPI_R370011, MS-WOPI_R370012, MS-WOPI_R370013, MS-WOPI_R370014, MS-WOPI_R370015.</t>
   </si>
   <si>
-    <t>Verified by requirements:MS-WOPI_R401, MS-WOPI_R401001, MS-WOPI_R401002, MS-WOPI_R401003, MS-WOPI_R401006, MS-WOPI_R401007, MS-WOPI_R401008, MS-WOPI_R401009, MS-WOPI_R401010.</t>
-  </si>
-  <si>
-    <t>Verified by requirements: MS-WOPI_R422002, MS-WOPI_R422003, MS-WOPI_R422004, MS-WOPI_R422005, MS-WOPI_R422008, MS-WOPI_R422009, MS-WOPI_R422010, MS-WOPI_R422011, MS-WOPI_R422012.</t>
-  </si>
-  <si>
     <t>Verified by requirements: MS-WOPI_R469008, MS-WOPI_R469009, MS-WOPI_R469010, MS-WOPI_R469011, MS-WOPI_R469014, MS-WOPI_R469015, MS-WOPI_R469016, MS-WOPI_R469017, MS-WOPI_R469018.</t>
   </si>
   <si>
-    <t>Verified by requirements: MS-WOPI_R460002, MS-WOPI_R460003, MS-WOPI_R460004, MS-WOPI_R460005, MS-WOPI_R460008, MS-WOPI_R460009, MS-WOPI_R460010, MS-WOPI_R460011, MS-WOPI_R460012.</t>
-  </si>
-  <si>
-    <t>Verified by requirements: MS-WOPI_R439002, MS-WOPI_R439003, MS-WOPI_R439004, MS-WOPI_R439005, MS-WOPI_R439008, MS-WOPI_R439009, MS-WOPI_R439010, MS-WOPI_R439011, MS-WOPI_R439012.</t>
-  </si>
-  <si>
-    <t>Verified by requirement: MS-WOPI_R685002, MS-WOPI_R685003, MS-WOPI_R685004, MS-WOPI_R685002, MS-WOPI_R685008, MS-WOPI_R685009, MS-WOPI_R685010, MS-WOPI_R685011, MS-WOPI_R685012.</t>
-  </si>
-  <si>
     <t>Verified by requirements: MS-WOPI_R40002, MS-WOPI_R42001, MS-WOPI_R44, MS-WOPI_R45, MS-WOPI_R45001, MS-WOPI_R46001, MS-WOPI_R467001, MS-WOPI_R793, MS-WOPI_R795.</t>
+  </si>
+  <si>
+    <t>Verified by requirements:MS-WOPI_R401,MS-WOPI_R401002, MS-WOPI_R401003, MS-WOPI_R401006, MS-WOPI_R401007, MS-WOPI_R401008,MS-WOPI_R401010.</t>
+  </si>
+  <si>
+    <t>Verified by requirements: MS-WOPI_R422002, MS-WOPI_R422004, MS-WOPI_R422005, MS-WOPI_R422008, MS-WOPI_R422009, MS-WOPI_R422010, MS-WOPI_R422011, MS-WOPI_R422012.</t>
+  </si>
+  <si>
+    <t>Verified by requirements: MS-WOPI_R439002, MS-WOPI_R439004, MS-WOPI_R439005, MS-WOPI_R439008, MS-WOPI_R439009, MS-WOPI_R439010, MS-WOPI_R439011, MS-WOPI_R439012.</t>
+  </si>
+  <si>
+    <t>Verified by requirements: MS-WOPI_R460002, MS-WOPI_R460003, MS-WOPI_R460004, MS-WOPI_R460005, MS-WOPI_R460008, MS-WOPI_R460009, MS-WOPI_R460010, MS-WOPI_R460012.</t>
+  </si>
+  <si>
+    <t>Verified by requirement: MS-WOPI_R685002, MS-WOPI_R685003, MS-WOPI_R685004, MS-WOPI_R685002, MS-WOPI_R685008, MS-WOPI_R685009, MS-WOPI_R685010, MS-WOPI_R685012.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.0.0"/>
@@ -7171,6 +7171,21 @@
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7194,21 +7209,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7966,7 +7966,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7999,9 +7999,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -8034,6 +8051,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -8213,9 +8247,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L964"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -8269,127 +8301,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -8402,12 +8434,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -8420,12 +8452,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -8438,12 +8470,12 @@
       <c r="C14" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -8456,60 +8488,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -9492,7 +9524,7 @@
         <v>17</v>
       </c>
       <c r="I57" s="20" t="s">
-        <v>2087</v>
+        <v>2082</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="30">
@@ -20144,7 +20176,7 @@
       </c>
       <c r="I478" s="31"/>
     </row>
-    <row r="479" spans="1:9" ht="150">
+    <row r="479" spans="1:9" ht="120">
       <c r="A479" s="29" t="s">
         <v>422</v>
       </c>
@@ -20168,7 +20200,7 @@
         <v>17</v>
       </c>
       <c r="I479" s="20" t="s">
-        <v>2081</v>
+        <v>2083</v>
       </c>
     </row>
     <row r="480" spans="1:9" ht="30">
@@ -20217,7 +20249,7 @@
         <v>15</v>
       </c>
       <c r="H481" s="33" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I481" s="35"/>
     </row>
@@ -20421,7 +20453,7 @@
         <v>15</v>
       </c>
       <c r="H489" s="33" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I489" s="35"/>
     </row>
@@ -20977,7 +21009,7 @@
       </c>
       <c r="I511" s="31"/>
     </row>
-    <row r="512" spans="1:9" ht="150">
+    <row r="512" spans="1:9" ht="135">
       <c r="A512" s="33" t="s">
         <v>1844</v>
       </c>
@@ -21000,8 +21032,8 @@
       <c r="H512" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="I512" s="35" t="s">
-        <v>2082</v>
+      <c r="I512" s="20" t="s">
+        <v>2084</v>
       </c>
     </row>
     <row r="513" spans="1:9" ht="30">
@@ -21050,7 +21082,7 @@
         <v>15</v>
       </c>
       <c r="H514" s="33" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I514" s="35"/>
     </row>
@@ -21760,7 +21792,7 @@
       </c>
       <c r="I542" s="31"/>
     </row>
-    <row r="543" spans="1:9" ht="150">
+    <row r="543" spans="1:9" ht="135">
       <c r="A543" s="22" t="s">
         <v>1873</v>
       </c>
@@ -21783,7 +21815,7 @@
       <c r="H543" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="I543" s="35" t="s">
+      <c r="I543" s="20" t="s">
         <v>2085</v>
       </c>
     </row>
@@ -21833,7 +21865,7 @@
         <v>15</v>
       </c>
       <c r="H545" s="33" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I545" s="35"/>
     </row>
@@ -22239,7 +22271,7 @@
         <v>15</v>
       </c>
       <c r="H561" s="33" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I561" s="35"/>
     </row>
@@ -22643,7 +22675,7 @@
       </c>
       <c r="I577" s="31"/>
     </row>
-    <row r="578" spans="1:9" ht="150">
+    <row r="578" spans="1:9" ht="135">
       <c r="A578" s="33" t="s">
         <v>1894</v>
       </c>
@@ -22666,8 +22698,8 @@
       <c r="H578" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="I578" s="35" t="s">
-        <v>2084</v>
+      <c r="I578" s="20" t="s">
+        <v>2086</v>
       </c>
     </row>
     <row r="579" spans="1:9" ht="30">
@@ -22920,7 +22952,7 @@
         <v>15</v>
       </c>
       <c r="H588" s="33" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I588" s="35"/>
     </row>
@@ -23400,7 +23432,7 @@
         <v>17</v>
       </c>
       <c r="I607" s="35" t="s">
-        <v>2083</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="608" spans="1:9" ht="30">
@@ -30271,7 +30303,7 @@
       </c>
       <c r="I881" s="31"/>
     </row>
-    <row r="882" spans="1:9" ht="150">
+    <row r="882" spans="1:9" ht="135">
       <c r="A882" s="33" t="s">
         <v>2038</v>
       </c>
@@ -30294,8 +30326,8 @@
       <c r="H882" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="I882" s="35" t="s">
-        <v>2086</v>
+      <c r="I882" s="20" t="s">
+        <v>2087</v>
       </c>
     </row>
     <row r="883" spans="1:9" ht="30">
@@ -30548,7 +30580,7 @@
         <v>15</v>
       </c>
       <c r="H892" s="33" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I892" s="35"/>
     </row>
@@ -31705,11 +31737,9 @@
         <v>15</v>
       </c>
       <c r="H937" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="I937" s="31" t="s">
-        <v>1424</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I937" s="31"/>
     </row>
     <row r="938" spans="1:9" ht="45">
       <c r="A938" s="33" t="s">
@@ -31908,11 +31938,9 @@
         <v>15</v>
       </c>
       <c r="H944" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="I944" s="31" t="s">
-        <v>1424</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I944" s="31"/>
     </row>
     <row r="945" spans="1:9" ht="45">
       <c r="A945" s="33" t="s">
@@ -31995,11 +32023,9 @@
         <v>15</v>
       </c>
       <c r="H947" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="I947" s="31" t="s">
-        <v>1424</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I947" s="31"/>
     </row>
     <row r="948" spans="1:9" ht="45">
       <c r="A948" s="33" t="s">
@@ -32428,11 +32454,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -32440,6 +32461,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="I20:I46 D342:I342 A342:B342 A962:I962 A961 A960:D960 E960:E961 A20:H341 F960:I960 F961:H961 A36:I341 A343:I959">

</xml_diff>

<commit_message>
MS-WOPI:move capture code to test suite.
</commit_message>
<xml_diff>
--- a/FileSyncandWOPI/Docs/MS-WOPI/MS-WOPI_RequirementSpecification.xlsx
+++ b/FileSyncandWOPI/Docs/MS-WOPI/MS-WOPI_RequirementSpecification.xlsx
@@ -6945,6 +6945,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -7171,6 +7172,21 @@
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7194,21 +7210,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8213,9 +8214,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L964"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B785" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C802" sqref="C802"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -8269,127 +8268,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -8402,12 +8401,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -8420,12 +8419,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -8438,12 +8437,12 @@
       <c r="C14" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -8456,60 +8455,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -19111,7 +19110,7 @@
         <v>15</v>
       </c>
       <c r="H437" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I437" s="35"/>
     </row>
@@ -19147,7 +19146,7 @@
       <c r="B439" s="30" t="s">
         <v>759</v>
       </c>
-      <c r="C439" s="35" t="s">
+      <c r="C439" s="20" t="s">
         <v>1558</v>
       </c>
       <c r="D439" s="33"/>
@@ -19160,7 +19159,7 @@
       <c r="G439" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="H439" s="33" t="s">
+      <c r="H439" s="22" t="s">
         <v>18</v>
       </c>
       <c r="I439" s="35"/>
@@ -19172,7 +19171,7 @@
       <c r="B440" s="30" t="s">
         <v>759</v>
       </c>
-      <c r="C440" s="35" t="s">
+      <c r="C440" s="20" t="s">
         <v>1559</v>
       </c>
       <c r="D440" s="33"/>
@@ -19299,7 +19298,7 @@
       <c r="B445" s="30" t="s">
         <v>759</v>
       </c>
-      <c r="C445" s="35" t="s">
+      <c r="C445" s="20" t="s">
         <v>1564</v>
       </c>
       <c r="D445" s="33"/>
@@ -20216,8 +20215,8 @@
       <c r="G481" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="H481" s="33" t="s">
-        <v>18</v>
+      <c r="H481" s="22" t="s">
+        <v>20</v>
       </c>
       <c r="I481" s="35"/>
     </row>
@@ -20269,7 +20268,7 @@
         <v>15</v>
       </c>
       <c r="H483" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I483" s="31"/>
     </row>
@@ -20371,7 +20370,7 @@
       <c r="H487" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="I487" s="35" t="s">
+      <c r="I487" s="20" t="s">
         <v>1836</v>
       </c>
     </row>
@@ -20382,7 +20381,7 @@
       <c r="B488" s="30" t="s">
         <v>763</v>
       </c>
-      <c r="C488" s="35" t="s">
+      <c r="C488" s="20" t="s">
         <v>1573</v>
       </c>
       <c r="D488" s="33"/>
@@ -21030,13 +21029,13 @@
       <c r="I513" s="35"/>
     </row>
     <row r="514" spans="1:9" ht="30">
-      <c r="A514" s="33" t="s">
+      <c r="A514" s="22" t="s">
         <v>1845</v>
       </c>
       <c r="B514" s="30" t="s">
         <v>765</v>
       </c>
-      <c r="C514" s="35" t="s">
+      <c r="C514" s="20" t="s">
         <v>1577</v>
       </c>
       <c r="D514" s="33"/>
@@ -21049,8 +21048,8 @@
       <c r="G514" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="H514" s="33" t="s">
-        <v>18</v>
+      <c r="H514" s="22" t="s">
+        <v>20</v>
       </c>
       <c r="I514" s="35"/>
     </row>
@@ -21082,13 +21081,13 @@
       </c>
     </row>
     <row r="516" spans="1:9">
-      <c r="A516" s="33" t="s">
+      <c r="A516" s="22" t="s">
         <v>1847</v>
       </c>
       <c r="B516" s="30" t="s">
         <v>765</v>
       </c>
-      <c r="C516" s="35" t="s">
+      <c r="C516" s="20" t="s">
         <v>1579</v>
       </c>
       <c r="D516" s="33"/>
@@ -21209,7 +21208,7 @@
       </c>
     </row>
     <row r="521" spans="1:9">
-      <c r="A521" s="33" t="s">
+      <c r="A521" s="22" t="s">
         <v>1852</v>
       </c>
       <c r="B521" s="30" t="s">
@@ -22767,8 +22766,8 @@
       <c r="G582" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="H582" s="33" t="s">
-        <v>21</v>
+      <c r="H582" s="22" t="s">
+        <v>20</v>
       </c>
       <c r="I582" s="35"/>
     </row>
@@ -22875,7 +22874,7 @@
       </c>
     </row>
     <row r="587" spans="1:9">
-      <c r="A587" s="33" t="s">
+      <c r="A587" s="22" t="s">
         <v>1904</v>
       </c>
       <c r="B587" s="30" t="s">
@@ -30395,8 +30394,8 @@
       <c r="G886" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="H886" s="33" t="s">
-        <v>21</v>
+      <c r="H886" s="22" t="s">
+        <v>20</v>
       </c>
       <c r="I886" s="35"/>
     </row>
@@ -31764,13 +31763,13 @@
       </c>
     </row>
     <row r="940" spans="1:9" ht="45">
-      <c r="A940" s="33" t="s">
+      <c r="A940" s="22" t="s">
         <v>1834</v>
       </c>
       <c r="B940" s="34" t="s">
         <v>800</v>
       </c>
-      <c r="C940" s="35" t="s">
+      <c r="C940" s="20" t="s">
         <v>1835</v>
       </c>
       <c r="D940" s="33" t="s">
@@ -31851,7 +31850,7 @@
       </c>
     </row>
     <row r="943" spans="1:9" ht="45">
-      <c r="A943" s="33" t="s">
+      <c r="A943" s="22" t="s">
         <v>1858</v>
       </c>
       <c r="B943" s="34" t="s">
@@ -31942,7 +31941,7 @@
       <c r="B946" s="34" t="s">
         <v>800</v>
       </c>
-      <c r="C946" s="35" t="s">
+      <c r="C946" s="20" t="s">
         <v>1888</v>
       </c>
       <c r="D946" s="22" t="s">
@@ -32021,7 +32020,7 @@
       </c>
     </row>
     <row r="949" spans="1:9" ht="45">
-      <c r="A949" s="33" t="s">
+      <c r="A949" s="22" t="s">
         <v>1910</v>
       </c>
       <c r="B949" s="34" t="s">
@@ -32406,11 +32405,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -32418,6 +32412,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="I20:I46 D342:I342 A342:B342 A962:I962 A961 A960:D960 E960:E961 A20:H341 F960:I960 F961:H961 A36:I341 A343:I959">

</xml_diff>

<commit_message>
MS-WOPI:update adapter to unverify.
</commit_message>
<xml_diff>
--- a/FileSyncandWOPI/Docs/MS-WOPI/MS-WOPI_RequirementSpecification.xlsx
+++ b/FileSyncandWOPI/Docs/MS-WOPI/MS-WOPI_RequirementSpecification.xlsx
@@ -5812,9 +5812,6 @@
     <t>[In Lock] Implementation does not include header X-WOPI-Lock when responding with the 200 status code. (SharePoint Server 2010 and above follows this behavior).</t>
   </si>
   <si>
-    <t xml:space="preserve">[In Response Body] FileExtension: A string specifying the file extension of the file. </t>
-  </si>
-  <si>
     <t>[In Response Body] This value [FileExtension] MUST begin with a ".".</t>
   </si>
   <si>
@@ -6885,6 +6882,9 @@
   </si>
   <si>
     <t>[In WOPI Protocol Server Details]Implementation does support ExecuteCellStorageRequest (see section 3.3.5.1.8) and ExcecuteCellStorageRelativeRequest (see section 3.3.5.1.9) operations.(Microsoft SharePoint Foundation 2013 and above follow this behavior)</t>
+  </si>
+  <si>
+    <t>[In Response Body] FileExtension: A string specifying the file extension of the file.</t>
   </si>
 </sst>
 </file>
@@ -7172,21 +7172,6 @@
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7210,6 +7195,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8257,7 +8257,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>1426</v>
@@ -8268,127 +8268,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -8401,12 +8401,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -8419,12 +8419,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -8437,12 +8437,12 @@
       <c r="C14" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -8455,60 +8455,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -9491,7 +9491,7 @@
         <v>17</v>
       </c>
       <c r="I57" s="20" t="s">
-        <v>2081</v>
+        <v>2080</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="30">
@@ -9652,7 +9652,7 @@
         <v>730</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
       <c r="D64" s="29"/>
       <c r="E64" s="29" t="s">
@@ -9671,13 +9671,13 @@
     </row>
     <row r="65" spans="1:9" ht="45">
       <c r="A65" s="22" t="s">
-        <v>2064</v>
+        <v>2063</v>
       </c>
       <c r="B65" s="30" t="s">
         <v>730</v>
       </c>
       <c r="C65" s="35" t="s">
-        <v>2066</v>
+        <v>2065</v>
       </c>
       <c r="D65" s="33"/>
       <c r="E65" s="29" t="s">
@@ -9727,7 +9727,7 @@
         <v>730</v>
       </c>
       <c r="C67" s="35" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
       <c r="D67" s="33"/>
       <c r="E67" s="29" t="s">
@@ -9752,7 +9752,7 @@
         <v>730</v>
       </c>
       <c r="C68" s="20" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
       <c r="D68" s="29"/>
       <c r="E68" s="29" t="s">
@@ -9771,13 +9771,13 @@
     </row>
     <row r="69" spans="1:9" ht="30">
       <c r="A69" s="22" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
       <c r="B69" s="30" t="s">
         <v>730</v>
       </c>
       <c r="C69" s="20" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
       <c r="D69" s="33"/>
       <c r="E69" s="22" t="s">
@@ -11331,7 +11331,7 @@
         <v>744</v>
       </c>
       <c r="C131" s="20" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
       <c r="D131" s="29"/>
       <c r="E131" s="29" t="s">
@@ -15659,8 +15659,8 @@
       <c r="B304" s="30" t="s">
         <v>757</v>
       </c>
-      <c r="C304" s="35" t="s">
-        <v>1739</v>
+      <c r="C304" s="20" t="s">
+        <v>2087</v>
       </c>
       <c r="D304" s="33"/>
       <c r="E304" s="29" t="s">
@@ -15682,8 +15682,8 @@
         <v>1519</v>
       </c>
       <c r="B305" s="34"/>
-      <c r="C305" s="35" t="s">
-        <v>1740</v>
+      <c r="C305" s="20" t="s">
+        <v>1739</v>
       </c>
       <c r="D305" s="33"/>
       <c r="E305" s="29" t="s">
@@ -15702,12 +15702,12 @@
     </row>
     <row r="306" spans="1:9" ht="30">
       <c r="A306" s="22" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="B306" s="30" t="s">
         <v>757</v>
       </c>
-      <c r="C306" s="35" t="s">
+      <c r="C306" s="20" t="s">
         <v>1513</v>
       </c>
       <c r="D306" s="33"/>
@@ -15853,7 +15853,7 @@
       </c>
     </row>
     <row r="312" spans="1:9" ht="30">
-      <c r="A312" s="29" t="s">
+      <c r="A312" s="22" t="s">
         <v>298</v>
       </c>
       <c r="B312" s="30" t="s">
@@ -16738,7 +16738,7 @@
         <v>17</v>
       </c>
       <c r="I346" s="20" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="347" spans="1:9" ht="45">
@@ -16775,7 +16775,7 @@
       <c r="B348" s="30" t="s">
         <v>757</v>
       </c>
-      <c r="C348" s="31" t="s">
+      <c r="C348" s="20" t="s">
         <v>1049</v>
       </c>
       <c r="D348" s="29" t="s">
@@ -16846,21 +16846,21 @@
         <v>17</v>
       </c>
       <c r="I350" s="20" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
     </row>
     <row r="351" spans="1:9">
       <c r="A351" s="33" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="B351" s="30" t="s">
         <v>757</v>
       </c>
-      <c r="C351" s="35" t="s">
-        <v>1754</v>
+      <c r="C351" s="20" t="s">
+        <v>1753</v>
       </c>
       <c r="D351" s="33" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="E351" s="29" t="s">
         <v>19</v>
@@ -16878,16 +16878,16 @@
     </row>
     <row r="352" spans="1:9" ht="30">
       <c r="A352" s="33" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="B352" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C352" s="35" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="D352" s="33" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="E352" s="29" t="s">
         <v>19</v>
@@ -16927,21 +16927,21 @@
         <v>17</v>
       </c>
       <c r="I353" s="20" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
     </row>
     <row r="354" spans="1:9">
       <c r="A354" s="33" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="B354" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C354" s="35" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="D354" s="33" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="E354" s="29" t="s">
         <v>19</v>
@@ -16959,16 +16959,16 @@
     </row>
     <row r="355" spans="1:9" ht="30">
       <c r="A355" s="33" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="B355" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C355" s="35" t="s">
+        <v>1748</v>
+      </c>
+      <c r="D355" s="33" t="s">
         <v>1749</v>
-      </c>
-      <c r="D355" s="33" t="s">
-        <v>1750</v>
       </c>
       <c r="E355" s="29" t="s">
         <v>19</v>
@@ -17089,21 +17089,21 @@
         <v>17</v>
       </c>
       <c r="I359" s="20" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
     </row>
     <row r="360" spans="1:9">
       <c r="A360" s="22" t="s">
-        <v>1758</v>
+        <v>1757</v>
       </c>
       <c r="B360" s="30" t="s">
         <v>757</v>
       </c>
-      <c r="C360" s="35" t="s">
-        <v>1756</v>
+      <c r="C360" s="20" t="s">
+        <v>1755</v>
       </c>
       <c r="D360" s="33" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="E360" s="29" t="s">
         <v>19</v>
@@ -17121,16 +17121,16 @@
     </row>
     <row r="361" spans="1:9" ht="30">
       <c r="A361" s="22" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="B361" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C361" s="35" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="D361" s="33" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="E361" s="29" t="s">
         <v>19</v>
@@ -17251,21 +17251,21 @@
         <v>17</v>
       </c>
       <c r="I365" s="20" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="366" spans="1:9">
       <c r="A366" s="22" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="B366" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C366" s="35" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="D366" s="33" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="E366" s="29" t="s">
         <v>19</v>
@@ -17283,16 +17283,16 @@
     </row>
     <row r="367" spans="1:9" ht="30">
       <c r="A367" s="22" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
       <c r="B367" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C367" s="35" t="s">
+        <v>1764</v>
+      </c>
+      <c r="D367" s="33" t="s">
         <v>1765</v>
-      </c>
-      <c r="D367" s="33" t="s">
-        <v>1766</v>
       </c>
       <c r="E367" s="29" t="s">
         <v>19</v>
@@ -17497,7 +17497,7 @@
     </row>
     <row r="375" spans="1:9" ht="60">
       <c r="A375" s="22" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="B375" s="30" t="s">
         <v>757</v>
@@ -17519,21 +17519,21 @@
         <v>17</v>
       </c>
       <c r="I375" s="20" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
     </row>
     <row r="376" spans="1:9">
       <c r="A376" s="22" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="B376" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C376" s="20" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="D376" s="22" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="E376" s="29" t="s">
         <v>19</v>
@@ -17551,16 +17551,16 @@
     </row>
     <row r="377" spans="1:9" ht="30">
       <c r="A377" s="22" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
       <c r="B377" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C377" s="20" t="s">
+        <v>1771</v>
+      </c>
+      <c r="D377" s="22" t="s">
         <v>1772</v>
-      </c>
-      <c r="D377" s="22" t="s">
-        <v>1773</v>
       </c>
       <c r="E377" s="29" t="s">
         <v>19</v>
@@ -17653,7 +17653,7 @@
     </row>
     <row r="381" spans="1:9" ht="45">
       <c r="A381" s="22" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="B381" s="30" t="s">
         <v>757</v>
@@ -17675,21 +17675,21 @@
         <v>17</v>
       </c>
       <c r="I381" s="20" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
     </row>
     <row r="382" spans="1:9">
       <c r="A382" s="22" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="B382" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C382" s="20" t="s">
+        <v>1775</v>
+      </c>
+      <c r="D382" s="22" t="s">
         <v>1776</v>
-      </c>
-      <c r="D382" s="22" t="s">
-        <v>1777</v>
       </c>
       <c r="E382" s="29" t="s">
         <v>19</v>
@@ -17707,7 +17707,7 @@
     </row>
     <row r="383" spans="1:9" ht="30">
       <c r="A383" s="22" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="B383" s="30" t="s">
         <v>757</v>
@@ -17732,7 +17732,7 @@
     </row>
     <row r="384" spans="1:9" ht="30">
       <c r="A384" s="22" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
       <c r="B384" s="30" t="s">
         <v>757</v>
@@ -17988,7 +17988,7 @@
     </row>
     <row r="394" spans="1:9" ht="60">
       <c r="A394" s="22" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="B394" s="30" t="s">
         <v>757</v>
@@ -18010,21 +18010,21 @@
         <v>17</v>
       </c>
       <c r="I394" s="20" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
     </row>
     <row r="395" spans="1:9">
       <c r="A395" s="22" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
       <c r="B395" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C395" s="20" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="D395" s="22" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="E395" s="22" t="s">
         <v>19</v>
@@ -18042,16 +18042,16 @@
     </row>
     <row r="396" spans="1:9" ht="30">
       <c r="A396" s="22" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="B396" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C396" s="20" t="s">
+        <v>1785</v>
+      </c>
+      <c r="D396" s="22" t="s">
         <v>1786</v>
-      </c>
-      <c r="D396" s="22" t="s">
-        <v>1787</v>
       </c>
       <c r="E396" s="22" t="s">
         <v>19</v>
@@ -18225,7 +18225,7 @@
     </row>
     <row r="403" spans="1:9" ht="30">
       <c r="A403" s="22" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
       <c r="B403" s="30" t="s">
         <v>757</v>
@@ -18250,7 +18250,7 @@
     </row>
     <row r="404" spans="1:9" ht="30">
       <c r="A404" s="22" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="B404" s="30" t="s">
         <v>757</v>
@@ -18985,13 +18985,13 @@
     </row>
     <row r="433" spans="1:9" ht="195">
       <c r="A433" s="22" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="B433" s="30" t="s">
         <v>759</v>
       </c>
       <c r="C433" s="20" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
       <c r="D433" s="33"/>
       <c r="E433" s="22" t="s">
@@ -19007,12 +19007,12 @@
         <v>17</v>
       </c>
       <c r="I433" s="35" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
     </row>
     <row r="434" spans="1:9" ht="45">
       <c r="A434" s="22" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="B434" s="30" t="s">
         <v>759</v>
@@ -19037,13 +19037,13 @@
     </row>
     <row r="435" spans="1:9" ht="60">
       <c r="A435" s="22" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
       <c r="B435" s="30" t="s">
         <v>759</v>
       </c>
       <c r="C435" s="20" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="D435" s="33"/>
       <c r="E435" s="22" t="s">
@@ -19059,18 +19059,18 @@
         <v>17</v>
       </c>
       <c r="I435" s="35" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="436" spans="1:9" ht="45">
       <c r="A436" s="22" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="B436" s="30" t="s">
         <v>759</v>
       </c>
       <c r="C436" s="20" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="D436" s="22"/>
       <c r="E436" s="22" t="s">
@@ -19086,12 +19086,12 @@
         <v>17</v>
       </c>
       <c r="I436" s="20" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="437" spans="1:9">
       <c r="A437" s="22" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
       <c r="B437" s="30" t="s">
         <v>759</v>
@@ -19116,7 +19116,7 @@
     </row>
     <row r="438" spans="1:9" ht="30">
       <c r="A438" s="22" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
       <c r="B438" s="30" t="s">
         <v>759</v>
@@ -19141,7 +19141,7 @@
     </row>
     <row r="439" spans="1:9" ht="30">
       <c r="A439" s="22" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="B439" s="30" t="s">
         <v>759</v>
@@ -19166,7 +19166,7 @@
     </row>
     <row r="440" spans="1:9">
       <c r="A440" s="22" t="s">
-        <v>1798</v>
+        <v>1797</v>
       </c>
       <c r="B440" s="30" t="s">
         <v>759</v>
@@ -19185,13 +19185,13 @@
         <v>15</v>
       </c>
       <c r="H440" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I440" s="35"/>
     </row>
     <row r="441" spans="1:9" ht="30">
       <c r="A441" s="22" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="B441" s="30" t="s">
         <v>759</v>
@@ -19216,7 +19216,7 @@
     </row>
     <row r="442" spans="1:9" ht="30">
       <c r="A442" s="22" t="s">
-        <v>1808</v>
+        <v>1807</v>
       </c>
       <c r="B442" s="30" t="s">
         <v>759</v>
@@ -19241,7 +19241,7 @@
     </row>
     <row r="443" spans="1:9" ht="30">
       <c r="A443" s="22" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
       <c r="B443" s="30" t="s">
         <v>759</v>
@@ -19266,7 +19266,7 @@
     </row>
     <row r="444" spans="1:9" ht="45">
       <c r="A444" s="22" t="s">
-        <v>1810</v>
+        <v>1809</v>
       </c>
       <c r="B444" s="30" t="s">
         <v>759</v>
@@ -19288,12 +19288,12 @@
         <v>17</v>
       </c>
       <c r="I444" s="35" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="445" spans="1:9">
       <c r="A445" s="22" t="s">
-        <v>1811</v>
+        <v>1810</v>
       </c>
       <c r="B445" s="30" t="s">
         <v>759</v>
@@ -19311,20 +19311,20 @@
       <c r="G445" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="H445" s="33" t="s">
-        <v>21</v>
+      <c r="H445" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="I445" s="35"/>
     </row>
     <row r="446" spans="1:9" ht="30">
       <c r="A446" s="22" t="s">
-        <v>1816</v>
+        <v>1815</v>
       </c>
       <c r="B446" s="30" t="s">
         <v>759</v>
       </c>
       <c r="C446" s="35" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
       <c r="D446" s="33"/>
       <c r="E446" s="33" t="s">
@@ -19343,7 +19343,7 @@
     </row>
     <row r="447" spans="1:9" ht="45">
       <c r="A447" s="22" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
       <c r="B447" s="30" t="s">
         <v>759</v>
@@ -19365,7 +19365,7 @@
         <v>17</v>
       </c>
       <c r="I447" s="35" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
     </row>
     <row r="448" spans="1:9" ht="30">
@@ -19545,7 +19545,7 @@
     </row>
     <row r="455" spans="1:9" ht="30">
       <c r="A455" s="33" t="s">
-        <v>2061</v>
+        <v>2060</v>
       </c>
       <c r="B455" s="30" t="s">
         <v>759</v>
@@ -20151,7 +20151,7 @@
         <v>763</v>
       </c>
       <c r="C479" s="20" t="s">
-        <v>2073</v>
+        <v>2072</v>
       </c>
       <c r="D479" s="29"/>
       <c r="E479" s="29" t="s">
@@ -20167,7 +20167,7 @@
         <v>17</v>
       </c>
       <c r="I479" s="20" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="480" spans="1:9" ht="30">
@@ -20249,7 +20249,7 @@
     </row>
     <row r="483" spans="1:9">
       <c r="A483" s="33" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
       <c r="B483" s="30" t="s">
         <v>763</v>
@@ -20274,7 +20274,7 @@
     </row>
     <row r="484" spans="1:9">
       <c r="A484" s="33" t="s">
-        <v>1827</v>
+        <v>1826</v>
       </c>
       <c r="B484" s="30" t="s">
         <v>763</v>
@@ -20299,7 +20299,7 @@
     </row>
     <row r="485" spans="1:9" ht="30">
       <c r="A485" s="33" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="B485" s="30" t="s">
         <v>763</v>
@@ -20324,7 +20324,7 @@
     </row>
     <row r="486" spans="1:9" ht="30">
       <c r="A486" s="33" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="B486" s="30" t="s">
         <v>763</v>
@@ -20349,7 +20349,7 @@
     </row>
     <row r="487" spans="1:9" ht="45">
       <c r="A487" s="33" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="B487" s="30" t="s">
         <v>763</v>
@@ -20371,12 +20371,12 @@
         <v>17</v>
       </c>
       <c r="I487" s="20" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="488" spans="1:9">
       <c r="A488" s="33" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
       <c r="B488" s="30" t="s">
         <v>763</v>
@@ -20394,20 +20394,20 @@
       <c r="G488" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="H488" s="33" t="s">
-        <v>21</v>
+      <c r="H488" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="I488" s="35"/>
     </row>
     <row r="489" spans="1:9" ht="30">
       <c r="A489" s="33" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
       <c r="B489" s="30" t="s">
         <v>763</v>
       </c>
       <c r="C489" s="35" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="D489" s="33"/>
       <c r="E489" s="29" t="s">
@@ -20426,7 +20426,7 @@
     </row>
     <row r="490" spans="1:9" ht="45">
       <c r="A490" s="33" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
       <c r="B490" s="30" t="s">
         <v>763</v>
@@ -20448,7 +20448,7 @@
         <v>17</v>
       </c>
       <c r="I490" s="35" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="491" spans="1:9">
@@ -20603,13 +20603,13 @@
     </row>
     <row r="497" spans="1:9" ht="30">
       <c r="A497" s="22" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="B497" s="30" t="s">
         <v>763</v>
       </c>
       <c r="C497" s="35" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
       <c r="D497" s="33"/>
       <c r="E497" s="33" t="s">
@@ -20978,13 +20978,13 @@
     </row>
     <row r="512" spans="1:9" ht="135">
       <c r="A512" s="33" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
       <c r="B512" s="30" t="s">
         <v>765</v>
       </c>
       <c r="C512" s="20" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
       <c r="D512" s="33"/>
       <c r="E512" s="33" t="s">
@@ -21000,12 +21000,12 @@
         <v>17</v>
       </c>
       <c r="I512" s="20" t="s">
-        <v>2083</v>
+        <v>2082</v>
       </c>
     </row>
     <row r="513" spans="1:9" ht="30">
       <c r="A513" s="33" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
       <c r="B513" s="30" t="s">
         <v>765</v>
@@ -21030,7 +21030,7 @@
     </row>
     <row r="514" spans="1:9" ht="30">
       <c r="A514" s="22" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
       <c r="B514" s="30" t="s">
         <v>765</v>
@@ -21055,7 +21055,7 @@
     </row>
     <row r="515" spans="1:9" ht="45">
       <c r="A515" s="33" t="s">
-        <v>1846</v>
+        <v>1845</v>
       </c>
       <c r="B515" s="30" t="s">
         <v>765</v>
@@ -21077,12 +21077,12 @@
         <v>17</v>
       </c>
       <c r="I515" s="35" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
     </row>
     <row r="516" spans="1:9">
       <c r="A516" s="22" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
       <c r="B516" s="30" t="s">
         <v>765</v>
@@ -21100,14 +21100,14 @@
       <c r="G516" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="H516" s="33" t="s">
-        <v>21</v>
+      <c r="H516" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="I516" s="35"/>
     </row>
     <row r="517" spans="1:9">
       <c r="A517" s="33" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="B517" s="30" t="s">
         <v>765</v>
@@ -21132,7 +21132,7 @@
     </row>
     <row r="518" spans="1:9" ht="30">
       <c r="A518" s="33" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="B518" s="30" t="s">
         <v>765</v>
@@ -21157,7 +21157,7 @@
     </row>
     <row r="519" spans="1:9" ht="30">
       <c r="A519" s="33" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
       <c r="B519" s="30" t="s">
         <v>765</v>
@@ -21182,7 +21182,7 @@
     </row>
     <row r="520" spans="1:9" ht="45">
       <c r="A520" s="33" t="s">
-        <v>1851</v>
+        <v>1850</v>
       </c>
       <c r="B520" s="30" t="s">
         <v>765</v>
@@ -21204,12 +21204,12 @@
         <v>17</v>
       </c>
       <c r="I520" s="35" t="s">
-        <v>1862</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="521" spans="1:9">
       <c r="A521" s="22" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="B521" s="30" t="s">
         <v>765</v>
@@ -21227,20 +21227,20 @@
       <c r="G521" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="H521" s="33" t="s">
-        <v>21</v>
+      <c r="H521" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="I521" s="35"/>
     </row>
     <row r="522" spans="1:9" ht="30">
       <c r="A522" s="33" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="B522" s="30" t="s">
         <v>765</v>
       </c>
       <c r="C522" s="35" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="D522" s="33"/>
       <c r="E522" s="33" t="s">
@@ -21259,7 +21259,7 @@
     </row>
     <row r="523" spans="1:9" ht="45">
       <c r="A523" s="33" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="B523" s="30" t="s">
         <v>765</v>
@@ -21281,7 +21281,7 @@
         <v>17</v>
       </c>
       <c r="I523" s="35" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
     </row>
     <row r="524" spans="1:9">
@@ -21761,13 +21761,13 @@
     </row>
     <row r="543" spans="1:9" ht="135">
       <c r="A543" s="22" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
       <c r="B543" s="30" t="s">
         <v>767</v>
       </c>
       <c r="C543" s="20" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="D543" s="33"/>
       <c r="E543" s="29" t="s">
@@ -21783,12 +21783,12 @@
         <v>17</v>
       </c>
       <c r="I543" s="20" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
     </row>
     <row r="544" spans="1:9" ht="30">
       <c r="A544" s="22" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="B544" s="30" t="s">
         <v>767</v>
@@ -21813,7 +21813,7 @@
     </row>
     <row r="545" spans="1:9" ht="30">
       <c r="A545" s="22" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="B545" s="30" t="s">
         <v>767</v>
@@ -21838,7 +21838,7 @@
     </row>
     <row r="546" spans="1:9" ht="45">
       <c r="A546" s="22" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="B546" s="30" t="s">
         <v>767</v>
@@ -21860,12 +21860,12 @@
         <v>17</v>
       </c>
       <c r="I546" s="35" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
     </row>
     <row r="547" spans="1:9">
       <c r="A547" s="22" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
       <c r="B547" s="30" t="s">
         <v>767</v>
@@ -21883,14 +21883,14 @@
       <c r="G547" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="H547" s="33" t="s">
-        <v>21</v>
+      <c r="H547" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="I547" s="35"/>
     </row>
     <row r="548" spans="1:9">
       <c r="A548" s="22" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="B548" s="30" t="s">
         <v>767</v>
@@ -21915,7 +21915,7 @@
     </row>
     <row r="549" spans="1:9" ht="30">
       <c r="A549" s="22" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="B549" s="30" t="s">
         <v>767</v>
@@ -21940,7 +21940,7 @@
     </row>
     <row r="550" spans="1:9" ht="30">
       <c r="A550" s="22" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="B550" s="30" t="s">
         <v>767</v>
@@ -21965,7 +21965,7 @@
     </row>
     <row r="551" spans="1:9" ht="45">
       <c r="A551" s="22" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="B551" s="30" t="s">
         <v>767</v>
@@ -21987,12 +21987,12 @@
         <v>17</v>
       </c>
       <c r="I551" s="20" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="552" spans="1:9">
       <c r="A552" s="22" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="B552" s="30" t="s">
         <v>767</v>
@@ -22010,20 +22010,20 @@
       <c r="G552" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="H552" s="33" t="s">
-        <v>21</v>
+      <c r="H552" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="I552" s="35"/>
     </row>
     <row r="553" spans="1:9" ht="30">
       <c r="A553" s="22" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="B553" s="30" t="s">
         <v>767</v>
       </c>
       <c r="C553" s="35" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
       <c r="D553" s="33"/>
       <c r="E553" s="29" t="s">
@@ -22042,7 +22042,7 @@
     </row>
     <row r="554" spans="1:9" ht="45">
       <c r="A554" s="22" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
       <c r="B554" s="30" t="s">
         <v>767</v>
@@ -22064,7 +22064,7 @@
         <v>17</v>
       </c>
       <c r="I554" s="35" t="s">
-        <v>1892</v>
+        <v>1891</v>
       </c>
     </row>
     <row r="555" spans="1:9" ht="30">
@@ -22644,20 +22644,20 @@
     </row>
     <row r="578" spans="1:9" ht="135">
       <c r="A578" s="33" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="B578" s="30" t="s">
         <v>769</v>
       </c>
       <c r="C578" s="20" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
       <c r="D578" s="33"/>
       <c r="E578" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F578" s="33" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="G578" s="22" t="s">
         <v>15</v>
@@ -22666,12 +22666,12 @@
         <v>17</v>
       </c>
       <c r="I578" s="20" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
     </row>
     <row r="579" spans="1:9" ht="30">
       <c r="A579" s="33" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="B579" s="30" t="s">
         <v>769</v>
@@ -22684,7 +22684,7 @@
         <v>19</v>
       </c>
       <c r="F579" s="33" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="G579" s="33" t="s">
         <v>15</v>
@@ -22696,7 +22696,7 @@
     </row>
     <row r="580" spans="1:9" ht="30">
       <c r="A580" s="33" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
       <c r="B580" s="30" t="s">
         <v>769</v>
@@ -22709,7 +22709,7 @@
         <v>19</v>
       </c>
       <c r="F580" s="33" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="G580" s="33" t="s">
         <v>15</v>
@@ -22721,7 +22721,7 @@
     </row>
     <row r="581" spans="1:9" ht="45">
       <c r="A581" s="33" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="B581" s="30" t="s">
         <v>769</v>
@@ -22734,7 +22734,7 @@
         <v>19</v>
       </c>
       <c r="F581" s="33" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="G581" s="33" t="s">
         <v>15</v>
@@ -22743,12 +22743,12 @@
         <v>17</v>
       </c>
       <c r="I581" s="35" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="582" spans="1:9">
       <c r="A582" s="33" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="B582" s="30" t="s">
         <v>769</v>
@@ -22761,7 +22761,7 @@
         <v>19</v>
       </c>
       <c r="F582" s="33" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="G582" s="33" t="s">
         <v>15</v>
@@ -22773,7 +22773,7 @@
     </row>
     <row r="583" spans="1:9" ht="30">
       <c r="A583" s="33" t="s">
-        <v>1900</v>
+        <v>1899</v>
       </c>
       <c r="B583" s="30" t="s">
         <v>769</v>
@@ -22786,7 +22786,7 @@
         <v>19</v>
       </c>
       <c r="F583" s="33" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="G583" s="33" t="s">
         <v>16</v>
@@ -22798,7 +22798,7 @@
     </row>
     <row r="584" spans="1:9" ht="30">
       <c r="A584" s="33" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
       <c r="B584" s="30" t="s">
         <v>769</v>
@@ -22811,7 +22811,7 @@
         <v>19</v>
       </c>
       <c r="F584" s="33" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="G584" s="33" t="s">
         <v>16</v>
@@ -22823,7 +22823,7 @@
     </row>
     <row r="585" spans="1:9">
       <c r="A585" s="33" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
       <c r="B585" s="30" t="s">
         <v>769</v>
@@ -22836,7 +22836,7 @@
         <v>19</v>
       </c>
       <c r="F585" s="33" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="G585" s="33" t="s">
         <v>15</v>
@@ -22848,20 +22848,20 @@
     </row>
     <row r="586" spans="1:9" ht="45">
       <c r="A586" s="33" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
       <c r="B586" s="30" t="s">
         <v>769</v>
       </c>
       <c r="C586" s="35" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="D586" s="33"/>
       <c r="E586" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F586" s="33" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="G586" s="33" t="s">
         <v>15</v>
@@ -22870,12 +22870,12 @@
         <v>17</v>
       </c>
       <c r="I586" s="35" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="587" spans="1:9">
       <c r="A587" s="22" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
       <c r="B587" s="30" t="s">
         <v>769</v>
@@ -22888,32 +22888,32 @@
         <v>19</v>
       </c>
       <c r="F587" s="33" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="G587" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="H587" s="33" t="s">
-        <v>21</v>
+      <c r="H587" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="I587" s="35"/>
     </row>
     <row r="588" spans="1:9" ht="30">
       <c r="A588" s="33" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="B588" s="30" t="s">
         <v>769</v>
       </c>
       <c r="C588" s="35" t="s">
-        <v>1895</v>
+        <v>1894</v>
       </c>
       <c r="D588" s="33"/>
       <c r="E588" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F588" s="33" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="G588" s="33" t="s">
         <v>15</v>
@@ -22925,7 +22925,7 @@
     </row>
     <row r="589" spans="1:9" ht="45">
       <c r="A589" s="33" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="B589" s="30" t="s">
         <v>769</v>
@@ -22938,7 +22938,7 @@
         <v>19</v>
       </c>
       <c r="F589" s="33" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="G589" s="33" t="s">
         <v>15</v>
@@ -22947,7 +22947,7 @@
         <v>17</v>
       </c>
       <c r="I589" s="35" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="590" spans="1:9" ht="30">
@@ -23227,7 +23227,7 @@
     </row>
     <row r="601" spans="1:9">
       <c r="A601" s="33" t="s">
-        <v>1924</v>
+        <v>1923</v>
       </c>
       <c r="B601" s="34" t="s">
         <v>771</v>
@@ -23252,7 +23252,7 @@
     </row>
     <row r="602" spans="1:9" ht="45">
       <c r="A602" s="33" t="s">
-        <v>1925</v>
+        <v>1924</v>
       </c>
       <c r="B602" s="34" t="s">
         <v>771</v>
@@ -23277,7 +23277,7 @@
     </row>
     <row r="603" spans="1:9" ht="30">
       <c r="A603" s="33" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="B603" s="34" t="s">
         <v>771</v>
@@ -23302,7 +23302,7 @@
     </row>
     <row r="604" spans="1:9" ht="30">
       <c r="A604" s="33" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
       <c r="B604" s="34" t="s">
         <v>771</v>
@@ -23327,7 +23327,7 @@
     </row>
     <row r="605" spans="1:9">
       <c r="A605" s="33" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
       <c r="B605" s="34" t="s">
         <v>771</v>
@@ -23352,7 +23352,7 @@
     </row>
     <row r="606" spans="1:9">
       <c r="A606" s="33" t="s">
-        <v>1929</v>
+        <v>1928</v>
       </c>
       <c r="B606" s="34" t="s">
         <v>771</v>
@@ -23377,7 +23377,7 @@
     </row>
     <row r="607" spans="1:9" ht="150">
       <c r="A607" s="33" t="s">
-        <v>1930</v>
+        <v>1929</v>
       </c>
       <c r="B607" s="34" t="s">
         <v>771</v>
@@ -23399,12 +23399,12 @@
         <v>17</v>
       </c>
       <c r="I607" s="35" t="s">
-        <v>2080</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="608" spans="1:9" ht="30">
       <c r="A608" s="33" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
       <c r="B608" s="34" t="s">
         <v>771</v>
@@ -23429,13 +23429,13 @@
     </row>
     <row r="609" spans="1:9" ht="45">
       <c r="A609" s="33" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="B609" s="34" t="s">
         <v>771</v>
       </c>
       <c r="C609" s="35" t="s">
-        <v>1923</v>
+        <v>1922</v>
       </c>
       <c r="D609" s="33"/>
       <c r="E609" s="29" t="s">
@@ -23454,13 +23454,13 @@
     </row>
     <row r="610" spans="1:9" ht="45">
       <c r="A610" s="33" t="s">
-        <v>1933</v>
+        <v>1932</v>
       </c>
       <c r="B610" s="34" t="s">
         <v>771</v>
       </c>
       <c r="C610" s="35" t="s">
-        <v>1922</v>
+        <v>1921</v>
       </c>
       <c r="D610" s="33"/>
       <c r="E610" s="33" t="s">
@@ -23479,7 +23479,7 @@
     </row>
     <row r="611" spans="1:9">
       <c r="A611" s="33" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
       <c r="B611" s="34" t="s">
         <v>771</v>
@@ -23504,7 +23504,7 @@
     </row>
     <row r="612" spans="1:9">
       <c r="A612" s="33" t="s">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="B612" s="34" t="s">
         <v>771</v>
@@ -23529,7 +23529,7 @@
     </row>
     <row r="613" spans="1:9" ht="30">
       <c r="A613" s="33" t="s">
-        <v>1936</v>
+        <v>1935</v>
       </c>
       <c r="B613" s="34" t="s">
         <v>771</v>
@@ -23554,7 +23554,7 @@
     </row>
     <row r="614" spans="1:9" ht="30">
       <c r="A614" s="33" t="s">
-        <v>1937</v>
+        <v>1936</v>
       </c>
       <c r="B614" s="34" t="s">
         <v>771</v>
@@ -23579,7 +23579,7 @@
     </row>
     <row r="615" spans="1:9" ht="45">
       <c r="A615" s="33" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
       <c r="B615" s="34" t="s">
         <v>771</v>
@@ -23601,12 +23601,12 @@
         <v>17</v>
       </c>
       <c r="I615" s="35" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="616" spans="1:9">
       <c r="A616" s="33" t="s">
-        <v>1939</v>
+        <v>1938</v>
       </c>
       <c r="B616" s="34" t="s">
         <v>771</v>
@@ -23631,13 +23631,13 @@
     </row>
     <row r="617" spans="1:9" ht="30">
       <c r="A617" s="33" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="B617" s="34" t="s">
         <v>771</v>
       </c>
       <c r="C617" s="35" t="s">
-        <v>1921</v>
+        <v>1920</v>
       </c>
       <c r="D617" s="33"/>
       <c r="E617" s="29" t="s">
@@ -23656,7 +23656,7 @@
     </row>
     <row r="618" spans="1:9" ht="45">
       <c r="A618" s="33" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="B618" s="34" t="s">
         <v>771</v>
@@ -23669,7 +23669,7 @@
         <v>19</v>
       </c>
       <c r="F618" s="33" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="G618" s="33" t="s">
         <v>15</v>
@@ -23678,12 +23678,12 @@
         <v>17</v>
       </c>
       <c r="I618" s="35" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="619" spans="1:9" ht="30">
       <c r="A619" s="33" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="B619" s="34" t="s">
         <v>771</v>
@@ -23708,7 +23708,7 @@
     </row>
     <row r="620" spans="1:9">
       <c r="A620" s="33" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="B620" s="34" t="s">
         <v>771</v>
@@ -23733,7 +23733,7 @@
     </row>
     <row r="621" spans="1:9">
       <c r="A621" s="33" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="B621" s="34" t="s">
         <v>771</v>
@@ -23758,7 +23758,7 @@
     </row>
     <row r="622" spans="1:9">
       <c r="A622" s="33" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="B622" s="34" t="s">
         <v>771</v>
@@ -23783,7 +23783,7 @@
     </row>
     <row r="623" spans="1:9">
       <c r="A623" s="33" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="B623" s="34" t="s">
         <v>771</v>
@@ -23808,7 +23808,7 @@
     </row>
     <row r="624" spans="1:9">
       <c r="A624" s="33" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
       <c r="B624" s="34" t="s">
         <v>771</v>
@@ -23833,7 +23833,7 @@
     </row>
     <row r="625" spans="1:9" ht="30">
       <c r="A625" s="33" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="B625" s="34" t="s">
         <v>771</v>
@@ -23858,7 +23858,7 @@
     </row>
     <row r="626" spans="1:9">
       <c r="A626" s="33" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="B626" s="34" t="s">
         <v>771</v>
@@ -23883,7 +23883,7 @@
     </row>
     <row r="627" spans="1:9">
       <c r="A627" s="33" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="B627" s="34" t="s">
         <v>771</v>
@@ -23908,7 +23908,7 @@
     </row>
     <row r="628" spans="1:9">
       <c r="A628" s="33" t="s">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="B628" s="34" t="s">
         <v>772</v>
@@ -26130,7 +26130,7 @@
         <v>17</v>
       </c>
       <c r="I716" s="20" t="s">
-        <v>2077</v>
+        <v>2076</v>
       </c>
     </row>
     <row r="717" spans="1:9" ht="30">
@@ -26860,7 +26860,7 @@
     </row>
     <row r="746" spans="1:9">
       <c r="A746" s="33" t="s">
-        <v>1963</v>
+        <v>1962</v>
       </c>
       <c r="B746" s="24" t="s">
         <v>1647</v>
@@ -26885,7 +26885,7 @@
     </row>
     <row r="747" spans="1:9" ht="45">
       <c r="A747" s="33" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="B747" s="24" t="s">
         <v>1647</v>
@@ -26910,7 +26910,7 @@
     </row>
     <row r="748" spans="1:9" ht="75">
       <c r="A748" s="33" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="B748" s="24" t="s">
         <v>1647</v>
@@ -26935,7 +26935,7 @@
     </row>
     <row r="749" spans="1:9" ht="30">
       <c r="A749" s="33" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
       <c r="B749" s="24" t="s">
         <v>1647</v>
@@ -26960,7 +26960,7 @@
     </row>
     <row r="750" spans="1:9">
       <c r="A750" s="33" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
       <c r="B750" s="24" t="s">
         <v>1647</v>
@@ -26985,7 +26985,7 @@
     </row>
     <row r="751" spans="1:9">
       <c r="A751" s="33" t="s">
-        <v>1968</v>
+        <v>1967</v>
       </c>
       <c r="B751" s="24" t="s">
         <v>1647</v>
@@ -27010,7 +27010,7 @@
     </row>
     <row r="752" spans="1:9" ht="30">
       <c r="A752" s="33" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
       <c r="B752" s="24" t="s">
         <v>1647</v>
@@ -27035,7 +27035,7 @@
     </row>
     <row r="753" spans="1:9">
       <c r="A753" s="33" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="B753" s="24" t="s">
         <v>1647</v>
@@ -27060,7 +27060,7 @@
     </row>
     <row r="754" spans="1:9" ht="30">
       <c r="A754" s="33" t="s">
-        <v>1971</v>
+        <v>1970</v>
       </c>
       <c r="B754" s="24" t="s">
         <v>1647</v>
@@ -27085,7 +27085,7 @@
     </row>
     <row r="755" spans="1:9">
       <c r="A755" s="33" t="s">
-        <v>1972</v>
+        <v>1971</v>
       </c>
       <c r="B755" s="24" t="s">
         <v>1647</v>
@@ -27110,7 +27110,7 @@
     </row>
     <row r="756" spans="1:9">
       <c r="A756" s="33" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
       <c r="B756" s="24" t="s">
         <v>1647</v>
@@ -27135,7 +27135,7 @@
     </row>
     <row r="757" spans="1:9">
       <c r="A757" s="33" t="s">
-        <v>1974</v>
+        <v>1973</v>
       </c>
       <c r="B757" s="24" t="s">
         <v>1647</v>
@@ -27160,7 +27160,7 @@
     </row>
     <row r="758" spans="1:9" ht="90">
       <c r="A758" s="33" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
       <c r="B758" s="24" t="s">
         <v>1647</v>
@@ -27185,7 +27185,7 @@
     </row>
     <row r="759" spans="1:9" ht="30">
       <c r="A759" s="33" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="B759" s="24" t="s">
         <v>1647</v>
@@ -27210,7 +27210,7 @@
     </row>
     <row r="760" spans="1:9" ht="30">
       <c r="A760" s="33" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="B760" s="24" t="s">
         <v>1647</v>
@@ -27235,7 +27235,7 @@
     </row>
     <row r="761" spans="1:9" ht="30">
       <c r="A761" s="33" t="s">
-        <v>1978</v>
+        <v>1977</v>
       </c>
       <c r="B761" s="24" t="s">
         <v>1647</v>
@@ -27260,7 +27260,7 @@
     </row>
     <row r="762" spans="1:9" ht="45">
       <c r="A762" s="33" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
       <c r="B762" s="24" t="s">
         <v>1647</v>
@@ -27282,12 +27282,12 @@
         <v>17</v>
       </c>
       <c r="I762" s="35" t="s">
-        <v>2023</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="763" spans="1:9">
       <c r="A763" s="33" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
       <c r="B763" s="24" t="s">
         <v>1647</v>
@@ -27312,7 +27312,7 @@
     </row>
     <row r="764" spans="1:9" ht="30">
       <c r="A764" s="33" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="B764" s="24" t="s">
         <v>1647</v>
@@ -27337,7 +27337,7 @@
     </row>
     <row r="765" spans="1:9" ht="30">
       <c r="A765" s="33" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="B765" s="24" t="s">
         <v>1647</v>
@@ -27362,7 +27362,7 @@
     </row>
     <row r="766" spans="1:9" ht="45">
       <c r="A766" s="33" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="B766" s="24" t="s">
         <v>1647</v>
@@ -27384,12 +27384,12 @@
         <v>17</v>
       </c>
       <c r="I766" s="35" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="767" spans="1:9">
       <c r="A767" s="33" t="s">
-        <v>1984</v>
+        <v>1983</v>
       </c>
       <c r="B767" s="24" t="s">
         <v>1647</v>
@@ -27414,7 +27414,7 @@
     </row>
     <row r="768" spans="1:9">
       <c r="A768" s="33" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="B768" s="24" t="s">
         <v>1647</v>
@@ -27439,7 +27439,7 @@
     </row>
     <row r="769" spans="1:9" ht="30">
       <c r="A769" s="33" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
       <c r="B769" s="24" t="s">
         <v>1647</v>
@@ -27464,7 +27464,7 @@
     </row>
     <row r="770" spans="1:9" ht="30">
       <c r="A770" s="33" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
       <c r="B770" s="24" t="s">
         <v>1647</v>
@@ -27489,7 +27489,7 @@
     </row>
     <row r="771" spans="1:9" ht="45">
       <c r="A771" s="33" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="B771" s="24" t="s">
         <v>1647</v>
@@ -27511,12 +27511,12 @@
         <v>17</v>
       </c>
       <c r="I771" s="35" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
     </row>
     <row r="772" spans="1:9">
       <c r="A772" s="33" t="s">
-        <v>1989</v>
+        <v>1988</v>
       </c>
       <c r="B772" s="24" t="s">
         <v>1647</v>
@@ -27541,13 +27541,13 @@
     </row>
     <row r="773" spans="1:9" ht="30">
       <c r="A773" s="33" t="s">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="B773" s="24" t="s">
         <v>1647</v>
       </c>
       <c r="C773" s="35" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
       <c r="D773" s="33"/>
       <c r="E773" s="33" t="s">
@@ -27566,7 +27566,7 @@
     </row>
     <row r="774" spans="1:9" ht="45">
       <c r="A774" s="33" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="B774" s="24" t="s">
         <v>1647</v>
@@ -27588,12 +27588,12 @@
         <v>17</v>
       </c>
       <c r="I774" s="35" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
     </row>
     <row r="775" spans="1:9" ht="30">
       <c r="A775" s="33" t="s">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="B775" s="24" t="s">
         <v>1647</v>
@@ -27618,7 +27618,7 @@
     </row>
     <row r="776" spans="1:9">
       <c r="A776" s="33" t="s">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="B776" s="24" t="s">
         <v>1647</v>
@@ -27643,7 +27643,7 @@
     </row>
     <row r="777" spans="1:9">
       <c r="A777" s="33" t="s">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="B777" s="24" t="s">
         <v>1647</v>
@@ -27668,7 +27668,7 @@
     </row>
     <row r="778" spans="1:9">
       <c r="A778" s="33" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="B778" s="24" t="s">
         <v>1647</v>
@@ -27693,7 +27693,7 @@
     </row>
     <row r="779" spans="1:9">
       <c r="A779" s="33" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="B779" s="24" t="s">
         <v>1647</v>
@@ -27718,7 +27718,7 @@
     </row>
     <row r="780" spans="1:9">
       <c r="A780" s="33" t="s">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="B780" s="24" t="s">
         <v>1647</v>
@@ -27743,7 +27743,7 @@
     </row>
     <row r="781" spans="1:9" ht="30">
       <c r="A781" s="33" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="B781" s="24" t="s">
         <v>1647</v>
@@ -27768,7 +27768,7 @@
     </row>
     <row r="782" spans="1:9">
       <c r="A782" s="33" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="B782" s="24" t="s">
         <v>1647</v>
@@ -27793,7 +27793,7 @@
     </row>
     <row r="783" spans="1:9">
       <c r="A783" s="33" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="B783" s="24" t="s">
         <v>1647</v>
@@ -27818,7 +27818,7 @@
     </row>
     <row r="784" spans="1:9" ht="105">
       <c r="A784" s="33" t="s">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="B784" s="24" t="s">
         <v>1647</v>
@@ -27843,7 +27843,7 @@
     </row>
     <row r="785" spans="1:9">
       <c r="A785" s="33" t="s">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="B785" s="24" t="s">
         <v>1647</v>
@@ -27868,7 +27868,7 @@
     </row>
     <row r="786" spans="1:9">
       <c r="A786" s="33" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="B786" s="34" t="s">
         <v>1686</v>
@@ -27893,7 +27893,7 @@
     </row>
     <row r="787" spans="1:9" ht="45">
       <c r="A787" s="33" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="B787" s="34" t="s">
         <v>1686</v>
@@ -27918,7 +27918,7 @@
     </row>
     <row r="788" spans="1:9" ht="45">
       <c r="A788" s="33" t="s">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="B788" s="34" t="s">
         <v>1686</v>
@@ -27943,7 +27943,7 @@
     </row>
     <row r="789" spans="1:9" ht="30">
       <c r="A789" s="33" t="s">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="B789" s="34" t="s">
         <v>1686</v>
@@ -27968,7 +27968,7 @@
     </row>
     <row r="790" spans="1:9">
       <c r="A790" s="33" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="B790" s="34" t="s">
         <v>1686</v>
@@ -27993,7 +27993,7 @@
     </row>
     <row r="791" spans="1:9">
       <c r="A791" s="33" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="B791" s="34" t="s">
         <v>1686</v>
@@ -28018,7 +28018,7 @@
     </row>
     <row r="792" spans="1:9" ht="30">
       <c r="A792" s="33" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="B792" s="34" t="s">
         <v>1686</v>
@@ -28043,7 +28043,7 @@
     </row>
     <row r="793" spans="1:9">
       <c r="A793" s="33" t="s">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="B793" s="34" t="s">
         <v>1686</v>
@@ -28068,7 +28068,7 @@
     </row>
     <row r="794" spans="1:9">
       <c r="A794" s="33" t="s">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="B794" s="34" t="s">
         <v>1686</v>
@@ -28093,7 +28093,7 @@
     </row>
     <row r="795" spans="1:9">
       <c r="A795" s="33" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="B795" s="34" t="s">
         <v>1686</v>
@@ -28118,7 +28118,7 @@
     </row>
     <row r="796" spans="1:9">
       <c r="A796" s="33" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="B796" s="34" t="s">
         <v>1686</v>
@@ -28143,7 +28143,7 @@
     </row>
     <row r="797" spans="1:9">
       <c r="A797" s="33" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="B797" s="34" t="s">
         <v>1686</v>
@@ -28168,7 +28168,7 @@
     </row>
     <row r="798" spans="1:9">
       <c r="A798" s="33" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="B798" s="34" t="s">
         <v>1686</v>
@@ -28193,7 +28193,7 @@
     </row>
     <row r="799" spans="1:9">
       <c r="A799" s="33" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B799" s="34" t="s">
         <v>1686</v>
@@ -28218,7 +28218,7 @@
     </row>
     <row r="800" spans="1:9">
       <c r="A800" s="33" t="s">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B800" s="34" t="s">
         <v>1686</v>
@@ -28243,7 +28243,7 @@
     </row>
     <row r="801" spans="1:9" ht="30">
       <c r="A801" s="33" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="B801" s="34" t="s">
         <v>1686</v>
@@ -28268,7 +28268,7 @@
     </row>
     <row r="802" spans="1:9" ht="30">
       <c r="A802" s="33" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B802" s="34" t="s">
         <v>1686</v>
@@ -30272,13 +30272,13 @@
     </row>
     <row r="882" spans="1:9" ht="135">
       <c r="A882" s="33" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="B882" s="30" t="s">
         <v>793</v>
       </c>
       <c r="C882" s="35" t="s">
-        <v>2078</v>
+        <v>2077</v>
       </c>
       <c r="D882" s="33"/>
       <c r="E882" s="33" t="s">
@@ -30294,12 +30294,12 @@
         <v>17</v>
       </c>
       <c r="I882" s="20" t="s">
-        <v>2086</v>
+        <v>2085</v>
       </c>
     </row>
     <row r="883" spans="1:9" ht="30">
       <c r="A883" s="33" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
       <c r="B883" s="30" t="s">
         <v>793</v>
@@ -30324,7 +30324,7 @@
     </row>
     <row r="884" spans="1:9" ht="30">
       <c r="A884" s="33" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
       <c r="B884" s="30" t="s">
         <v>793</v>
@@ -30349,7 +30349,7 @@
     </row>
     <row r="885" spans="1:9" ht="45">
       <c r="A885" s="33" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
       <c r="B885" s="30" t="s">
         <v>793</v>
@@ -30371,12 +30371,12 @@
         <v>17</v>
       </c>
       <c r="I885" s="35" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="886" spans="1:9">
       <c r="A886" s="33" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
       <c r="B886" s="30" t="s">
         <v>793</v>
@@ -30401,7 +30401,7 @@
     </row>
     <row r="887" spans="1:9">
       <c r="A887" s="33" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
       <c r="B887" s="30" t="s">
         <v>793</v>
@@ -30426,7 +30426,7 @@
     </row>
     <row r="888" spans="1:9" ht="30">
       <c r="A888" s="33" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="B888" s="30" t="s">
         <v>793</v>
@@ -30451,7 +30451,7 @@
     </row>
     <row r="889" spans="1:9" ht="30">
       <c r="A889" s="33" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
       <c r="B889" s="30" t="s">
         <v>793</v>
@@ -30476,7 +30476,7 @@
     </row>
     <row r="890" spans="1:9" ht="45">
       <c r="A890" s="33" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
       <c r="B890" s="30" t="s">
         <v>793</v>
@@ -30498,12 +30498,12 @@
         <v>17</v>
       </c>
       <c r="I890" s="35" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
     </row>
     <row r="891" spans="1:9">
       <c r="A891" s="33" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="B891" s="30" t="s">
         <v>793</v>
@@ -30521,20 +30521,20 @@
       <c r="G891" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="H891" s="33" t="s">
-        <v>21</v>
+      <c r="H891" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="I891" s="35"/>
     </row>
     <row r="892" spans="1:9" ht="30">
       <c r="A892" s="33" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="B892" s="30" t="s">
         <v>793</v>
       </c>
       <c r="C892" s="35" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="D892" s="33"/>
       <c r="E892" s="33" t="s">
@@ -30553,7 +30553,7 @@
     </row>
     <row r="893" spans="1:9" ht="45">
       <c r="A893" s="33" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
       <c r="B893" s="30" t="s">
         <v>793</v>
@@ -30575,7 +30575,7 @@
         <v>17</v>
       </c>
       <c r="I893" s="35" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="894" spans="1:9">
@@ -30730,7 +30730,7 @@
     </row>
     <row r="900" spans="1:9" ht="30">
       <c r="A900" s="33" t="s">
-        <v>2062</v>
+        <v>2061</v>
       </c>
       <c r="B900" s="30" t="s">
         <v>793</v>
@@ -31544,7 +31544,7 @@
         <v>800</v>
       </c>
       <c r="C932" s="20" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
       <c r="D932" s="29" t="s">
         <v>1405</v>
@@ -31605,7 +31605,7 @@
         <v>1733</v>
       </c>
       <c r="D934" s="33" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="E934" s="29" t="s">
         <v>22</v>
@@ -31632,7 +31632,7 @@
         <v>1738</v>
       </c>
       <c r="D935" s="33" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="E935" s="29" t="s">
         <v>22</v>
@@ -31652,16 +31652,16 @@
     </row>
     <row r="936" spans="1:9" ht="60">
       <c r="A936" s="22" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="B936" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C936" s="20" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="D936" s="33" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
       <c r="E936" s="29" t="s">
         <v>22</v>
@@ -31679,16 +31679,16 @@
     </row>
     <row r="937" spans="1:9" ht="60">
       <c r="A937" s="33" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="B937" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C937" s="35" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="D937" s="33" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="E937" s="29" t="s">
         <v>22</v>
@@ -31706,16 +31706,16 @@
     </row>
     <row r="938" spans="1:9" ht="45">
       <c r="A938" s="33" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
       <c r="B938" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C938" s="35" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="D938" s="33" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="E938" s="29" t="s">
         <v>22</v>
@@ -31735,16 +31735,16 @@
     </row>
     <row r="939" spans="1:9" ht="45">
       <c r="A939" s="33" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="B939" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C939" s="35" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="D939" s="33" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="E939" s="29" t="s">
         <v>22</v>
@@ -31764,16 +31764,16 @@
     </row>
     <row r="940" spans="1:9" ht="45">
       <c r="A940" s="22" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
       <c r="B940" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C940" s="20" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
       <c r="D940" s="33" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="E940" s="29" t="s">
         <v>22</v>
@@ -31793,16 +31793,16 @@
     </row>
     <row r="941" spans="1:9" ht="45">
       <c r="A941" s="33" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
       <c r="B941" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C941" s="35" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="D941" s="33" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="E941" s="29" t="s">
         <v>22</v>
@@ -31822,16 +31822,16 @@
     </row>
     <row r="942" spans="1:9" ht="45">
       <c r="A942" s="33" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="B942" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C942" s="35" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
       <c r="D942" s="33" t="s">
-        <v>1867</v>
+        <v>1866</v>
       </c>
       <c r="E942" s="29" t="s">
         <v>22</v>
@@ -31851,16 +31851,16 @@
     </row>
     <row r="943" spans="1:9" ht="45">
       <c r="A943" s="22" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
       <c r="B943" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C943" s="35" t="s">
-        <v>1861</v>
+        <v>1860</v>
       </c>
       <c r="D943" s="33" t="s">
-        <v>1866</v>
+        <v>1865</v>
       </c>
       <c r="E943" s="29" t="s">
         <v>22</v>
@@ -31880,16 +31880,16 @@
     </row>
     <row r="944" spans="1:9" ht="45">
       <c r="A944" s="33" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="B944" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C944" s="20" t="s">
+        <v>1863</v>
+      </c>
+      <c r="D944" s="33" t="s">
         <v>1864</v>
-      </c>
-      <c r="D944" s="33" t="s">
-        <v>1865</v>
       </c>
       <c r="E944" s="29" t="s">
         <v>22</v>
@@ -31907,16 +31907,16 @@
     </row>
     <row r="945" spans="1:9" ht="45">
       <c r="A945" s="33" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="B945" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C945" s="35" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="D945" s="33" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="E945" s="29" t="s">
         <v>22</v>
@@ -31936,16 +31936,16 @@
     </row>
     <row r="946" spans="1:9" ht="45">
       <c r="A946" s="22" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
       <c r="B946" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C946" s="20" t="s">
-        <v>1888</v>
+        <v>1887</v>
       </c>
       <c r="D946" s="22" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="E946" s="29" t="s">
         <v>22</v>
@@ -31965,16 +31965,16 @@
     </row>
     <row r="947" spans="1:9" ht="45">
       <c r="A947" s="22" t="s">
-        <v>1890</v>
+        <v>1889</v>
       </c>
       <c r="B947" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C947" s="20" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
       <c r="D947" s="22" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="E947" s="29" t="s">
         <v>22</v>
@@ -31992,16 +31992,16 @@
     </row>
     <row r="948" spans="1:9" ht="45">
       <c r="A948" s="33" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="B948" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C948" s="35" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="D948" s="33" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
       <c r="E948" s="29" t="s">
         <v>22</v>
@@ -32021,16 +32021,16 @@
     </row>
     <row r="949" spans="1:9" ht="45">
       <c r="A949" s="22" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="B949" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C949" s="35" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="D949" s="33" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
       <c r="E949" s="29" t="s">
         <v>22</v>
@@ -32050,16 +32050,16 @@
     </row>
     <row r="950" spans="1:9" ht="45">
       <c r="A950" s="33" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="B950" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C950" s="35" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="D950" s="33" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="E950" s="29" t="s">
         <v>22</v>
@@ -32079,16 +32079,16 @@
     </row>
     <row r="951" spans="1:9" ht="45">
       <c r="A951" s="33" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="B951" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C951" s="35" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="D951" s="33" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="E951" s="29" t="s">
         <v>22</v>
@@ -32106,16 +32106,16 @@
     </row>
     <row r="952" spans="1:9" ht="45">
       <c r="A952" s="33" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="B952" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C952" s="35" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="D952" s="33" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="E952" s="29" t="s">
         <v>22</v>
@@ -32133,16 +32133,16 @@
     </row>
     <row r="953" spans="1:9" ht="45">
       <c r="A953" s="33" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="B953" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C953" s="35" t="s">
+        <v>2020</v>
+      </c>
+      <c r="D953" s="33" t="s">
         <v>2021</v>
-      </c>
-      <c r="D953" s="33" t="s">
-        <v>2022</v>
       </c>
       <c r="E953" s="29" t="s">
         <v>22</v>
@@ -32160,16 +32160,16 @@
     </row>
     <row r="954" spans="1:9" ht="45">
       <c r="A954" s="33" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="B954" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C954" s="35" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="D954" s="33" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="E954" s="29" t="s">
         <v>22</v>
@@ -32187,16 +32187,16 @@
     </row>
     <row r="955" spans="1:9" ht="45">
       <c r="A955" s="33" t="s">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="B955" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C955" s="35" t="s">
-        <v>2033</v>
+        <v>2032</v>
       </c>
       <c r="D955" s="33" t="s">
-        <v>2029</v>
+        <v>2028</v>
       </c>
       <c r="E955" s="29" t="s">
         <v>22</v>
@@ -32214,16 +32214,16 @@
     </row>
     <row r="956" spans="1:9" ht="45">
       <c r="A956" s="33" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="B956" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C956" s="35" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
       <c r="D956" s="33" t="s">
-        <v>2032</v>
+        <v>2031</v>
       </c>
       <c r="E956" s="29" t="s">
         <v>22</v>
@@ -32241,16 +32241,16 @@
     </row>
     <row r="957" spans="1:9" ht="45">
       <c r="A957" s="33" t="s">
-        <v>2049</v>
+        <v>2048</v>
       </c>
       <c r="B957" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C957" s="35" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
       <c r="D957" s="33" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
       <c r="E957" s="29" t="s">
         <v>22</v>
@@ -32270,16 +32270,16 @@
     </row>
     <row r="958" spans="1:9" ht="45">
       <c r="A958" s="33" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="B958" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C958" s="35" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
       <c r="D958" s="33" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="E958" s="29" t="s">
         <v>22</v>
@@ -32299,16 +32299,16 @@
     </row>
     <row r="959" spans="1:9" ht="45">
       <c r="A959" s="33" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
       <c r="B959" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C959" s="35" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
       <c r="D959" s="33" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
       <c r="E959" s="29" t="s">
         <v>22</v>
@@ -32363,7 +32363,7 @@
         <v>8</v>
       </c>
       <c r="C961" s="35" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="D961" s="33" t="s">
         <v>1728</v>
@@ -32405,6 +32405,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -32412,11 +32417,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="I20:I46 D342:I342 A342:B342 A962:I962 A961 A960:D960 E960:E961 A20:H341 F960:I960 F961:H961 A36:I341 A343:I959">

</xml_diff>

<commit_message>
MS-WOPI: chang R292004, R292005, R778001001 to Unverified.
</commit_message>
<xml_diff>
--- a/FileSyncandWOPI/Docs/MS-WOPI/MS-WOPI_RequirementSpecification.xlsx
+++ b/FileSyncandWOPI/Docs/MS-WOPI/MS-WOPI_RequirementSpecification.xlsx
@@ -7172,6 +7172,21 @@
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7196,26 +7211,41 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="57">
+  <dxfs count="63">
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -7877,34 +7907,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I961" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I961" tableType="xml" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" connectionId="1">
   <autoFilter ref="A19:I961"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="22">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="21">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="20">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="19">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="18">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="17">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -7913,12 +7943,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="2"/>
-    <tableColumn id="2" name="Test" dataDxfId="1"/>
-    <tableColumn id="3" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" name="Scope" dataDxfId="8"/>
+    <tableColumn id="2" name="Test" dataDxfId="7"/>
+    <tableColumn id="3" name="Description" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8268,127 +8298,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -8401,12 +8431,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -8419,12 +8449,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -8437,12 +8467,12 @@
       <c r="C14" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -8455,60 +8485,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -15672,8 +15702,8 @@
       <c r="G304" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="H304" s="33" t="s">
-        <v>21</v>
+      <c r="H304" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="I304" s="35"/>
     </row>
@@ -15695,8 +15725,8 @@
       <c r="G305" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="H305" s="33" t="s">
-        <v>21</v>
+      <c r="H305" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="I305" s="35"/>
     </row>
@@ -17114,8 +17144,8 @@
       <c r="G360" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="H360" s="33" t="s">
-        <v>21</v>
+      <c r="H360" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="I360" s="35"/>
     </row>
@@ -32405,11 +32435,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -32417,145 +32442,150 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="I20:I46 D342:I342 A342:B342 A962:I962 A961 A960:D960 E960:E961 A20:H341 F960:I960 F961:H961 A36:I341 A343:I959">
-    <cfRule type="expression" dxfId="56" priority="83">
+  <conditionalFormatting sqref="I20:I46 D342:I342 A342:B342 A962:I962 A961 A960:D960 E960:E961 A20:H341 F960:I960 F961:H961 A343:I959 A36:I341">
+    <cfRule type="expression" dxfId="62" priority="83">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="84">
+    <cfRule type="expression" dxfId="61" priority="84">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="91">
+    <cfRule type="expression" dxfId="60" priority="91">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20:I46 D342:I342 A342:B342 A962:I962 A961 A960:D960 E960:E961 A20:H341 F960:I960 F961:H961 A36:I341 A343:I959">
-    <cfRule type="expression" dxfId="53" priority="37">
+  <conditionalFormatting sqref="I20:I46 D342:I342 A342:B342 A962:I962 A961 A960:D960 E960:E961 A20:H341 F960:I960 F961:H961 A343:I959 A36:I341">
+    <cfRule type="expression" dxfId="59" priority="37">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="38">
+    <cfRule type="expression" dxfId="58" priority="38">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="39">
+    <cfRule type="expression" dxfId="57" priority="39">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F962">
-    <cfRule type="expression" dxfId="50" priority="43">
+    <cfRule type="expression" dxfId="56" priority="43">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="44">
+    <cfRule type="expression" dxfId="55" priority="44">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C342">
-    <cfRule type="expression" dxfId="48" priority="28">
+    <cfRule type="expression" dxfId="54" priority="28">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="29">
+    <cfRule type="expression" dxfId="53" priority="29">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="30">
+    <cfRule type="expression" dxfId="52" priority="30">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C342">
-    <cfRule type="expression" dxfId="45" priority="25">
+    <cfRule type="expression" dxfId="51" priority="25">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="26">
+    <cfRule type="expression" dxfId="50" priority="26">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="27">
+    <cfRule type="expression" dxfId="49" priority="27">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B961">
-    <cfRule type="expression" dxfId="42" priority="22">
+    <cfRule type="expression" dxfId="48" priority="22">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="23">
+    <cfRule type="expression" dxfId="47" priority="23">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="24">
+    <cfRule type="expression" dxfId="46" priority="24">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B961">
-    <cfRule type="expression" dxfId="39" priority="19">
+    <cfRule type="expression" dxfId="45" priority="19">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="20">
+    <cfRule type="expression" dxfId="44" priority="20">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="21">
+    <cfRule type="expression" dxfId="43" priority="21">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C961">
-    <cfRule type="expression" dxfId="36" priority="16">
+    <cfRule type="expression" dxfId="42" priority="16">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="17">
+    <cfRule type="expression" dxfId="41" priority="17">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="18">
+    <cfRule type="expression" dxfId="40" priority="18">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C961">
-    <cfRule type="expression" dxfId="33" priority="13">
+    <cfRule type="expression" dxfId="39" priority="13">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="14">
+    <cfRule type="expression" dxfId="38" priority="14">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="15">
+    <cfRule type="expression" dxfId="37" priority="15">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D961">
-    <cfRule type="expression" dxfId="30" priority="10">
+    <cfRule type="expression" dxfId="36" priority="10">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="11">
+    <cfRule type="expression" dxfId="35" priority="11">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="12">
+    <cfRule type="expression" dxfId="34" priority="12">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D961">
-    <cfRule type="expression" dxfId="27" priority="7">
+    <cfRule type="expression" dxfId="33" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="8">
+    <cfRule type="expression" dxfId="32" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="9">
+    <cfRule type="expression" dxfId="31" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I961">
-    <cfRule type="expression" dxfId="24" priority="4">
+    <cfRule type="expression" dxfId="30" priority="4">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="5">
+    <cfRule type="expression" dxfId="29" priority="5">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="6">
+    <cfRule type="expression" dxfId="28" priority="6">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I961">
-    <cfRule type="expression" dxfId="21" priority="1">
+    <cfRule type="expression" dxfId="27" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="2">
+    <cfRule type="expression" dxfId="26" priority="2">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="3">
+    <cfRule type="expression" dxfId="25" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Ms-WOPI:disable  r685003 on O16
</commit_message>
<xml_diff>
--- a/FileSyncandWOPI/Docs/MS-WOPI/MS-WOPI_RequirementSpecification.xlsx
+++ b/FileSyncandWOPI/Docs/MS-WOPI/MS-WOPI_RequirementSpecification.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6787" uniqueCount="2088">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6788" uniqueCount="2088">
   <si>
     <t>Req ID</t>
   </si>
@@ -7215,37 +7215,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="63">
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
+  <dxfs count="57">
     <dxf>
       <font>
         <b val="0"/>
@@ -7907,34 +7877,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I961" tableType="xml" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I961" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
   <autoFilter ref="A19:I961"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="22">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="21">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="20">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="19">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="18">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="17">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="16">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="15">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="14">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -7943,12 +7913,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="8"/>
-    <tableColumn id="2" name="Test" dataDxfId="7"/>
-    <tableColumn id="3" name="Description" dataDxfId="6"/>
+    <tableColumn id="1" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -30352,7 +30322,7 @@
       </c>
       <c r="I883" s="35"/>
     </row>
-    <row r="884" spans="1:9" ht="30">
+    <row r="884" spans="1:9" ht="45">
       <c r="A884" s="33" t="s">
         <v>2038</v>
       </c>
@@ -30372,10 +30342,12 @@
       <c r="G884" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="H884" s="33" t="s">
+      <c r="H884" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="I884" s="35"/>
+      <c r="I884" s="35" t="s">
+        <v>1423</v>
+      </c>
     </row>
     <row r="885" spans="1:9" ht="45">
       <c r="A885" s="33" t="s">
@@ -31759,7 +31731,7 @@
       <c r="H938" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="I938" s="31" t="s">
+      <c r="I938" s="20" t="s">
         <v>1423</v>
       </c>
     </row>
@@ -32450,142 +32422,142 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="I20:I46 D342:I342 A342:B342 A962:I962 A961 A960:D960 E960:E961 A20:H341 F960:I960 F961:H961 A343:I959 A36:I341">
-    <cfRule type="expression" dxfId="62" priority="83">
+    <cfRule type="expression" dxfId="56" priority="83">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="84">
+    <cfRule type="expression" dxfId="55" priority="84">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="91">
+    <cfRule type="expression" dxfId="54" priority="91">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:I46 D342:I342 A342:B342 A962:I962 A961 A960:D960 E960:E961 A20:H341 F960:I960 F961:H961 A343:I959 A36:I341">
-    <cfRule type="expression" dxfId="59" priority="37">
+    <cfRule type="expression" dxfId="53" priority="37">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="38">
+    <cfRule type="expression" dxfId="52" priority="38">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="39">
+    <cfRule type="expression" dxfId="51" priority="39">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F962">
-    <cfRule type="expression" dxfId="56" priority="43">
+    <cfRule type="expression" dxfId="50" priority="43">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="44">
+    <cfRule type="expression" dxfId="49" priority="44">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C342">
-    <cfRule type="expression" dxfId="54" priority="28">
+    <cfRule type="expression" dxfId="48" priority="28">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="29">
+    <cfRule type="expression" dxfId="47" priority="29">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="30">
+    <cfRule type="expression" dxfId="46" priority="30">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C342">
-    <cfRule type="expression" dxfId="51" priority="25">
+    <cfRule type="expression" dxfId="45" priority="25">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="26">
+    <cfRule type="expression" dxfId="44" priority="26">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="27">
+    <cfRule type="expression" dxfId="43" priority="27">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B961">
-    <cfRule type="expression" dxfId="48" priority="22">
+    <cfRule type="expression" dxfId="42" priority="22">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="23">
+    <cfRule type="expression" dxfId="41" priority="23">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="24">
+    <cfRule type="expression" dxfId="40" priority="24">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B961">
-    <cfRule type="expression" dxfId="45" priority="19">
+    <cfRule type="expression" dxfId="39" priority="19">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="20">
+    <cfRule type="expression" dxfId="38" priority="20">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="21">
+    <cfRule type="expression" dxfId="37" priority="21">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C961">
-    <cfRule type="expression" dxfId="42" priority="16">
+    <cfRule type="expression" dxfId="36" priority="16">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="17">
+    <cfRule type="expression" dxfId="35" priority="17">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="18">
+    <cfRule type="expression" dxfId="34" priority="18">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C961">
-    <cfRule type="expression" dxfId="39" priority="13">
+    <cfRule type="expression" dxfId="33" priority="13">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="14">
+    <cfRule type="expression" dxfId="32" priority="14">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="15">
+    <cfRule type="expression" dxfId="31" priority="15">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D961">
-    <cfRule type="expression" dxfId="36" priority="10">
+    <cfRule type="expression" dxfId="30" priority="10">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="11">
+    <cfRule type="expression" dxfId="29" priority="11">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="12">
+    <cfRule type="expression" dxfId="28" priority="12">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D961">
-    <cfRule type="expression" dxfId="33" priority="7">
+    <cfRule type="expression" dxfId="27" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="8">
+    <cfRule type="expression" dxfId="26" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="9">
+    <cfRule type="expression" dxfId="25" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I961">
-    <cfRule type="expression" dxfId="30" priority="4">
+    <cfRule type="expression" dxfId="24" priority="4">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="5">
+    <cfRule type="expression" dxfId="23" priority="5">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="6">
+    <cfRule type="expression" dxfId="22" priority="6">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I961">
-    <cfRule type="expression" dxfId="27" priority="1">
+    <cfRule type="expression" dxfId="21" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="2">
+    <cfRule type="expression" dxfId="20" priority="2">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="3">
+    <cfRule type="expression" dxfId="19" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
MS-WOPI: Update rs to generate report.
</commit_message>
<xml_diff>
--- a/FileSyncandWOPI/Docs/MS-WOPI/MS-WOPI_RequirementSpecification.xlsx
+++ b/FileSyncandWOPI/Docs/MS-WOPI/MS-WOPI_RequirementSpecification.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6788" uniqueCount="2088">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6789" uniqueCount="2088">
   <si>
     <t>Req ID</t>
   </si>
@@ -5779,9 +5779,6 @@
     <t>MS-WOPI_R950002</t>
   </si>
   <si>
-    <t>MS-WOPI_R950:1</t>
-  </si>
-  <si>
     <t>[In Response Body] Implementation does return the value false for field SupportsCoauth. &lt;1&gt; Section 3.3.5.1.1.2:  SharePoint Foundation 2013, SharePoint Server 2013 and above return the value false for the SupportsCoauth field.</t>
   </si>
   <si>
@@ -6885,6 +6882,9 @@
   </si>
   <si>
     <t>[In Response Body] FileExtension: A string specifying the file extension of the file.</t>
+  </si>
+  <si>
+    <t>MS-WOPI_R950:i</t>
   </si>
 </sst>
 </file>
@@ -7172,21 +7172,6 @@
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7210,6 +7195,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8218,7 +8218,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
     <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
@@ -8257,7 +8257,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>2062</v>
+        <v>2061</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>1426</v>
@@ -8268,127 +8268,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -8401,12 +8401,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -8419,12 +8419,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -8437,12 +8437,12 @@
       <c r="C14" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -8455,60 +8455,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -9491,7 +9491,7 @@
         <v>17</v>
       </c>
       <c r="I57" s="20" t="s">
-        <v>2080</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="30">
@@ -9652,7 +9652,7 @@
         <v>730</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>2064</v>
+        <v>2063</v>
       </c>
       <c r="D64" s="29"/>
       <c r="E64" s="29" t="s">
@@ -9671,13 +9671,13 @@
     </row>
     <row r="65" spans="1:9" ht="45">
       <c r="A65" s="22" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
       <c r="B65" s="30" t="s">
         <v>730</v>
       </c>
       <c r="C65" s="35" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
       <c r="D65" s="33"/>
       <c r="E65" s="29" t="s">
@@ -9727,7 +9727,7 @@
         <v>730</v>
       </c>
       <c r="C67" s="35" t="s">
-        <v>2066</v>
+        <v>2065</v>
       </c>
       <c r="D67" s="33"/>
       <c r="E67" s="29" t="s">
@@ -9752,7 +9752,7 @@
         <v>730</v>
       </c>
       <c r="C68" s="20" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
       <c r="D68" s="29"/>
       <c r="E68" s="29" t="s">
@@ -9771,13 +9771,13 @@
     </row>
     <row r="69" spans="1:9" ht="30">
       <c r="A69" s="22" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
       <c r="B69" s="30" t="s">
         <v>730</v>
       </c>
       <c r="C69" s="20" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
       <c r="D69" s="33"/>
       <c r="E69" s="22" t="s">
@@ -9818,7 +9818,7 @@
         <v>17</v>
       </c>
       <c r="I70" s="20" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="30">
@@ -11331,7 +11331,7 @@
         <v>744</v>
       </c>
       <c r="C131" s="20" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
       <c r="D131" s="29"/>
       <c r="E131" s="29" t="s">
@@ -15660,7 +15660,7 @@
         <v>757</v>
       </c>
       <c r="C304" s="20" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
       <c r="D304" s="33"/>
       <c r="E304" s="29" t="s">
@@ -15681,9 +15681,11 @@
       <c r="A305" s="22" t="s">
         <v>1519</v>
       </c>
-      <c r="B305" s="34"/>
+      <c r="B305" s="30" t="s">
+        <v>757</v>
+      </c>
       <c r="C305" s="20" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="D305" s="33"/>
       <c r="E305" s="29" t="s">
@@ -15702,7 +15704,7 @@
     </row>
     <row r="306" spans="1:9" ht="30">
       <c r="A306" s="22" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="B306" s="30" t="s">
         <v>757</v>
@@ -16738,7 +16740,7 @@
         <v>17</v>
       </c>
       <c r="I346" s="20" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="347" spans="1:9" ht="45">
@@ -16846,21 +16848,21 @@
         <v>17</v>
       </c>
       <c r="I350" s="20" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="351" spans="1:9">
       <c r="A351" s="33" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="B351" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C351" s="20" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
       <c r="D351" s="33" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="E351" s="29" t="s">
         <v>19</v>
@@ -16878,16 +16880,16 @@
     </row>
     <row r="352" spans="1:9" ht="30">
       <c r="A352" s="33" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="B352" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C352" s="35" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="D352" s="33" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="E352" s="29" t="s">
         <v>19</v>
@@ -16927,21 +16929,21 @@
         <v>17</v>
       </c>
       <c r="I353" s="20" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
     </row>
     <row r="354" spans="1:9">
       <c r="A354" s="33" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="B354" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C354" s="35" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
       <c r="D354" s="33" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="E354" s="29" t="s">
         <v>19</v>
@@ -16959,16 +16961,16 @@
     </row>
     <row r="355" spans="1:9" ht="30">
       <c r="A355" s="33" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="B355" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C355" s="35" t="s">
+        <v>1747</v>
+      </c>
+      <c r="D355" s="33" t="s">
         <v>1748</v>
-      </c>
-      <c r="D355" s="33" t="s">
-        <v>1749</v>
       </c>
       <c r="E355" s="29" t="s">
         <v>19</v>
@@ -17089,21 +17091,21 @@
         <v>17</v>
       </c>
       <c r="I359" s="20" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="360" spans="1:9">
       <c r="A360" s="22" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="B360" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C360" s="20" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="D360" s="33" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="E360" s="29" t="s">
         <v>19</v>
@@ -17121,16 +17123,16 @@
     </row>
     <row r="361" spans="1:9" ht="30">
       <c r="A361" s="22" t="s">
-        <v>1758</v>
+        <v>1757</v>
       </c>
       <c r="B361" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C361" s="35" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="D361" s="33" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="E361" s="29" t="s">
         <v>19</v>
@@ -17251,21 +17253,21 @@
         <v>17</v>
       </c>
       <c r="I365" s="20" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="366" spans="1:9">
       <c r="A366" s="22" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
       <c r="B366" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C366" s="35" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
       <c r="D366" s="33" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
       <c r="E366" s="29" t="s">
         <v>19</v>
@@ -17283,16 +17285,16 @@
     </row>
     <row r="367" spans="1:9" ht="30">
       <c r="A367" s="22" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="B367" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C367" s="35" t="s">
+        <v>1763</v>
+      </c>
+      <c r="D367" s="33" t="s">
         <v>1764</v>
-      </c>
-      <c r="D367" s="33" t="s">
-        <v>1765</v>
       </c>
       <c r="E367" s="29" t="s">
         <v>19</v>
@@ -17497,7 +17499,7 @@
     </row>
     <row r="375" spans="1:9" ht="60">
       <c r="A375" s="22" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
       <c r="B375" s="30" t="s">
         <v>757</v>
@@ -17519,21 +17521,21 @@
         <v>17</v>
       </c>
       <c r="I375" s="20" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
     </row>
     <row r="376" spans="1:9">
       <c r="A376" s="22" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="B376" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C376" s="20" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
       <c r="D376" s="22" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="E376" s="29" t="s">
         <v>19</v>
@@ -17551,16 +17553,16 @@
     </row>
     <row r="377" spans="1:9" ht="30">
       <c r="A377" s="22" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="B377" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C377" s="20" t="s">
+        <v>1770</v>
+      </c>
+      <c r="D377" s="22" t="s">
         <v>1771</v>
-      </c>
-      <c r="D377" s="22" t="s">
-        <v>1772</v>
       </c>
       <c r="E377" s="29" t="s">
         <v>19</v>
@@ -17653,7 +17655,7 @@
     </row>
     <row r="381" spans="1:9" ht="45">
       <c r="A381" s="22" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="B381" s="30" t="s">
         <v>757</v>
@@ -17675,21 +17677,21 @@
         <v>17</v>
       </c>
       <c r="I381" s="20" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
     </row>
     <row r="382" spans="1:9">
       <c r="A382" s="22" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="B382" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C382" s="20" t="s">
+        <v>1774</v>
+      </c>
+      <c r="D382" s="22" t="s">
         <v>1775</v>
-      </c>
-      <c r="D382" s="22" t="s">
-        <v>1776</v>
       </c>
       <c r="E382" s="29" t="s">
         <v>19</v>
@@ -17707,7 +17709,7 @@
     </row>
     <row r="383" spans="1:9" ht="30">
       <c r="A383" s="22" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="B383" s="30" t="s">
         <v>757</v>
@@ -17732,7 +17734,7 @@
     </row>
     <row r="384" spans="1:9" ht="30">
       <c r="A384" s="22" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="B384" s="30" t="s">
         <v>757</v>
@@ -17988,7 +17990,7 @@
     </row>
     <row r="394" spans="1:9" ht="60">
       <c r="A394" s="22" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
       <c r="B394" s="30" t="s">
         <v>757</v>
@@ -18010,21 +18012,21 @@
         <v>17</v>
       </c>
       <c r="I394" s="20" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
     </row>
     <row r="395" spans="1:9">
       <c r="A395" s="22" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="B395" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C395" s="20" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="D395" s="22" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
       <c r="E395" s="22" t="s">
         <v>19</v>
@@ -18042,16 +18044,16 @@
     </row>
     <row r="396" spans="1:9" ht="30">
       <c r="A396" s="22" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
       <c r="B396" s="30" t="s">
         <v>757</v>
       </c>
       <c r="C396" s="20" t="s">
+        <v>1784</v>
+      </c>
+      <c r="D396" s="22" t="s">
         <v>1785</v>
-      </c>
-      <c r="D396" s="22" t="s">
-        <v>1786</v>
       </c>
       <c r="E396" s="22" t="s">
         <v>19</v>
@@ -18225,7 +18227,7 @@
     </row>
     <row r="403" spans="1:9" ht="30">
       <c r="A403" s="22" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
       <c r="B403" s="30" t="s">
         <v>757</v>
@@ -18250,7 +18252,7 @@
     </row>
     <row r="404" spans="1:9" ht="30">
       <c r="A404" s="22" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
       <c r="B404" s="30" t="s">
         <v>757</v>
@@ -18985,13 +18987,13 @@
     </row>
     <row r="433" spans="1:9" ht="195">
       <c r="A433" s="22" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="B433" s="30" t="s">
         <v>759</v>
       </c>
       <c r="C433" s="20" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
       <c r="D433" s="33"/>
       <c r="E433" s="22" t="s">
@@ -19007,12 +19009,12 @@
         <v>17</v>
       </c>
       <c r="I433" s="35" t="s">
-        <v>2078</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="434" spans="1:9" ht="45">
       <c r="A434" s="22" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="B434" s="30" t="s">
         <v>759</v>
@@ -19037,13 +19039,13 @@
     </row>
     <row r="435" spans="1:9" ht="60">
       <c r="A435" s="22" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="B435" s="30" t="s">
         <v>759</v>
       </c>
       <c r="C435" s="20" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="D435" s="33"/>
       <c r="E435" s="22" t="s">
@@ -19059,18 +19061,18 @@
         <v>17</v>
       </c>
       <c r="I435" s="35" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="436" spans="1:9" ht="45">
       <c r="A436" s="22" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
       <c r="B436" s="30" t="s">
         <v>759</v>
       </c>
       <c r="C436" s="20" t="s">
-        <v>1798</v>
+        <v>1797</v>
       </c>
       <c r="D436" s="22"/>
       <c r="E436" s="22" t="s">
@@ -19086,12 +19088,12 @@
         <v>17</v>
       </c>
       <c r="I436" s="20" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="437" spans="1:9">
       <c r="A437" s="22" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="B437" s="30" t="s">
         <v>759</v>
@@ -19116,7 +19118,7 @@
     </row>
     <row r="438" spans="1:9" ht="30">
       <c r="A438" s="22" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
       <c r="B438" s="30" t="s">
         <v>759</v>
@@ -19141,7 +19143,7 @@
     </row>
     <row r="439" spans="1:9" ht="30">
       <c r="A439" s="22" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
       <c r="B439" s="30" t="s">
         <v>759</v>
@@ -19166,7 +19168,7 @@
     </row>
     <row r="440" spans="1:9">
       <c r="A440" s="22" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="B440" s="30" t="s">
         <v>759</v>
@@ -19191,7 +19193,7 @@
     </row>
     <row r="441" spans="1:9" ht="30">
       <c r="A441" s="22" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="B441" s="30" t="s">
         <v>759</v>
@@ -19216,7 +19218,7 @@
     </row>
     <row r="442" spans="1:9" ht="30">
       <c r="A442" s="22" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="B442" s="30" t="s">
         <v>759</v>
@@ -19241,7 +19243,7 @@
     </row>
     <row r="443" spans="1:9" ht="30">
       <c r="A443" s="22" t="s">
-        <v>1808</v>
+        <v>1807</v>
       </c>
       <c r="B443" s="30" t="s">
         <v>759</v>
@@ -19266,7 +19268,7 @@
     </row>
     <row r="444" spans="1:9" ht="45">
       <c r="A444" s="22" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
       <c r="B444" s="30" t="s">
         <v>759</v>
@@ -19288,12 +19290,12 @@
         <v>17</v>
       </c>
       <c r="I444" s="35" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
     </row>
     <row r="445" spans="1:9">
       <c r="A445" s="22" t="s">
-        <v>1810</v>
+        <v>1809</v>
       </c>
       <c r="B445" s="30" t="s">
         <v>759</v>
@@ -19318,13 +19320,13 @@
     </row>
     <row r="446" spans="1:9" ht="30">
       <c r="A446" s="22" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
       <c r="B446" s="30" t="s">
         <v>759</v>
       </c>
       <c r="C446" s="35" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="D446" s="33"/>
       <c r="E446" s="33" t="s">
@@ -19343,7 +19345,7 @@
     </row>
     <row r="447" spans="1:9" ht="45">
       <c r="A447" s="22" t="s">
-        <v>1816</v>
+        <v>1815</v>
       </c>
       <c r="B447" s="30" t="s">
         <v>759</v>
@@ -19365,7 +19367,7 @@
         <v>17</v>
       </c>
       <c r="I447" s="35" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="448" spans="1:9" ht="30">
@@ -19545,7 +19547,7 @@
     </row>
     <row r="455" spans="1:9" ht="30">
       <c r="A455" s="33" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="B455" s="30" t="s">
         <v>759</v>
@@ -20151,7 +20153,7 @@
         <v>763</v>
       </c>
       <c r="C479" s="20" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
       <c r="D479" s="29"/>
       <c r="E479" s="29" t="s">
@@ -20167,7 +20169,7 @@
         <v>17</v>
       </c>
       <c r="I479" s="20" t="s">
-        <v>2081</v>
+        <v>2080</v>
       </c>
     </row>
     <row r="480" spans="1:9" ht="30">
@@ -20197,7 +20199,7 @@
     </row>
     <row r="481" spans="1:9" ht="30">
       <c r="A481" s="33" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="B481" s="30" t="s">
         <v>763</v>
@@ -20222,7 +20224,7 @@
     </row>
     <row r="482" spans="1:9" ht="45">
       <c r="A482" s="33" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="B482" s="30" t="s">
         <v>763</v>
@@ -20244,12 +20246,12 @@
         <v>17</v>
       </c>
       <c r="I482" s="35" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="483" spans="1:9">
       <c r="A483" s="33" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="B483" s="30" t="s">
         <v>763</v>
@@ -20274,7 +20276,7 @@
     </row>
     <row r="484" spans="1:9">
       <c r="A484" s="33" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
       <c r="B484" s="30" t="s">
         <v>763</v>
@@ -20299,7 +20301,7 @@
     </row>
     <row r="485" spans="1:9" ht="30">
       <c r="A485" s="33" t="s">
-        <v>1827</v>
+        <v>1826</v>
       </c>
       <c r="B485" s="30" t="s">
         <v>763</v>
@@ -20324,7 +20326,7 @@
     </row>
     <row r="486" spans="1:9" ht="30">
       <c r="A486" s="33" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="B486" s="30" t="s">
         <v>763</v>
@@ -20349,7 +20351,7 @@
     </row>
     <row r="487" spans="1:9" ht="45">
       <c r="A487" s="33" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="B487" s="30" t="s">
         <v>763</v>
@@ -20371,12 +20373,12 @@
         <v>17</v>
       </c>
       <c r="I487" s="20" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="488" spans="1:9">
       <c r="A488" s="33" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="B488" s="30" t="s">
         <v>763</v>
@@ -20401,13 +20403,13 @@
     </row>
     <row r="489" spans="1:9" ht="30">
       <c r="A489" s="33" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
       <c r="B489" s="30" t="s">
         <v>763</v>
       </c>
       <c r="C489" s="35" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
       <c r="D489" s="33"/>
       <c r="E489" s="29" t="s">
@@ -20426,7 +20428,7 @@
     </row>
     <row r="490" spans="1:9" ht="45">
       <c r="A490" s="33" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
       <c r="B490" s="30" t="s">
         <v>763</v>
@@ -20448,7 +20450,7 @@
         <v>17</v>
       </c>
       <c r="I490" s="35" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="491" spans="1:9">
@@ -20603,13 +20605,13 @@
     </row>
     <row r="497" spans="1:9" ht="30">
       <c r="A497" s="22" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
       <c r="B497" s="30" t="s">
         <v>763</v>
       </c>
       <c r="C497" s="35" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="D497" s="33"/>
       <c r="E497" s="33" t="s">
@@ -20978,13 +20980,13 @@
     </row>
     <row r="512" spans="1:9" ht="135">
       <c r="A512" s="33" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="B512" s="30" t="s">
         <v>765</v>
       </c>
       <c r="C512" s="20" t="s">
-        <v>2073</v>
+        <v>2072</v>
       </c>
       <c r="D512" s="33"/>
       <c r="E512" s="33" t="s">
@@ -21000,12 +21002,12 @@
         <v>17</v>
       </c>
       <c r="I512" s="20" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="513" spans="1:9" ht="30">
       <c r="A513" s="33" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
       <c r="B513" s="30" t="s">
         <v>765</v>
@@ -21030,7 +21032,7 @@
     </row>
     <row r="514" spans="1:9" ht="30">
       <c r="A514" s="22" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
       <c r="B514" s="30" t="s">
         <v>765</v>
@@ -21055,7 +21057,7 @@
     </row>
     <row r="515" spans="1:9" ht="45">
       <c r="A515" s="33" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
       <c r="B515" s="30" t="s">
         <v>765</v>
@@ -21077,12 +21079,12 @@
         <v>17</v>
       </c>
       <c r="I515" s="35" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
     </row>
     <row r="516" spans="1:9">
       <c r="A516" s="22" t="s">
-        <v>1846</v>
+        <v>1845</v>
       </c>
       <c r="B516" s="30" t="s">
         <v>765</v>
@@ -21107,7 +21109,7 @@
     </row>
     <row r="517" spans="1:9">
       <c r="A517" s="33" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
       <c r="B517" s="30" t="s">
         <v>765</v>
@@ -21132,7 +21134,7 @@
     </row>
     <row r="518" spans="1:9" ht="30">
       <c r="A518" s="33" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="B518" s="30" t="s">
         <v>765</v>
@@ -21157,7 +21159,7 @@
     </row>
     <row r="519" spans="1:9" ht="30">
       <c r="A519" s="33" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="B519" s="30" t="s">
         <v>765</v>
@@ -21182,7 +21184,7 @@
     </row>
     <row r="520" spans="1:9" ht="45">
       <c r="A520" s="33" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
       <c r="B520" s="30" t="s">
         <v>765</v>
@@ -21204,12 +21206,12 @@
         <v>17</v>
       </c>
       <c r="I520" s="35" t="s">
-        <v>1861</v>
+        <v>1860</v>
       </c>
     </row>
     <row r="521" spans="1:9">
       <c r="A521" s="22" t="s">
-        <v>1851</v>
+        <v>1850</v>
       </c>
       <c r="B521" s="30" t="s">
         <v>765</v>
@@ -21234,13 +21236,13 @@
     </row>
     <row r="522" spans="1:9" ht="30">
       <c r="A522" s="33" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="B522" s="30" t="s">
         <v>765</v>
       </c>
       <c r="C522" s="35" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="D522" s="33"/>
       <c r="E522" s="33" t="s">
@@ -21259,7 +21261,7 @@
     </row>
     <row r="523" spans="1:9" ht="45">
       <c r="A523" s="33" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="B523" s="30" t="s">
         <v>765</v>
@@ -21281,7 +21283,7 @@
         <v>17</v>
       </c>
       <c r="I523" s="35" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="524" spans="1:9">
@@ -21761,13 +21763,13 @@
     </row>
     <row r="543" spans="1:9" ht="135">
       <c r="A543" s="22" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
       <c r="B543" s="30" t="s">
         <v>767</v>
       </c>
       <c r="C543" s="20" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
       <c r="D543" s="33"/>
       <c r="E543" s="29" t="s">
@@ -21783,12 +21785,12 @@
         <v>17</v>
       </c>
       <c r="I543" s="20" t="s">
-        <v>2083</v>
+        <v>2082</v>
       </c>
     </row>
     <row r="544" spans="1:9" ht="30">
       <c r="A544" s="22" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
       <c r="B544" s="30" t="s">
         <v>767</v>
@@ -21813,7 +21815,7 @@
     </row>
     <row r="545" spans="1:9" ht="30">
       <c r="A545" s="22" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="B545" s="30" t="s">
         <v>767</v>
@@ -21838,7 +21840,7 @@
     </row>
     <row r="546" spans="1:9" ht="45">
       <c r="A546" s="22" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="B546" s="30" t="s">
         <v>767</v>
@@ -21860,12 +21862,12 @@
         <v>17</v>
       </c>
       <c r="I546" s="35" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
     </row>
     <row r="547" spans="1:9">
       <c r="A547" s="22" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="B547" s="30" t="s">
         <v>767</v>
@@ -21890,7 +21892,7 @@
     </row>
     <row r="548" spans="1:9">
       <c r="A548" s="22" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
       <c r="B548" s="30" t="s">
         <v>767</v>
@@ -21915,7 +21917,7 @@
     </row>
     <row r="549" spans="1:9" ht="30">
       <c r="A549" s="22" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="B549" s="30" t="s">
         <v>767</v>
@@ -21940,7 +21942,7 @@
     </row>
     <row r="550" spans="1:9" ht="30">
       <c r="A550" s="22" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="B550" s="30" t="s">
         <v>767</v>
@@ -21965,7 +21967,7 @@
     </row>
     <row r="551" spans="1:9" ht="45">
       <c r="A551" s="22" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="B551" s="30" t="s">
         <v>767</v>
@@ -21987,12 +21989,12 @@
         <v>17</v>
       </c>
       <c r="I551" s="20" t="s">
-        <v>1888</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="552" spans="1:9">
       <c r="A552" s="22" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="B552" s="30" t="s">
         <v>767</v>
@@ -22017,13 +22019,13 @@
     </row>
     <row r="553" spans="1:9" ht="30">
       <c r="A553" s="22" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="B553" s="30" t="s">
         <v>767</v>
       </c>
       <c r="C553" s="35" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="D553" s="33"/>
       <c r="E553" s="29" t="s">
@@ -22042,7 +22044,7 @@
     </row>
     <row r="554" spans="1:9" ht="45">
       <c r="A554" s="22" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="B554" s="30" t="s">
         <v>767</v>
@@ -22064,7 +22066,7 @@
         <v>17</v>
       </c>
       <c r="I554" s="35" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="555" spans="1:9" ht="30">
@@ -22644,20 +22646,20 @@
     </row>
     <row r="578" spans="1:9" ht="135">
       <c r="A578" s="33" t="s">
-        <v>1892</v>
+        <v>1891</v>
       </c>
       <c r="B578" s="30" t="s">
         <v>769</v>
       </c>
       <c r="C578" s="20" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="D578" s="33"/>
       <c r="E578" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F578" s="33" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="G578" s="22" t="s">
         <v>15</v>
@@ -22666,12 +22668,12 @@
         <v>17</v>
       </c>
       <c r="I578" s="20" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
     </row>
     <row r="579" spans="1:9" ht="30">
       <c r="A579" s="33" t="s">
-        <v>1895</v>
+        <v>1894</v>
       </c>
       <c r="B579" s="30" t="s">
         <v>769</v>
@@ -22684,7 +22686,7 @@
         <v>19</v>
       </c>
       <c r="F579" s="33" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="G579" s="33" t="s">
         <v>15</v>
@@ -22696,7 +22698,7 @@
     </row>
     <row r="580" spans="1:9" ht="30">
       <c r="A580" s="33" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="B580" s="30" t="s">
         <v>769</v>
@@ -22709,7 +22711,7 @@
         <v>19</v>
       </c>
       <c r="F580" s="33" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="G580" s="33" t="s">
         <v>15</v>
@@ -22721,7 +22723,7 @@
     </row>
     <row r="581" spans="1:9" ht="45">
       <c r="A581" s="33" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
       <c r="B581" s="30" t="s">
         <v>769</v>
@@ -22734,7 +22736,7 @@
         <v>19</v>
       </c>
       <c r="F581" s="33" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="G581" s="33" t="s">
         <v>15</v>
@@ -22743,12 +22745,12 @@
         <v>17</v>
       </c>
       <c r="I581" s="35" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="582" spans="1:9">
       <c r="A582" s="33" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="B582" s="30" t="s">
         <v>769</v>
@@ -22761,7 +22763,7 @@
         <v>19</v>
       </c>
       <c r="F582" s="33" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="G582" s="33" t="s">
         <v>15</v>
@@ -22773,7 +22775,7 @@
     </row>
     <row r="583" spans="1:9" ht="30">
       <c r="A583" s="33" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="B583" s="30" t="s">
         <v>769</v>
@@ -22786,7 +22788,7 @@
         <v>19</v>
       </c>
       <c r="F583" s="33" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="G583" s="33" t="s">
         <v>16</v>
@@ -22798,7 +22800,7 @@
     </row>
     <row r="584" spans="1:9" ht="30">
       <c r="A584" s="33" t="s">
-        <v>1900</v>
+        <v>1899</v>
       </c>
       <c r="B584" s="30" t="s">
         <v>769</v>
@@ -22811,7 +22813,7 @@
         <v>19</v>
       </c>
       <c r="F584" s="33" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="G584" s="33" t="s">
         <v>16</v>
@@ -22823,7 +22825,7 @@
     </row>
     <row r="585" spans="1:9">
       <c r="A585" s="33" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
       <c r="B585" s="30" t="s">
         <v>769</v>
@@ -22836,7 +22838,7 @@
         <v>19</v>
       </c>
       <c r="F585" s="33" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="G585" s="33" t="s">
         <v>15</v>
@@ -22848,20 +22850,20 @@
     </row>
     <row r="586" spans="1:9" ht="45">
       <c r="A586" s="33" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
       <c r="B586" s="30" t="s">
         <v>769</v>
       </c>
       <c r="C586" s="35" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="D586" s="33"/>
       <c r="E586" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F586" s="33" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="G586" s="33" t="s">
         <v>15</v>
@@ -22870,12 +22872,12 @@
         <v>17</v>
       </c>
       <c r="I586" s="35" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="587" spans="1:9">
       <c r="A587" s="22" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
       <c r="B587" s="30" t="s">
         <v>769</v>
@@ -22888,7 +22890,7 @@
         <v>19</v>
       </c>
       <c r="F587" s="33" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="G587" s="33" t="s">
         <v>15</v>
@@ -22900,20 +22902,20 @@
     </row>
     <row r="588" spans="1:9" ht="30">
       <c r="A588" s="33" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
       <c r="B588" s="30" t="s">
         <v>769</v>
       </c>
       <c r="C588" s="35" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="D588" s="33"/>
       <c r="E588" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F588" s="33" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="G588" s="33" t="s">
         <v>15</v>
@@ -22925,7 +22927,7 @@
     </row>
     <row r="589" spans="1:9" ht="45">
       <c r="A589" s="33" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="B589" s="30" t="s">
         <v>769</v>
@@ -22938,7 +22940,7 @@
         <v>19</v>
       </c>
       <c r="F589" s="33" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="G589" s="33" t="s">
         <v>15</v>
@@ -22947,7 +22949,7 @@
         <v>17</v>
       </c>
       <c r="I589" s="35" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="590" spans="1:9" ht="30">
@@ -23227,7 +23229,7 @@
     </row>
     <row r="601" spans="1:9">
       <c r="A601" s="33" t="s">
-        <v>1923</v>
+        <v>1922</v>
       </c>
       <c r="B601" s="34" t="s">
         <v>771</v>
@@ -23252,7 +23254,7 @@
     </row>
     <row r="602" spans="1:9" ht="45">
       <c r="A602" s="33" t="s">
-        <v>1924</v>
+        <v>1923</v>
       </c>
       <c r="B602" s="34" t="s">
         <v>771</v>
@@ -23277,7 +23279,7 @@
     </row>
     <row r="603" spans="1:9" ht="30">
       <c r="A603" s="33" t="s">
-        <v>1925</v>
+        <v>1924</v>
       </c>
       <c r="B603" s="34" t="s">
         <v>771</v>
@@ -23302,7 +23304,7 @@
     </row>
     <row r="604" spans="1:9" ht="30">
       <c r="A604" s="33" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="B604" s="34" t="s">
         <v>771</v>
@@ -23327,7 +23329,7 @@
     </row>
     <row r="605" spans="1:9">
       <c r="A605" s="33" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
       <c r="B605" s="34" t="s">
         <v>771</v>
@@ -23352,7 +23354,7 @@
     </row>
     <row r="606" spans="1:9">
       <c r="A606" s="33" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
       <c r="B606" s="34" t="s">
         <v>771</v>
@@ -23377,7 +23379,7 @@
     </row>
     <row r="607" spans="1:9" ht="150">
       <c r="A607" s="33" t="s">
-        <v>1929</v>
+        <v>1928</v>
       </c>
       <c r="B607" s="34" t="s">
         <v>771</v>
@@ -23399,12 +23401,12 @@
         <v>17</v>
       </c>
       <c r="I607" s="35" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
     </row>
     <row r="608" spans="1:9" ht="30">
       <c r="A608" s="33" t="s">
-        <v>1930</v>
+        <v>1929</v>
       </c>
       <c r="B608" s="34" t="s">
         <v>771</v>
@@ -23429,13 +23431,13 @@
     </row>
     <row r="609" spans="1:9" ht="45">
       <c r="A609" s="33" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
       <c r="B609" s="34" t="s">
         <v>771</v>
       </c>
       <c r="C609" s="35" t="s">
-        <v>1922</v>
+        <v>1921</v>
       </c>
       <c r="D609" s="33"/>
       <c r="E609" s="29" t="s">
@@ -23454,13 +23456,13 @@
     </row>
     <row r="610" spans="1:9" ht="45">
       <c r="A610" s="33" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="B610" s="34" t="s">
         <v>771</v>
       </c>
       <c r="C610" s="35" t="s">
-        <v>1921</v>
+        <v>1920</v>
       </c>
       <c r="D610" s="33"/>
       <c r="E610" s="33" t="s">
@@ -23479,7 +23481,7 @@
     </row>
     <row r="611" spans="1:9">
       <c r="A611" s="33" t="s">
-        <v>1933</v>
+        <v>1932</v>
       </c>
       <c r="B611" s="34" t="s">
         <v>771</v>
@@ -23504,7 +23506,7 @@
     </row>
     <row r="612" spans="1:9">
       <c r="A612" s="33" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
       <c r="B612" s="34" t="s">
         <v>771</v>
@@ -23529,7 +23531,7 @@
     </row>
     <row r="613" spans="1:9" ht="30">
       <c r="A613" s="33" t="s">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="B613" s="34" t="s">
         <v>771</v>
@@ -23554,7 +23556,7 @@
     </row>
     <row r="614" spans="1:9" ht="30">
       <c r="A614" s="33" t="s">
-        <v>1936</v>
+        <v>1935</v>
       </c>
       <c r="B614" s="34" t="s">
         <v>771</v>
@@ -23579,7 +23581,7 @@
     </row>
     <row r="615" spans="1:9" ht="45">
       <c r="A615" s="33" t="s">
-        <v>1937</v>
+        <v>1936</v>
       </c>
       <c r="B615" s="34" t="s">
         <v>771</v>
@@ -23601,12 +23603,12 @@
         <v>17</v>
       </c>
       <c r="I615" s="35" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="616" spans="1:9">
       <c r="A616" s="33" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
       <c r="B616" s="34" t="s">
         <v>771</v>
@@ -23631,13 +23633,13 @@
     </row>
     <row r="617" spans="1:9" ht="30">
       <c r="A617" s="33" t="s">
-        <v>1939</v>
+        <v>1938</v>
       </c>
       <c r="B617" s="34" t="s">
         <v>771</v>
       </c>
       <c r="C617" s="35" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="D617" s="33"/>
       <c r="E617" s="29" t="s">
@@ -23656,7 +23658,7 @@
     </row>
     <row r="618" spans="1:9" ht="45">
       <c r="A618" s="33" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="B618" s="34" t="s">
         <v>771</v>
@@ -23669,7 +23671,7 @@
         <v>19</v>
       </c>
       <c r="F618" s="33" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="G618" s="33" t="s">
         <v>15</v>
@@ -23678,12 +23680,12 @@
         <v>17</v>
       </c>
       <c r="I618" s="35" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="619" spans="1:9" ht="30">
       <c r="A619" s="33" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="B619" s="34" t="s">
         <v>771</v>
@@ -23708,7 +23710,7 @@
     </row>
     <row r="620" spans="1:9">
       <c r="A620" s="33" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="B620" s="34" t="s">
         <v>771</v>
@@ -23733,7 +23735,7 @@
     </row>
     <row r="621" spans="1:9">
       <c r="A621" s="33" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="B621" s="34" t="s">
         <v>771</v>
@@ -23758,7 +23760,7 @@
     </row>
     <row r="622" spans="1:9">
       <c r="A622" s="33" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="B622" s="34" t="s">
         <v>771</v>
@@ -23783,7 +23785,7 @@
     </row>
     <row r="623" spans="1:9">
       <c r="A623" s="33" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="B623" s="34" t="s">
         <v>771</v>
@@ -23808,7 +23810,7 @@
     </row>
     <row r="624" spans="1:9">
       <c r="A624" s="33" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="B624" s="34" t="s">
         <v>771</v>
@@ -23833,7 +23835,7 @@
     </row>
     <row r="625" spans="1:9" ht="30">
       <c r="A625" s="33" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
       <c r="B625" s="34" t="s">
         <v>771</v>
@@ -23858,7 +23860,7 @@
     </row>
     <row r="626" spans="1:9">
       <c r="A626" s="33" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="B626" s="34" t="s">
         <v>771</v>
@@ -23883,7 +23885,7 @@
     </row>
     <row r="627" spans="1:9">
       <c r="A627" s="33" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="B627" s="34" t="s">
         <v>771</v>
@@ -23908,7 +23910,7 @@
     </row>
     <row r="628" spans="1:9">
       <c r="A628" s="33" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="B628" s="34" t="s">
         <v>772</v>
@@ -26130,7 +26132,7 @@
         <v>17</v>
       </c>
       <c r="I716" s="20" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="717" spans="1:9" ht="30">
@@ -26860,7 +26862,7 @@
     </row>
     <row r="746" spans="1:9">
       <c r="A746" s="33" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
       <c r="B746" s="24" t="s">
         <v>1647</v>
@@ -26885,7 +26887,7 @@
     </row>
     <row r="747" spans="1:9" ht="45">
       <c r="A747" s="33" t="s">
-        <v>1963</v>
+        <v>1962</v>
       </c>
       <c r="B747" s="24" t="s">
         <v>1647</v>
@@ -26910,7 +26912,7 @@
     </row>
     <row r="748" spans="1:9" ht="75">
       <c r="A748" s="33" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="B748" s="24" t="s">
         <v>1647</v>
@@ -26935,7 +26937,7 @@
     </row>
     <row r="749" spans="1:9" ht="30">
       <c r="A749" s="33" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="B749" s="24" t="s">
         <v>1647</v>
@@ -26960,7 +26962,7 @@
     </row>
     <row r="750" spans="1:9">
       <c r="A750" s="33" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
       <c r="B750" s="24" t="s">
         <v>1647</v>
@@ -26985,7 +26987,7 @@
     </row>
     <row r="751" spans="1:9">
       <c r="A751" s="33" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
       <c r="B751" s="24" t="s">
         <v>1647</v>
@@ -27010,7 +27012,7 @@
     </row>
     <row r="752" spans="1:9" ht="30">
       <c r="A752" s="33" t="s">
-        <v>1968</v>
+        <v>1967</v>
       </c>
       <c r="B752" s="24" t="s">
         <v>1647</v>
@@ -27035,7 +27037,7 @@
     </row>
     <row r="753" spans="1:9">
       <c r="A753" s="33" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
       <c r="B753" s="24" t="s">
         <v>1647</v>
@@ -27060,7 +27062,7 @@
     </row>
     <row r="754" spans="1:9" ht="30">
       <c r="A754" s="33" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="B754" s="24" t="s">
         <v>1647</v>
@@ -27085,7 +27087,7 @@
     </row>
     <row r="755" spans="1:9">
       <c r="A755" s="33" t="s">
-        <v>1971</v>
+        <v>1970</v>
       </c>
       <c r="B755" s="24" t="s">
         <v>1647</v>
@@ -27110,7 +27112,7 @@
     </row>
     <row r="756" spans="1:9">
       <c r="A756" s="33" t="s">
-        <v>1972</v>
+        <v>1971</v>
       </c>
       <c r="B756" s="24" t="s">
         <v>1647</v>
@@ -27135,7 +27137,7 @@
     </row>
     <row r="757" spans="1:9">
       <c r="A757" s="33" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
       <c r="B757" s="24" t="s">
         <v>1647</v>
@@ -27160,7 +27162,7 @@
     </row>
     <row r="758" spans="1:9" ht="90">
       <c r="A758" s="33" t="s">
-        <v>1974</v>
+        <v>1973</v>
       </c>
       <c r="B758" s="24" t="s">
         <v>1647</v>
@@ -27185,7 +27187,7 @@
     </row>
     <row r="759" spans="1:9" ht="30">
       <c r="A759" s="33" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
       <c r="B759" s="24" t="s">
         <v>1647</v>
@@ -27210,7 +27212,7 @@
     </row>
     <row r="760" spans="1:9" ht="30">
       <c r="A760" s="33" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="B760" s="24" t="s">
         <v>1647</v>
@@ -27235,7 +27237,7 @@
     </row>
     <row r="761" spans="1:9" ht="30">
       <c r="A761" s="33" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="B761" s="24" t="s">
         <v>1647</v>
@@ -27260,7 +27262,7 @@
     </row>
     <row r="762" spans="1:9" ht="45">
       <c r="A762" s="33" t="s">
-        <v>1978</v>
+        <v>1977</v>
       </c>
       <c r="B762" s="24" t="s">
         <v>1647</v>
@@ -27282,12 +27284,12 @@
         <v>17</v>
       </c>
       <c r="I762" s="35" t="s">
-        <v>2022</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="763" spans="1:9">
       <c r="A763" s="33" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
       <c r="B763" s="24" t="s">
         <v>1647</v>
@@ -27312,7 +27314,7 @@
     </row>
     <row r="764" spans="1:9" ht="30">
       <c r="A764" s="33" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
       <c r="B764" s="24" t="s">
         <v>1647</v>
@@ -27337,7 +27339,7 @@
     </row>
     <row r="765" spans="1:9" ht="30">
       <c r="A765" s="33" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="B765" s="24" t="s">
         <v>1647</v>
@@ -27362,7 +27364,7 @@
     </row>
     <row r="766" spans="1:9" ht="45">
       <c r="A766" s="33" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="B766" s="24" t="s">
         <v>1647</v>
@@ -27384,12 +27386,12 @@
         <v>17</v>
       </c>
       <c r="I766" s="35" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="767" spans="1:9">
       <c r="A767" s="33" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="B767" s="24" t="s">
         <v>1647</v>
@@ -27414,7 +27416,7 @@
     </row>
     <row r="768" spans="1:9">
       <c r="A768" s="33" t="s">
-        <v>1984</v>
+        <v>1983</v>
       </c>
       <c r="B768" s="24" t="s">
         <v>1647</v>
@@ -27439,7 +27441,7 @@
     </row>
     <row r="769" spans="1:9" ht="30">
       <c r="A769" s="33" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="B769" s="24" t="s">
         <v>1647</v>
@@ -27464,7 +27466,7 @@
     </row>
     <row r="770" spans="1:9" ht="30">
       <c r="A770" s="33" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
       <c r="B770" s="24" t="s">
         <v>1647</v>
@@ -27489,7 +27491,7 @@
     </row>
     <row r="771" spans="1:9" ht="45">
       <c r="A771" s="33" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
       <c r="B771" s="24" t="s">
         <v>1647</v>
@@ -27511,12 +27513,12 @@
         <v>17</v>
       </c>
       <c r="I771" s="35" t="s">
-        <v>2029</v>
+        <v>2028</v>
       </c>
     </row>
     <row r="772" spans="1:9">
       <c r="A772" s="33" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="B772" s="24" t="s">
         <v>1647</v>
@@ -27541,13 +27543,13 @@
     </row>
     <row r="773" spans="1:9" ht="30">
       <c r="A773" s="33" t="s">
-        <v>1989</v>
+        <v>1988</v>
       </c>
       <c r="B773" s="24" t="s">
         <v>1647</v>
       </c>
       <c r="C773" s="35" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="D773" s="33"/>
       <c r="E773" s="33" t="s">
@@ -27566,7 +27568,7 @@
     </row>
     <row r="774" spans="1:9" ht="45">
       <c r="A774" s="33" t="s">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="B774" s="24" t="s">
         <v>1647</v>
@@ -27588,12 +27590,12 @@
         <v>17</v>
       </c>
       <c r="I774" s="35" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="775" spans="1:9" ht="30">
       <c r="A775" s="33" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="B775" s="24" t="s">
         <v>1647</v>
@@ -27618,7 +27620,7 @@
     </row>
     <row r="776" spans="1:9">
       <c r="A776" s="33" t="s">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="B776" s="24" t="s">
         <v>1647</v>
@@ -27643,7 +27645,7 @@
     </row>
     <row r="777" spans="1:9">
       <c r="A777" s="33" t="s">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="B777" s="24" t="s">
         <v>1647</v>
@@ -27668,7 +27670,7 @@
     </row>
     <row r="778" spans="1:9">
       <c r="A778" s="33" t="s">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="B778" s="24" t="s">
         <v>1647</v>
@@ -27693,7 +27695,7 @@
     </row>
     <row r="779" spans="1:9">
       <c r="A779" s="33" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="B779" s="24" t="s">
         <v>1647</v>
@@ -27718,7 +27720,7 @@
     </row>
     <row r="780" spans="1:9">
       <c r="A780" s="33" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="B780" s="24" t="s">
         <v>1647</v>
@@ -27743,7 +27745,7 @@
     </row>
     <row r="781" spans="1:9" ht="30">
       <c r="A781" s="33" t="s">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="B781" s="24" t="s">
         <v>1647</v>
@@ -27768,7 +27770,7 @@
     </row>
     <row r="782" spans="1:9">
       <c r="A782" s="33" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="B782" s="24" t="s">
         <v>1647</v>
@@ -27793,7 +27795,7 @@
     </row>
     <row r="783" spans="1:9">
       <c r="A783" s="33" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="B783" s="24" t="s">
         <v>1647</v>
@@ -27818,7 +27820,7 @@
     </row>
     <row r="784" spans="1:9" ht="105">
       <c r="A784" s="33" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="B784" s="24" t="s">
         <v>1647</v>
@@ -27843,7 +27845,7 @@
     </row>
     <row r="785" spans="1:9">
       <c r="A785" s="33" t="s">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="B785" s="24" t="s">
         <v>1647</v>
@@ -27868,7 +27870,7 @@
     </row>
     <row r="786" spans="1:9">
       <c r="A786" s="33" t="s">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="B786" s="34" t="s">
         <v>1686</v>
@@ -27893,7 +27895,7 @@
     </row>
     <row r="787" spans="1:9" ht="45">
       <c r="A787" s="33" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="B787" s="34" t="s">
         <v>1686</v>
@@ -27918,7 +27920,7 @@
     </row>
     <row r="788" spans="1:9" ht="45">
       <c r="A788" s="33" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="B788" s="34" t="s">
         <v>1686</v>
@@ -27943,7 +27945,7 @@
     </row>
     <row r="789" spans="1:9" ht="30">
       <c r="A789" s="33" t="s">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="B789" s="34" t="s">
         <v>1686</v>
@@ -27968,7 +27970,7 @@
     </row>
     <row r="790" spans="1:9">
       <c r="A790" s="33" t="s">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="B790" s="34" t="s">
         <v>1686</v>
@@ -27993,7 +27995,7 @@
     </row>
     <row r="791" spans="1:9">
       <c r="A791" s="33" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="B791" s="34" t="s">
         <v>1686</v>
@@ -28018,7 +28020,7 @@
     </row>
     <row r="792" spans="1:9" ht="30">
       <c r="A792" s="33" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="B792" s="34" t="s">
         <v>1686</v>
@@ -28043,7 +28045,7 @@
     </row>
     <row r="793" spans="1:9">
       <c r="A793" s="33" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="B793" s="34" t="s">
         <v>1686</v>
@@ -28068,7 +28070,7 @@
     </row>
     <row r="794" spans="1:9">
       <c r="A794" s="33" t="s">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="B794" s="34" t="s">
         <v>1686</v>
@@ -28093,7 +28095,7 @@
     </row>
     <row r="795" spans="1:9">
       <c r="A795" s="33" t="s">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="B795" s="34" t="s">
         <v>1686</v>
@@ -28118,7 +28120,7 @@
     </row>
     <row r="796" spans="1:9">
       <c r="A796" s="33" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="B796" s="34" t="s">
         <v>1686</v>
@@ -28143,7 +28145,7 @@
     </row>
     <row r="797" spans="1:9">
       <c r="A797" s="33" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="B797" s="34" t="s">
         <v>1686</v>
@@ -28168,7 +28170,7 @@
     </row>
     <row r="798" spans="1:9">
       <c r="A798" s="33" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="B798" s="34" t="s">
         <v>1686</v>
@@ -28193,7 +28195,7 @@
     </row>
     <row r="799" spans="1:9">
       <c r="A799" s="33" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="B799" s="34" t="s">
         <v>1686</v>
@@ -28218,7 +28220,7 @@
     </row>
     <row r="800" spans="1:9">
       <c r="A800" s="33" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B800" s="34" t="s">
         <v>1686</v>
@@ -28243,7 +28245,7 @@
     </row>
     <row r="801" spans="1:9" ht="30">
       <c r="A801" s="33" t="s">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B801" s="34" t="s">
         <v>1686</v>
@@ -28268,7 +28270,7 @@
     </row>
     <row r="802" spans="1:9" ht="30">
       <c r="A802" s="33" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="B802" s="34" t="s">
         <v>1686</v>
@@ -30272,13 +30274,13 @@
     </row>
     <row r="882" spans="1:9" ht="135">
       <c r="A882" s="33" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="B882" s="30" t="s">
         <v>793</v>
       </c>
       <c r="C882" s="35" t="s">
-        <v>2077</v>
+        <v>2076</v>
       </c>
       <c r="D882" s="33"/>
       <c r="E882" s="33" t="s">
@@ -30294,12 +30296,12 @@
         <v>17</v>
       </c>
       <c r="I882" s="20" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
     </row>
     <row r="883" spans="1:9" ht="30">
       <c r="A883" s="33" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="B883" s="30" t="s">
         <v>793</v>
@@ -30324,7 +30326,7 @@
     </row>
     <row r="884" spans="1:9" ht="45">
       <c r="A884" s="33" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
       <c r="B884" s="30" t="s">
         <v>793</v>
@@ -30351,7 +30353,7 @@
     </row>
     <row r="885" spans="1:9" ht="45">
       <c r="A885" s="33" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
       <c r="B885" s="30" t="s">
         <v>793</v>
@@ -30373,12 +30375,12 @@
         <v>17</v>
       </c>
       <c r="I885" s="35" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
     </row>
     <row r="886" spans="1:9">
       <c r="A886" s="33" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
       <c r="B886" s="30" t="s">
         <v>793</v>
@@ -30403,7 +30405,7 @@
     </row>
     <row r="887" spans="1:9">
       <c r="A887" s="33" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
       <c r="B887" s="30" t="s">
         <v>793</v>
@@ -30428,7 +30430,7 @@
     </row>
     <row r="888" spans="1:9" ht="30">
       <c r="A888" s="33" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
       <c r="B888" s="30" t="s">
         <v>793</v>
@@ -30453,7 +30455,7 @@
     </row>
     <row r="889" spans="1:9" ht="30">
       <c r="A889" s="33" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="B889" s="30" t="s">
         <v>793</v>
@@ -30478,7 +30480,7 @@
     </row>
     <row r="890" spans="1:9" ht="45">
       <c r="A890" s="33" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
       <c r="B890" s="30" t="s">
         <v>793</v>
@@ -30500,12 +30502,12 @@
         <v>17</v>
       </c>
       <c r="I890" s="35" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="891" spans="1:9">
       <c r="A891" s="33" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
       <c r="B891" s="30" t="s">
         <v>793</v>
@@ -30530,13 +30532,13 @@
     </row>
     <row r="892" spans="1:9" ht="30">
       <c r="A892" s="33" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="B892" s="30" t="s">
         <v>793</v>
       </c>
       <c r="C892" s="35" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
       <c r="D892" s="33"/>
       <c r="E892" s="33" t="s">
@@ -30555,7 +30557,7 @@
     </row>
     <row r="893" spans="1:9" ht="45">
       <c r="A893" s="33" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="B893" s="30" t="s">
         <v>793</v>
@@ -30577,7 +30579,7 @@
         <v>17</v>
       </c>
       <c r="I893" s="35" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
     </row>
     <row r="894" spans="1:9">
@@ -30732,7 +30734,7 @@
     </row>
     <row r="900" spans="1:9" ht="30">
       <c r="A900" s="33" t="s">
-        <v>2061</v>
+        <v>2060</v>
       </c>
       <c r="B900" s="30" t="s">
         <v>793</v>
@@ -31546,7 +31548,7 @@
         <v>800</v>
       </c>
       <c r="C932" s="20" t="s">
-        <v>2086</v>
+        <v>2085</v>
       </c>
       <c r="D932" s="29" t="s">
         <v>1405</v>
@@ -31575,7 +31577,7 @@
         <v>800</v>
       </c>
       <c r="C933" s="20" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="D933" s="22" t="s">
         <v>1406</v>
@@ -31598,16 +31600,16 @@
     </row>
     <row r="934" spans="1:9" ht="30">
       <c r="A934" s="33" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="B934" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C934" s="35" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="D934" s="33" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="E934" s="29" t="s">
         <v>22</v>
@@ -31625,16 +31627,16 @@
     </row>
     <row r="935" spans="1:9" ht="45">
       <c r="A935" s="33" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="B935" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C935" s="35" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="D935" s="33" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="E935" s="29" t="s">
         <v>22</v>
@@ -31654,16 +31656,16 @@
     </row>
     <row r="936" spans="1:9" ht="60">
       <c r="A936" s="22" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="B936" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C936" s="20" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="D936" s="33" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="E936" s="29" t="s">
         <v>22</v>
@@ -31681,16 +31683,16 @@
     </row>
     <row r="937" spans="1:9" ht="60">
       <c r="A937" s="33" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="B937" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C937" s="35" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="D937" s="33" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
       <c r="E937" s="29" t="s">
         <v>22</v>
@@ -31708,16 +31710,16 @@
     </row>
     <row r="938" spans="1:9" ht="45">
       <c r="A938" s="33" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="B938" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C938" s="35" t="s">
-        <v>1811</v>
+        <v>1810</v>
       </c>
       <c r="D938" s="33" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
       <c r="E938" s="29" t="s">
         <v>22</v>
@@ -31737,16 +31739,16 @@
     </row>
     <row r="939" spans="1:9" ht="45">
       <c r="A939" s="33" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
       <c r="B939" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C939" s="35" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="D939" s="33" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="E939" s="29" t="s">
         <v>22</v>
@@ -31766,16 +31768,16 @@
     </row>
     <row r="940" spans="1:9" ht="45">
       <c r="A940" s="22" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
       <c r="B940" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C940" s="20" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
       <c r="D940" s="33" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="E940" s="29" t="s">
         <v>22</v>
@@ -31795,16 +31797,16 @@
     </row>
     <row r="941" spans="1:9" ht="45">
       <c r="A941" s="33" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
       <c r="B941" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C941" s="35" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
       <c r="D941" s="33" t="s">
-        <v>1867</v>
+        <v>1866</v>
       </c>
       <c r="E941" s="29" t="s">
         <v>22</v>
@@ -31824,16 +31826,16 @@
     </row>
     <row r="942" spans="1:9" ht="45">
       <c r="A942" s="33" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="B942" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C942" s="35" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="D942" s="33" t="s">
-        <v>1866</v>
+        <v>1865</v>
       </c>
       <c r="E942" s="29" t="s">
         <v>22</v>
@@ -31853,16 +31855,16 @@
     </row>
     <row r="943" spans="1:9" ht="45">
       <c r="A943" s="22" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="B943" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C943" s="35" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
       <c r="D943" s="33" t="s">
-        <v>1865</v>
+        <v>1864</v>
       </c>
       <c r="E943" s="29" t="s">
         <v>22</v>
@@ -31882,16 +31884,16 @@
     </row>
     <row r="944" spans="1:9" ht="45">
       <c r="A944" s="33" t="s">
-        <v>1862</v>
+        <v>1861</v>
       </c>
       <c r="B944" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C944" s="20" t="s">
+        <v>1862</v>
+      </c>
+      <c r="D944" s="33" t="s">
         <v>1863</v>
-      </c>
-      <c r="D944" s="33" t="s">
-        <v>1864</v>
       </c>
       <c r="E944" s="29" t="s">
         <v>22</v>
@@ -31909,16 +31911,16 @@
     </row>
     <row r="945" spans="1:9" ht="45">
       <c r="A945" s="33" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
       <c r="B945" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C945" s="35" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="D945" s="33" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="E945" s="29" t="s">
         <v>22</v>
@@ -31938,16 +31940,16 @@
     </row>
     <row r="946" spans="1:9" ht="45">
       <c r="A946" s="22" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="B946" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C946" s="20" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
       <c r="D946" s="22" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="E946" s="29" t="s">
         <v>22</v>
@@ -31967,16 +31969,16 @@
     </row>
     <row r="947" spans="1:9" ht="45">
       <c r="A947" s="22" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="B947" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C947" s="20" t="s">
-        <v>1890</v>
+        <v>1889</v>
       </c>
       <c r="D947" s="22" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
       <c r="E947" s="29" t="s">
         <v>22</v>
@@ -31994,16 +31996,16 @@
     </row>
     <row r="948" spans="1:9" ht="45">
       <c r="A948" s="33" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="B948" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C948" s="35" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="D948" s="33" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
       <c r="E948" s="29" t="s">
         <v>22</v>
@@ -32023,16 +32025,16 @@
     </row>
     <row r="949" spans="1:9" ht="45">
       <c r="A949" s="22" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
       <c r="B949" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C949" s="35" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="D949" s="33" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="E949" s="29" t="s">
         <v>22</v>
@@ -32052,16 +32054,16 @@
     </row>
     <row r="950" spans="1:9" ht="45">
       <c r="A950" s="33" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="B950" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C950" s="35" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="D950" s="33" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="E950" s="29" t="s">
         <v>22</v>
@@ -32081,16 +32083,16 @@
     </row>
     <row r="951" spans="1:9" ht="45">
       <c r="A951" s="33" t="s">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="B951" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C951" s="35" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="D951" s="33" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="E951" s="29" t="s">
         <v>22</v>
@@ -32108,16 +32110,16 @@
     </row>
     <row r="952" spans="1:9" ht="45">
       <c r="A952" s="33" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="B952" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C952" s="35" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="D952" s="33" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="E952" s="29" t="s">
         <v>22</v>
@@ -32135,16 +32137,16 @@
     </row>
     <row r="953" spans="1:9" ht="45">
       <c r="A953" s="33" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B953" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C953" s="35" t="s">
+        <v>2019</v>
+      </c>
+      <c r="D953" s="33" t="s">
         <v>2020</v>
-      </c>
-      <c r="D953" s="33" t="s">
-        <v>2021</v>
       </c>
       <c r="E953" s="29" t="s">
         <v>22</v>
@@ -32162,16 +32164,16 @@
     </row>
     <row r="954" spans="1:9" ht="45">
       <c r="A954" s="33" t="s">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="B954" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C954" s="35" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D954" s="33" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="E954" s="29" t="s">
         <v>22</v>
@@ -32189,16 +32191,16 @@
     </row>
     <row r="955" spans="1:9" ht="45">
       <c r="A955" s="33" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="B955" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C955" s="35" t="s">
-        <v>2032</v>
+        <v>2031</v>
       </c>
       <c r="D955" s="33" t="s">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="E955" s="29" t="s">
         <v>22</v>
@@ -32216,16 +32218,16 @@
     </row>
     <row r="956" spans="1:9" ht="45">
       <c r="A956" s="33" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="B956" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C956" s="35" t="s">
-        <v>2033</v>
+        <v>2032</v>
       </c>
       <c r="D956" s="33" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="E956" s="29" t="s">
         <v>22</v>
@@ -32243,16 +32245,16 @@
     </row>
     <row r="957" spans="1:9" ht="45">
       <c r="A957" s="33" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
       <c r="B957" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C957" s="35" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
       <c r="D957" s="33" t="s">
-        <v>2049</v>
+        <v>2048</v>
       </c>
       <c r="E957" s="29" t="s">
         <v>22</v>
@@ -32272,16 +32274,16 @@
     </row>
     <row r="958" spans="1:9" ht="45">
       <c r="A958" s="33" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
       <c r="B958" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C958" s="35" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
       <c r="D958" s="33" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="E958" s="29" t="s">
         <v>22</v>
@@ -32301,16 +32303,16 @@
     </row>
     <row r="959" spans="1:9" ht="45">
       <c r="A959" s="33" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="B959" s="34" t="s">
         <v>800</v>
       </c>
       <c r="C959" s="35" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
       <c r="D959" s="33" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
       <c r="E959" s="29" t="s">
         <v>22</v>
@@ -32336,10 +32338,10 @@
         <v>800</v>
       </c>
       <c r="C960" s="35" t="s">
-        <v>1729</v>
-      </c>
-      <c r="D960" s="33" t="s">
         <v>1728</v>
+      </c>
+      <c r="D960" s="22" t="s">
+        <v>2087</v>
       </c>
       <c r="E960" s="29" t="s">
         <v>22</v>
@@ -32365,10 +32367,10 @@
         <v>8</v>
       </c>
       <c r="C961" s="35" t="s">
-        <v>1741</v>
-      </c>
-      <c r="D961" s="33" t="s">
-        <v>1728</v>
+        <v>1740</v>
+      </c>
+      <c r="D961" s="22" t="s">
+        <v>2087</v>
       </c>
       <c r="E961" s="29" t="s">
         <v>22</v>
@@ -32407,6 +32409,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -32414,11 +32421,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="I20:I46 D342:I342 A342:B342 A962:I962 A961 A960:D960 E960:E961 A20:H341 F960:I960 F961:H961 A343:I959 A36:I341">
@@ -32582,7 +32584,7 @@
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="74" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B19:B27 B47:B51 B30:B45 B53:B57 B66 B60 B70:B132 B134:B136 B145:B154 B156:B175 B180:B221 B224:B294 B296:B300 B307 B309:B327 B329 B331:B341 B343:B349 B356:B358 B362:B364 B368:B374 B378:B380 B385:B393 B397:B402 B405:B432 B448:B454 B456:B480 B483 B491:B496 B498:B511 B524:B529 B531:B542 B555:B560 B562:B577 B590:B595 B597:B600 B803:B881 B894:B899 B963:B964 B901:B932 B62:B64 B68" numberStoredAsText="1"/>
+    <ignoredError sqref="B19:B29 B46:B52 B30:B45 B53:B59 B65:B67 B60:B61 B69:B900 B963:B964 B901:B961 B62:B64 B68 C3" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>

</xml_diff>